<commit_message>
Updated main code to current LED strip + sensors.
</commit_message>
<xml_diff>
--- a/hardware/SeeBoat_fullPartsList.xlsx
+++ b/hardware/SeeBoat_fullPartsList.xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\talia\Documents\GitHub\seeboat\hardware\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11478" windowHeight="8484"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="final" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="scrap" sheetId="2" r:id="rId4"/>
+    <sheet name="final" sheetId="1" r:id="rId1"/>
+    <sheet name="scrap" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="317">
   <si>
     <t>Parts list for SeeBoat &amp; full sensor suite</t>
   </si>
@@ -960,130 +968,191 @@
   </si>
   <si>
     <t>for waterproofing the electronics</t>
+  </si>
+  <si>
+    <t>6-32 1/2'' Phillips</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="mmmm yyyy"/>
+    <numFmt numFmtId="164" formatCode="mmmm\ yyyy"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
       <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <u/>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <u/>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <u/>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <u/>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <u/>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1091,7 +1160,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1107,256 +1176,486 @@
     </fill>
   </fills>
   <borders count="10">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="59">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="18" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="19" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="23" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AB126"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.0"/>
-    <col customWidth="1" min="5" max="5" width="21.14"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1369,15 +1668,15 @@
       <c r="H1" s="3"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="8"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="9">
-        <v>43221.0</v>
+        <v>43221</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -1388,13 +1687,13 @@
       <c r="H3" s="11"/>
       <c r="I3" s="12"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="13"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
         <v>19</v>
       </c>
@@ -1438,7 +1737,7 @@
       <c r="AA6" s="16"/>
       <c r="AB6" s="16"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>39</v>
       </c>
@@ -1452,16 +1751,16 @@
         <v>46</v>
       </c>
       <c r="F7" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="23">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>56</v>
       </c>
@@ -1472,16 +1771,16 @@
         <v>58</v>
       </c>
       <c r="F8" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="23">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="22" t="s">
         <v>60</v>
       </c>
@@ -1492,16 +1791,16 @@
         <v>62</v>
       </c>
       <c r="F9" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="23">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>64</v>
       </c>
@@ -1512,16 +1811,16 @@
         <v>65</v>
       </c>
       <c r="F10" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="23">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="25" t="s">
         <v>68</v>
       </c>
@@ -1534,10 +1833,10 @@
         <v>69</v>
       </c>
       <c r="F11" s="29">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="G11" s="30">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="H11" s="26" t="s">
         <v>72</v>
@@ -1563,7 +1862,7 @@
       <c r="AA11" s="16"/>
       <c r="AB11" s="16"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>77</v>
       </c>
@@ -1574,16 +1873,16 @@
         <v>62</v>
       </c>
       <c r="F12" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="23">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>81</v>
       </c>
@@ -1594,16 +1893,16 @@
         <v>82</v>
       </c>
       <c r="F13" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="23">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H13" s="10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="22" t="s">
         <v>84</v>
       </c>
@@ -1614,16 +1913,16 @@
         <v>86</v>
       </c>
       <c r="F15" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="23">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="H15" s="10" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="22" t="s">
         <v>88</v>
       </c>
@@ -1634,16 +1933,16 @@
         <v>86</v>
       </c>
       <c r="F16" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="23">
-        <v>126.0</v>
+        <v>126</v>
       </c>
       <c r="H16" s="10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="22" t="s">
         <v>90</v>
       </c>
@@ -1654,20 +1953,20 @@
         <v>91</v>
       </c>
       <c r="F17" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="23">
-        <v>160.0</v>
+        <v>160</v>
       </c>
       <c r="H17" s="10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="32"/>
       <c r="B19" s="32"/>
       <c r="C19" s="32"/>
@@ -1697,13 +1996,13 @@
       <c r="AA19" s="32"/>
       <c r="AB19" s="32"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D20" s="13"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="14" t="s">
         <v>19</v>
       </c>
@@ -1747,7 +2046,7 @@
       <c r="AA21" s="16"/>
       <c r="AB21" s="16"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="25" t="s">
         <v>94</v>
       </c>
@@ -1760,10 +2059,10 @@
         <v>95</v>
       </c>
       <c r="F22" s="29">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="30">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="H22" s="33" t="s">
         <v>96</v>
@@ -1789,7 +2088,7 @@
       <c r="AA22" s="16"/>
       <c r="AB22" s="16"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="25" t="s">
         <v>97</v>
       </c>
@@ -1802,10 +2101,10 @@
         <v>98</v>
       </c>
       <c r="F23" s="29">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="30">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="H23" s="26" t="s">
         <v>99</v>
@@ -1831,7 +2130,7 @@
       <c r="AA23" s="16"/>
       <c r="AB23" s="16"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="25" t="s">
         <v>100</v>
       </c>
@@ -1844,10 +2143,10 @@
         <v>101</v>
       </c>
       <c r="F24" s="29">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="30">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="26" t="s">
         <v>102</v>
@@ -1873,7 +2172,7 @@
       <c r="AA24" s="16"/>
       <c r="AB24" s="16"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="25" t="s">
         <v>103</v>
       </c>
@@ -1886,10 +2185,10 @@
         <v>75</v>
       </c>
       <c r="F25" s="24">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="G25" s="31">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="H25" s="26" t="s">
         <v>104</v>
@@ -1915,7 +2214,7 @@
       <c r="AA25" s="16"/>
       <c r="AB25" s="16"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="25" t="s">
         <v>105</v>
       </c>
@@ -1928,7 +2227,7 @@
         <v>106</v>
       </c>
       <c r="F26" s="24">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="G26" s="31">
         <v>1.25</v>
@@ -1957,7 +2256,7 @@
       <c r="AA26" s="16"/>
       <c r="AB26" s="16"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A27" s="25" t="s">
         <v>108</v>
       </c>
@@ -1970,10 +2269,10 @@
         <v>109</v>
       </c>
       <c r="F27" s="24">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="G27" s="31">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H27" s="26" t="s">
         <v>110</v>
@@ -1999,7 +2298,7 @@
       <c r="AA27" s="16"/>
       <c r="AB27" s="16"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A28" s="25" t="s">
         <v>111</v>
       </c>
@@ -2012,7 +2311,7 @@
         <v>113</v>
       </c>
       <c r="F28" s="24">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G28" s="31">
         <v>5.59</v>
@@ -2041,7 +2340,7 @@
       <c r="AA28" s="16"/>
       <c r="AB28" s="16"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A29" s="25" t="s">
         <v>115</v>
       </c>
@@ -2054,10 +2353,10 @@
         <v>116</v>
       </c>
       <c r="F29" s="34">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="30">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="H29" s="26" t="s">
         <v>117</v>
@@ -2081,14 +2380,14 @@
       <c r="Y29" s="16"/>
       <c r="Z29" s="16"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A30" s="35"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A31" s="35" t="s">
         <v>118</v>
       </c>
@@ -2099,16 +2398,16 @@
         <v>120</v>
       </c>
       <c r="F31" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G31" s="23">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H31" s="10" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
         <v>122</v>
       </c>
@@ -2122,7 +2421,7 @@
         <v>125</v>
       </c>
       <c r="F32" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G32" s="36">
         <v>0.1</v>
@@ -2131,7 +2430,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>127</v>
       </c>
@@ -2145,7 +2444,7 @@
         <v>129</v>
       </c>
       <c r="F33" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="G33" s="36">
         <v>0.1</v>
@@ -2154,7 +2453,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>131</v>
       </c>
@@ -2168,7 +2467,7 @@
         <v>133</v>
       </c>
       <c r="F34" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G34" s="37">
         <v>1.07</v>
@@ -2177,12 +2476,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>135</v>
       </c>
       <c r="C35" s="22">
-        <v>2343.0</v>
+        <v>2343</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>74</v>
@@ -2191,7 +2490,7 @@
         <v>136</v>
       </c>
       <c r="F35" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G35" s="36">
         <v>4.5</v>
@@ -2200,7 +2499,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
         <v>138</v>
       </c>
@@ -2214,7 +2513,7 @@
         <v>140</v>
       </c>
       <c r="F36" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="G36" s="36">
         <v>0.94</v>
@@ -2223,7 +2522,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
         <v>142</v>
       </c>
@@ -2237,7 +2536,7 @@
         <v>144</v>
       </c>
       <c r="F37" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="G37" s="36">
         <v>1.46</v>
@@ -2246,7 +2545,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>146</v>
       </c>
@@ -2260,7 +2559,7 @@
         <v>148</v>
       </c>
       <c r="F38" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G38" s="36">
         <v>0.87</v>
@@ -2269,7 +2568,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>150</v>
       </c>
@@ -2283,7 +2582,7 @@
         <v>152</v>
       </c>
       <c r="F39" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G39" s="36">
         <v>0.99</v>
@@ -2292,7 +2591,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>154</v>
       </c>
@@ -2306,7 +2605,7 @@
         <v>156</v>
       </c>
       <c r="F40" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G40" s="36">
         <v>95.15</v>
@@ -2318,7 +2617,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A41" s="16" t="s">
         <v>159</v>
       </c>
@@ -2335,10 +2634,10 @@
         <v>161</v>
       </c>
       <c r="F41" s="24">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G41" s="38">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="H41" s="26" t="s">
         <v>162</v>
@@ -2364,7 +2663,7 @@
       <c r="AA41" s="16"/>
       <c r="AB41" s="16"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A43" s="32"/>
       <c r="B43" s="32"/>
       <c r="C43" s="32"/>
@@ -2394,13 +2693,13 @@
       <c r="AA43" s="32"/>
       <c r="AB43" s="32"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A44" s="4" t="s">
         <v>163</v>
       </c>
       <c r="D44" s="13"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:28" ht="12.6" x14ac:dyDescent="0.45">
       <c r="A45" s="14" t="s">
         <v>19</v>
       </c>
@@ -2444,7 +2743,7 @@
       <c r="AA45" s="16"/>
       <c r="AB45" s="16"/>
     </row>
-    <row r="46">
+    <row r="46" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A46" s="39" t="s">
         <v>164</v>
       </c>
@@ -2457,10 +2756,10 @@
         <v>165</v>
       </c>
       <c r="F46" s="24">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G46" s="30">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="H46" s="26" t="s">
         <v>166</v>
@@ -2485,7 +2784,7 @@
       <c r="AA46" s="16"/>
       <c r="AB46" s="16"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A47" s="25" t="s">
         <v>167</v>
       </c>
@@ -2498,10 +2797,10 @@
         <v>168</v>
       </c>
       <c r="F47" s="24">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G47" s="38">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="H47" s="26" t="s">
         <v>169</v>
@@ -2526,7 +2825,7 @@
       <c r="AA47" s="16"/>
       <c r="AB47" s="16"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A48" s="35" t="s">
         <v>170</v>
       </c>
@@ -2537,16 +2836,16 @@
         <v>172</v>
       </c>
       <c r="F48" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G48" s="23">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="H48" s="10" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
         <v>174</v>
       </c>
@@ -2557,16 +2856,16 @@
         <v>175</v>
       </c>
       <c r="F49" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G49" s="23">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="H49" s="10" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A50" s="35" t="s">
         <v>177</v>
       </c>
@@ -2577,16 +2876,16 @@
         <v>178</v>
       </c>
       <c r="F50" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G50" s="23">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="H50" s="10" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A51" s="35" t="s">
         <v>180</v>
       </c>
@@ -2597,13 +2896,13 @@
         <v>182</v>
       </c>
       <c r="F51" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G51" s="23">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="52">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A52" s="35" t="s">
         <v>183</v>
       </c>
@@ -2614,16 +2913,16 @@
         <v>184</v>
       </c>
       <c r="F52" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G52" s="23">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="H52" s="10" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A53" s="35" t="s">
         <v>186</v>
       </c>
@@ -2634,22 +2933,22 @@
         <v>188</v>
       </c>
       <c r="F53" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G53" s="23">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="H53" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A54" s="4"/>
     </row>
-    <row r="55">
+    <row r="55" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A55" s="4"/>
     </row>
-    <row r="56">
+    <row r="56" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A56" s="32"/>
       <c r="B56" s="32"/>
       <c r="C56" s="32"/>
@@ -2679,13 +2978,13 @@
       <c r="AA56" s="32"/>
       <c r="AB56" s="32"/>
     </row>
-    <row r="57">
+    <row r="57" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A57" s="4" t="s">
         <v>189</v>
       </c>
       <c r="D57" s="13"/>
     </row>
-    <row r="58">
+    <row r="58" spans="1:28" ht="12.6" x14ac:dyDescent="0.45">
       <c r="A58" s="14" t="s">
         <v>19</v>
       </c>
@@ -2729,7 +3028,7 @@
       <c r="AA58" s="16"/>
       <c r="AB58" s="16"/>
     </row>
-    <row r="59">
+    <row r="59" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A59" s="16" t="s">
         <v>190</v>
       </c>
@@ -2742,10 +3041,10 @@
         <v>192</v>
       </c>
       <c r="F59" s="24">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G59" s="30">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="H59" s="26" t="s">
         <v>193</v>
@@ -2769,7 +3068,7 @@
       <c r="Y59" s="16"/>
       <c r="Z59" s="16"/>
     </row>
-    <row r="60">
+    <row r="60" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A60" s="25" t="s">
         <v>194</v>
       </c>
@@ -2782,10 +3081,10 @@
         <v>192</v>
       </c>
       <c r="F60" s="24">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G60" s="30">
-        <v>72.0</v>
+        <v>72</v>
       </c>
       <c r="H60" s="26" t="s">
         <v>195</v>
@@ -2809,7 +3108,7 @@
       <c r="Y60" s="16"/>
       <c r="Z60" s="16"/>
     </row>
-    <row r="61">
+    <row r="61" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A61" s="25" t="s">
         <v>196</v>
       </c>
@@ -2822,10 +3121,10 @@
         <v>197</v>
       </c>
       <c r="F61" s="24">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G61" s="38">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="H61" s="26" t="s">
         <v>198</v>
@@ -2849,7 +3148,7 @@
       <c r="Y61" s="16"/>
       <c r="Z61" s="16"/>
     </row>
-    <row r="62">
+    <row r="62" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A62" s="2" t="s">
         <v>199</v>
       </c>
@@ -2860,16 +3159,16 @@
         <v>201</v>
       </c>
       <c r="F62" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G62" s="23">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="H62" s="10" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
         <v>203</v>
       </c>
@@ -2880,19 +3179,19 @@
         <v>204</v>
       </c>
       <c r="F63" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G63" s="23">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="H63" s="10" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A64" s="2"/>
     </row>
-    <row r="65">
+    <row r="65" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
         <v>206</v>
       </c>
@@ -2903,10 +3202,10 @@
         <v>208</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A66" s="2"/>
     </row>
-    <row r="67">
+    <row r="67" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A67" s="32"/>
       <c r="B67" s="32"/>
       <c r="C67" s="32"/>
@@ -2936,12 +3235,12 @@
       <c r="AA67" s="32"/>
       <c r="AB67" s="32"/>
     </row>
-    <row r="68">
+    <row r="68" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A68" s="4" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:28" ht="12.6" x14ac:dyDescent="0.45">
       <c r="A69" s="14" t="s">
         <v>19</v>
       </c>
@@ -2985,7 +3284,7 @@
       <c r="AA69" s="16"/>
       <c r="AB69" s="16"/>
     </row>
-    <row r="70">
+    <row r="70" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
         <v>210</v>
       </c>
@@ -2994,16 +3293,16 @@
       </c>
       <c r="E70" s="40"/>
       <c r="F70" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G70" s="23">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="H70" s="10" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
         <v>212</v>
       </c>
@@ -3014,7 +3313,7 @@
         <v>124</v>
       </c>
       <c r="F71" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="G71" s="36">
         <v>0.17</v>
@@ -3023,7 +3322,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A72" s="27" t="s">
         <v>215</v>
       </c>
@@ -3036,7 +3335,7 @@
       </c>
       <c r="E72" s="27"/>
       <c r="F72" s="29">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G72" s="36">
         <v>0.1</v>
@@ -3065,7 +3364,7 @@
       <c r="AA72" s="16"/>
       <c r="AB72" s="16"/>
     </row>
-    <row r="73">
+    <row r="73" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A73" s="27" t="s">
         <v>217</v>
       </c>
@@ -3078,7 +3377,7 @@
       </c>
       <c r="E73" s="27"/>
       <c r="F73" s="29">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G73" s="37">
         <v>0.34</v>
@@ -3107,7 +3406,7 @@
       <c r="AA73" s="16"/>
       <c r="AB73" s="16"/>
     </row>
-    <row r="74">
+    <row r="74" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A74" s="27" t="s">
         <v>220</v>
       </c>
@@ -3120,7 +3419,7 @@
       </c>
       <c r="E74" s="27"/>
       <c r="F74" s="29">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G74" s="36">
         <v>0.1</v>
@@ -3149,7 +3448,7 @@
       <c r="AA74" s="16"/>
       <c r="AB74" s="16"/>
     </row>
-    <row r="75">
+    <row r="75" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A75" s="27" t="s">
         <v>223</v>
       </c>
@@ -3162,7 +3461,7 @@
       </c>
       <c r="E75" s="27"/>
       <c r="F75" s="29">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G75" s="36">
         <v>0.34</v>
@@ -3191,7 +3490,7 @@
       <c r="AA75" s="16"/>
       <c r="AB75" s="16"/>
     </row>
-    <row r="76">
+    <row r="76" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A76" s="27" t="s">
         <v>226</v>
       </c>
@@ -3204,7 +3503,7 @@
       </c>
       <c r="E76" s="27"/>
       <c r="F76" s="29">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G76" s="37">
         <v>0.12</v>
@@ -3233,7 +3532,7 @@
       <c r="AA76" s="16"/>
       <c r="AB76" s="16"/>
     </row>
-    <row r="77">
+    <row r="77" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A77" s="27" t="s">
         <v>229</v>
       </c>
@@ -3245,7 +3544,7 @@
         <v>124</v>
       </c>
       <c r="F77" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G77" s="31">
         <v>0.32</v>
@@ -3274,7 +3573,7 @@
       <c r="AA77" s="16"/>
       <c r="AB77" s="16"/>
     </row>
-    <row r="78">
+    <row r="78" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A78" s="43" t="s">
         <v>232</v>
       </c>
@@ -3286,7 +3585,7 @@
       </c>
       <c r="E78" s="40"/>
       <c r="F78" s="44">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G78" s="36">
         <v>0.37</v>
@@ -3295,7 +3594,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A79" s="27" t="s">
         <v>235</v>
       </c>
@@ -3307,7 +3606,7 @@
         <v>124</v>
       </c>
       <c r="F79" s="29">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G79" s="30">
         <v>1.86</v>
@@ -3334,7 +3633,7 @@
       <c r="Y79" s="16"/>
       <c r="Z79" s="16"/>
     </row>
-    <row r="80">
+    <row r="80" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A80" s="27" t="s">
         <v>238</v>
       </c>
@@ -3346,7 +3645,7 @@
         <v>124</v>
       </c>
       <c r="F80" s="29">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G80" s="37">
         <v>2.64</v>
@@ -3373,7 +3672,7 @@
       <c r="Y80" s="16"/>
       <c r="Z80" s="16"/>
     </row>
-    <row r="81">
+    <row r="81" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A81" s="27" t="s">
         <v>238</v>
       </c>
@@ -3383,7 +3682,7 @@
       </c>
       <c r="E81" s="25"/>
       <c r="F81" s="29">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G81" s="30">
         <v>1.81</v>
@@ -3410,7 +3709,7 @@
       <c r="Y81" s="16"/>
       <c r="Z81" s="16"/>
     </row>
-    <row r="82">
+    <row r="82" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
         <v>131</v>
       </c>
@@ -3424,7 +3723,7 @@
         <v>243</v>
       </c>
       <c r="F82" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G82" s="37">
         <v>1.07</v>
@@ -3433,7 +3732,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A83" s="16"/>
       <c r="B83" s="16"/>
       <c r="C83" s="22"/>
@@ -3463,7 +3762,7 @@
       <c r="AA83" s="16"/>
       <c r="AB83" s="16"/>
     </row>
-    <row r="84">
+    <row r="84" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A84" s="16" t="s">
         <v>244</v>
       </c>
@@ -3480,10 +3779,10 @@
         <v>246</v>
       </c>
       <c r="F84" s="24">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G84" s="38">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="H84" s="26" t="s">
         <v>247</v>
@@ -3509,7 +3808,7 @@
       <c r="AA84" s="16"/>
       <c r="AB84" s="16"/>
     </row>
-    <row r="85">
+    <row r="85" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A85" s="16" t="s">
         <v>159</v>
       </c>
@@ -3526,10 +3825,10 @@
         <v>246</v>
       </c>
       <c r="F85" s="24">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G85" s="38">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="H85" s="26" t="s">
         <v>162</v>
@@ -3555,26 +3854,29 @@
       <c r="AA85" s="16"/>
       <c r="AB85" s="16"/>
     </row>
-    <row r="87">
+    <row r="87" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
         <v>248</v>
       </c>
       <c r="F87" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
         <v>249</v>
       </c>
+      <c r="C88" s="58" t="s">
+        <v>316</v>
+      </c>
       <c r="E88" s="2" t="s">
         <v>250</v>
       </c>
       <c r="F88" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
         <v>251</v>
       </c>
@@ -3582,10 +3884,10 @@
         <v>250</v>
       </c>
       <c r="F89" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:28" ht="12.6" x14ac:dyDescent="0.45">
       <c r="A90" s="48" t="s">
         <v>252</v>
       </c>
@@ -3628,7 +3930,7 @@
       <c r="AA90" s="49"/>
       <c r="AB90" s="49"/>
     </row>
-    <row r="91">
+    <row r="91" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A91" s="22" t="s">
         <v>255</v>
       </c>
@@ -3639,16 +3941,16 @@
         <v>201</v>
       </c>
       <c r="F91" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G91" s="23">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="H91" s="10" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A92" s="22" t="s">
         <v>257</v>
       </c>
@@ -3659,16 +3961,16 @@
         <v>201</v>
       </c>
       <c r="F92" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G92" s="23">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="H92" s="10" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A94" s="32"/>
       <c r="B94" s="32"/>
       <c r="C94" s="32"/>
@@ -3698,13 +4000,13 @@
       <c r="AA94" s="32"/>
       <c r="AB94" s="32"/>
     </row>
-    <row r="95">
+    <row r="95" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A95" s="4" t="s">
         <v>259</v>
       </c>
       <c r="D95" s="13"/>
     </row>
-    <row r="96">
+    <row r="96" spans="1:28" ht="12.6" x14ac:dyDescent="0.45">
       <c r="A96" s="14" t="s">
         <v>19</v>
       </c>
@@ -3747,7 +4049,7 @@
       <c r="AA96" s="16"/>
       <c r="AB96" s="16"/>
     </row>
-    <row r="97">
+    <row r="97" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A97" s="16" t="s">
         <v>260</v>
       </c>
@@ -3759,7 +4061,7 @@
       </c>
       <c r="E97" s="16"/>
       <c r="F97" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G97" s="31">
         <v>1.06</v>
@@ -3768,7 +4070,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A98" s="16" t="s">
         <v>263</v>
       </c>
@@ -3780,7 +4082,7 @@
       </c>
       <c r="E98" s="16"/>
       <c r="F98" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G98" s="31">
         <v>5.31</v>
@@ -3789,7 +4091,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A99" s="51" t="s">
         <v>266</v>
       </c>
@@ -3800,7 +4102,7 @@
         <v>124</v>
       </c>
       <c r="F99" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G99" s="31">
         <v>0.32</v>
@@ -3809,7 +4111,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A100" s="16" t="s">
         <v>267</v>
       </c>
@@ -3820,7 +4122,7 @@
         <v>124</v>
       </c>
       <c r="F100" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G100" s="31">
         <v>0.12</v>
@@ -3829,7 +4131,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
         <v>270</v>
       </c>
@@ -3837,16 +4139,16 @@
         <v>119</v>
       </c>
       <c r="F101" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G101" s="23">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="H101" s="10" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A102" s="2" t="s">
         <v>272</v>
       </c>
@@ -3854,16 +4156,16 @@
         <v>119</v>
       </c>
       <c r="F102" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G102" s="23">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="H102" s="10" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A103" s="16" t="s">
         <v>274</v>
       </c>
@@ -3876,16 +4178,16 @@
       </c>
       <c r="E103" s="27"/>
       <c r="F103" s="24">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G103" s="38">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="H103" s="26" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A104" s="16" t="s">
         <v>277</v>
       </c>
@@ -3898,10 +4200,10 @@
       </c>
       <c r="E104" s="25"/>
       <c r="F104" s="24">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G104" s="38">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="H104" s="26" t="s">
         <v>278</v>
@@ -3927,7 +4229,7 @@
       <c r="AA104" s="16"/>
       <c r="AB104" s="16"/>
     </row>
-    <row r="105">
+    <row r="105" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A105" s="16" t="s">
         <v>279</v>
       </c>
@@ -3940,10 +4242,10 @@
       </c>
       <c r="E105" s="25"/>
       <c r="F105" s="24">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G105" s="38">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="H105" s="26" t="s">
         <v>280</v>
@@ -3969,7 +4271,7 @@
       <c r="AA105" s="16"/>
       <c r="AB105" s="16"/>
     </row>
-    <row r="106">
+    <row r="106" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A106" s="2" t="s">
         <v>281</v>
       </c>
@@ -3980,16 +4282,16 @@
         <v>282</v>
       </c>
       <c r="F106" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G106" s="23">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="H106" s="10" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A107" s="2" t="s">
         <v>284</v>
       </c>
@@ -4000,7 +4302,7 @@
         <v>285</v>
       </c>
       <c r="F107" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G107" s="36">
         <v>43.95</v>
@@ -4009,7 +4311,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
         <v>287</v>
       </c>
@@ -4020,16 +4322,16 @@
         <v>288</v>
       </c>
       <c r="F108" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G108" s="23">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="H108" s="10" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A109" s="2" t="s">
         <v>290</v>
       </c>
@@ -4040,16 +4342,16 @@
         <v>288</v>
       </c>
       <c r="F109" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G109" s="23">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="H109" s="10" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:28" ht="12.6" x14ac:dyDescent="0.45">
       <c r="A110" s="52" t="s">
         <v>293</v>
       </c>
@@ -4062,10 +4364,10 @@
         <v>294</v>
       </c>
       <c r="F110" s="48">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G110" s="54">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="H110" s="55" t="s">
         <v>295</v>
@@ -4091,10 +4393,10 @@
       <c r="AA110" s="49"/>
       <c r="AB110" s="49"/>
     </row>
-    <row r="111">
+    <row r="111" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A111" s="2"/>
     </row>
-    <row r="112">
+    <row r="112" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A112" s="32"/>
       <c r="B112" s="32"/>
       <c r="C112" s="32"/>
@@ -4124,13 +4426,13 @@
       <c r="AA112" s="32"/>
       <c r="AB112" s="32"/>
     </row>
-    <row r="113">
+    <row r="113" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A113" s="4" t="s">
         <v>296</v>
       </c>
       <c r="D113" s="13"/>
     </row>
-    <row r="114">
+    <row r="114" spans="1:28" ht="12.6" x14ac:dyDescent="0.45">
       <c r="A114" s="14" t="s">
         <v>19</v>
       </c>
@@ -4174,7 +4476,7 @@
       <c r="AA114" s="16"/>
       <c r="AB114" s="16"/>
     </row>
-    <row r="115">
+    <row r="115" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A115" s="2" t="s">
         <v>297</v>
       </c>
@@ -4185,16 +4487,16 @@
         <v>298</v>
       </c>
       <c r="F115" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G115" s="23">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H115" s="10" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A116" s="2" t="s">
         <v>300</v>
       </c>
@@ -4208,7 +4510,7 @@
         <v>302</v>
       </c>
       <c r="F116" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G116" s="36">
         <v>0.6</v>
@@ -4217,7 +4519,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A117" s="27" t="s">
         <v>304</v>
       </c>
@@ -4231,7 +4533,7 @@
         <v>306</v>
       </c>
       <c r="F117" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G117" s="36">
         <v>0.1</v>
@@ -4240,7 +4542,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A118" s="27" t="s">
         <v>308</v>
       </c>
@@ -4251,7 +4553,7 @@
         <v>124</v>
       </c>
       <c r="F118" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G118" s="36">
         <v>0.36</v>
@@ -4260,7 +4562,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A119" s="27" t="s">
         <v>311</v>
       </c>
@@ -4277,10 +4579,10 @@
         <v>313</v>
       </c>
       <c r="F119" s="24">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G119" s="38">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="H119" s="57" t="s">
         <v>314</v>
@@ -4306,7 +4608,7 @@
       <c r="AA119" s="16"/>
       <c r="AB119" s="16"/>
     </row>
-    <row r="120">
+    <row r="120" spans="1:28" ht="12.6" x14ac:dyDescent="0.45">
       <c r="A120" s="53" t="s">
         <v>274</v>
       </c>
@@ -4350,7 +4652,7 @@
       <c r="AA120" s="49"/>
       <c r="AB120" s="49"/>
     </row>
-    <row r="121">
+    <row r="121" spans="1:28" ht="12.6" x14ac:dyDescent="0.45">
       <c r="A121" s="53" t="s">
         <v>277</v>
       </c>
@@ -4373,7 +4675,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:28" ht="12.6" x14ac:dyDescent="0.45">
       <c r="A122" s="53" t="s">
         <v>279</v>
       </c>
@@ -4396,7 +4698,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:28" ht="12.6" x14ac:dyDescent="0.45">
       <c r="A123" s="48" t="s">
         <v>252</v>
       </c>
@@ -4439,7 +4741,7 @@
       <c r="AA123" s="49"/>
       <c r="AB123" s="49"/>
     </row>
-    <row r="126">
+    <row r="126" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A126" s="32"/>
       <c r="B126" s="32"/>
       <c r="C126" s="32"/>
@@ -4471,108 +4773,109 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="H7"/>
-    <hyperlink r:id="rId2" ref="H8"/>
-    <hyperlink r:id="rId3" ref="H9"/>
-    <hyperlink r:id="rId4" ref="H10"/>
-    <hyperlink r:id="rId5" ref="H11"/>
-    <hyperlink r:id="rId6" ref="H12"/>
-    <hyperlink r:id="rId7" ref="H13"/>
-    <hyperlink r:id="rId8" ref="H15"/>
-    <hyperlink r:id="rId9" ref="H16"/>
-    <hyperlink r:id="rId10" ref="H17"/>
-    <hyperlink r:id="rId11" ref="H23"/>
-    <hyperlink r:id="rId12" ref="H24"/>
-    <hyperlink r:id="rId13" ref="H25"/>
-    <hyperlink r:id="rId14" ref="H26"/>
-    <hyperlink r:id="rId15" ref="H27"/>
-    <hyperlink r:id="rId16" ref="H28"/>
-    <hyperlink r:id="rId17" ref="H29"/>
-    <hyperlink r:id="rId18" ref="H31"/>
-    <hyperlink r:id="rId19" ref="H32"/>
-    <hyperlink r:id="rId20" ref="H33"/>
-    <hyperlink r:id="rId21" ref="H34"/>
-    <hyperlink r:id="rId22" ref="H35"/>
-    <hyperlink r:id="rId23" ref="H36"/>
-    <hyperlink r:id="rId24" ref="H37"/>
-    <hyperlink r:id="rId25" ref="H38"/>
-    <hyperlink r:id="rId26" ref="H39"/>
-    <hyperlink r:id="rId27" ref="H40"/>
-    <hyperlink r:id="rId28" ref="H41"/>
-    <hyperlink r:id="rId29" ref="H46"/>
-    <hyperlink r:id="rId30" ref="H47"/>
-    <hyperlink r:id="rId31" ref="H48"/>
-    <hyperlink r:id="rId32" ref="H49"/>
-    <hyperlink r:id="rId33" ref="H50"/>
-    <hyperlink r:id="rId34" ref="H52"/>
-    <hyperlink r:id="rId35" ref="H53"/>
-    <hyperlink r:id="rId36" ref="H59"/>
-    <hyperlink r:id="rId37" ref="H60"/>
-    <hyperlink r:id="rId38" ref="H61"/>
-    <hyperlink r:id="rId39" ref="H62"/>
-    <hyperlink r:id="rId40" ref="H63"/>
-    <hyperlink r:id="rId41" ref="H70"/>
-    <hyperlink r:id="rId42" ref="H71"/>
-    <hyperlink r:id="rId43" ref="H72"/>
-    <hyperlink r:id="rId44" ref="H73"/>
-    <hyperlink r:id="rId45" ref="H74"/>
-    <hyperlink r:id="rId46" ref="H75"/>
-    <hyperlink r:id="rId47" ref="H76"/>
-    <hyperlink r:id="rId48" ref="H77"/>
-    <hyperlink r:id="rId49" ref="H78"/>
-    <hyperlink r:id="rId50" ref="H79"/>
-    <hyperlink r:id="rId51" ref="H80"/>
-    <hyperlink r:id="rId52" ref="H81"/>
-    <hyperlink r:id="rId53" ref="H82"/>
-    <hyperlink r:id="rId54" ref="H84"/>
-    <hyperlink r:id="rId55" ref="H85"/>
-    <hyperlink r:id="rId56" ref="H91"/>
-    <hyperlink r:id="rId57" ref="H92"/>
-    <hyperlink r:id="rId58" ref="H97"/>
-    <hyperlink r:id="rId59" ref="H98"/>
-    <hyperlink r:id="rId60" ref="H99"/>
-    <hyperlink r:id="rId61" ref="H100"/>
-    <hyperlink r:id="rId62" ref="H101"/>
-    <hyperlink r:id="rId63" ref="H102"/>
-    <hyperlink r:id="rId64" ref="H103"/>
-    <hyperlink r:id="rId65" ref="H104"/>
-    <hyperlink r:id="rId66" ref="H105"/>
-    <hyperlink r:id="rId67" ref="H106"/>
-    <hyperlink r:id="rId68" location="product-description-iframe" ref="H107"/>
-    <hyperlink r:id="rId69" ref="H108"/>
-    <hyperlink r:id="rId70" ref="H109"/>
-    <hyperlink r:id="rId71" ref="H110"/>
-    <hyperlink r:id="rId72" ref="H115"/>
-    <hyperlink r:id="rId73" ref="H116"/>
-    <hyperlink r:id="rId74" ref="H117"/>
-    <hyperlink r:id="rId75" ref="H118"/>
-    <hyperlink r:id="rId76" ref="H119"/>
+    <hyperlink ref="H7" r:id="rId1"/>
+    <hyperlink ref="H8" r:id="rId2"/>
+    <hyperlink ref="H9" r:id="rId3"/>
+    <hyperlink ref="H10" r:id="rId4"/>
+    <hyperlink ref="H11" r:id="rId5"/>
+    <hyperlink ref="H12" r:id="rId6"/>
+    <hyperlink ref="H13" r:id="rId7"/>
+    <hyperlink ref="H15" r:id="rId8"/>
+    <hyperlink ref="H16" r:id="rId9"/>
+    <hyperlink ref="H17" r:id="rId10"/>
+    <hyperlink ref="H23" r:id="rId11"/>
+    <hyperlink ref="H24" r:id="rId12"/>
+    <hyperlink ref="H25" r:id="rId13"/>
+    <hyperlink ref="H26" r:id="rId14"/>
+    <hyperlink ref="H27" r:id="rId15"/>
+    <hyperlink ref="H28" r:id="rId16"/>
+    <hyperlink ref="H29" r:id="rId17"/>
+    <hyperlink ref="H31" r:id="rId18"/>
+    <hyperlink ref="H32" r:id="rId19"/>
+    <hyperlink ref="H33" r:id="rId20"/>
+    <hyperlink ref="H34" r:id="rId21"/>
+    <hyperlink ref="H35" r:id="rId22"/>
+    <hyperlink ref="H36" r:id="rId23"/>
+    <hyperlink ref="H37" r:id="rId24"/>
+    <hyperlink ref="H38" r:id="rId25"/>
+    <hyperlink ref="H39" r:id="rId26"/>
+    <hyperlink ref="H40" r:id="rId27"/>
+    <hyperlink ref="H41" r:id="rId28"/>
+    <hyperlink ref="H46" r:id="rId29"/>
+    <hyperlink ref="H47" r:id="rId30"/>
+    <hyperlink ref="H48" r:id="rId31"/>
+    <hyperlink ref="H49" r:id="rId32"/>
+    <hyperlink ref="H50" r:id="rId33"/>
+    <hyperlink ref="H52" r:id="rId34"/>
+    <hyperlink ref="H53" r:id="rId35"/>
+    <hyperlink ref="H59" r:id="rId36"/>
+    <hyperlink ref="H60" r:id="rId37"/>
+    <hyperlink ref="H61" r:id="rId38"/>
+    <hyperlink ref="H62" r:id="rId39"/>
+    <hyperlink ref="H63" r:id="rId40"/>
+    <hyperlink ref="H70" r:id="rId41"/>
+    <hyperlink ref="H71" r:id="rId42"/>
+    <hyperlink ref="H72" r:id="rId43"/>
+    <hyperlink ref="H73" r:id="rId44"/>
+    <hyperlink ref="H74" r:id="rId45"/>
+    <hyperlink ref="H75" r:id="rId46"/>
+    <hyperlink ref="H76" r:id="rId47"/>
+    <hyperlink ref="H77" r:id="rId48"/>
+    <hyperlink ref="H78" r:id="rId49"/>
+    <hyperlink ref="H79" r:id="rId50"/>
+    <hyperlink ref="H80" r:id="rId51"/>
+    <hyperlink ref="H81" r:id="rId52"/>
+    <hyperlink ref="H82" r:id="rId53"/>
+    <hyperlink ref="H84" r:id="rId54"/>
+    <hyperlink ref="H85" r:id="rId55"/>
+    <hyperlink ref="H91" r:id="rId56"/>
+    <hyperlink ref="H92" r:id="rId57"/>
+    <hyperlink ref="H97" r:id="rId58"/>
+    <hyperlink ref="H98" r:id="rId59"/>
+    <hyperlink ref="H99" r:id="rId60"/>
+    <hyperlink ref="H100" r:id="rId61"/>
+    <hyperlink ref="H101" r:id="rId62"/>
+    <hyperlink ref="H102" r:id="rId63"/>
+    <hyperlink ref="H103" r:id="rId64"/>
+    <hyperlink ref="H104" r:id="rId65"/>
+    <hyperlink ref="H105" r:id="rId66"/>
+    <hyperlink ref="H106" r:id="rId67"/>
+    <hyperlink ref="H107" r:id="rId68" location="product-description-iframe"/>
+    <hyperlink ref="H108" r:id="rId69"/>
+    <hyperlink ref="H109" r:id="rId70"/>
+    <hyperlink ref="H110" r:id="rId71"/>
+    <hyperlink ref="H115" r:id="rId72"/>
+    <hyperlink ref="H116" r:id="rId73"/>
+    <hyperlink ref="H117" r:id="rId74"/>
+    <hyperlink ref="H118" r:id="rId75"/>
+    <hyperlink ref="H119" r:id="rId76"/>
   </hyperlinks>
-  <drawing r:id="rId77"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AB31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="21.86"/>
-    <col customWidth="1" min="6" max="6" width="18.57"/>
-    <col customWidth="1" min="7" max="7" width="64.86"/>
+    <col min="4" max="4" width="21.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" customWidth="1"/>
+    <col min="7" max="7" width="64.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -4580,17 +4883,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -4604,7 +4907,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -4615,7 +4918,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -4632,7 +4935,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -4646,7 +4949,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -4663,7 +4966,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D13" s="10" t="s">
         <v>32</v>
       </c>
@@ -4671,7 +4974,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D14" s="10" t="s">
         <v>35</v>
       </c>
@@ -4679,7 +4982,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D15" s="10" t="s">
         <v>38</v>
       </c>
@@ -4687,11 +4990,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D17" s="10" t="s">
         <v>42</v>
       </c>
@@ -4699,17 +5002,17 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E18" s="22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E19" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>48</v>
       </c>
@@ -4723,17 +5026,17 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A28" s="16" t="s">
         <v>55</v>
       </c>
@@ -4744,10 +5047,10 @@
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
       <c r="F28" s="24">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G28" s="24">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="H28" s="26" t="s">
         <v>66</v>
@@ -4773,7 +5076,7 @@
       <c r="AA28" s="16"/>
       <c r="AB28" s="16"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A29" s="16" t="s">
         <v>70</v>
       </c>
@@ -4784,10 +5087,10 @@
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
       <c r="F29" s="24">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="24">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="H29" s="26" t="s">
         <v>71</v>
@@ -4813,7 +5116,7 @@
       <c r="AA29" s="16"/>
       <c r="AB29" s="16"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A30" s="25" t="s">
         <v>73</v>
       </c>
@@ -4826,7 +5129,7 @@
         <v>75</v>
       </c>
       <c r="F30" s="24">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="G30" s="31">
         <v>0.5</v>
@@ -4855,7 +5158,7 @@
       <c r="AA30" s="16"/>
       <c r="AB30" s="16"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A31" s="25" t="s">
         <v>78</v>
       </c>
@@ -4866,7 +5169,7 @@
       </c>
       <c r="E31" s="16"/>
       <c r="F31" s="24">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="G31" s="31">
         <v>1.5</v>
@@ -4897,22 +5200,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D7"/>
-    <hyperlink r:id="rId2" ref="D8"/>
-    <hyperlink r:id="rId3" ref="D9"/>
-    <hyperlink r:id="rId4" ref="G9"/>
-    <hyperlink r:id="rId5" ref="D10"/>
-    <hyperlink r:id="rId6" ref="D11"/>
-    <hyperlink r:id="rId7" ref="D13"/>
-    <hyperlink r:id="rId8" ref="D14"/>
-    <hyperlink r:id="rId9" ref="D15"/>
-    <hyperlink r:id="rId10" ref="D17"/>
-    <hyperlink r:id="rId11" ref="D20"/>
-    <hyperlink r:id="rId12" ref="H28"/>
-    <hyperlink r:id="rId13" ref="H29"/>
-    <hyperlink r:id="rId14" ref="H30"/>
-    <hyperlink r:id="rId15" ref="H31"/>
+    <hyperlink ref="D7" r:id="rId1"/>
+    <hyperlink ref="D8" r:id="rId2"/>
+    <hyperlink ref="D9" r:id="rId3"/>
+    <hyperlink ref="G9" r:id="rId4"/>
+    <hyperlink ref="D10" r:id="rId5"/>
+    <hyperlink ref="D11" r:id="rId6"/>
+    <hyperlink ref="D13" r:id="rId7"/>
+    <hyperlink ref="D14" r:id="rId8"/>
+    <hyperlink ref="D15" r:id="rId9"/>
+    <hyperlink ref="D17" r:id="rId10"/>
+    <hyperlink ref="D20" r:id="rId11"/>
+    <hyperlink ref="H28" r:id="rId12"/>
+    <hyperlink ref="H29" r:id="rId13"/>
+    <hyperlink ref="H30" r:id="rId14"/>
+    <hyperlink ref="H31" r:id="rId15"/>
   </hyperlinks>
-  <drawing r:id="rId16"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Updated main code to current LED strip + sensors."
This reverts commit e346d15b47c64aa68b4e26eb6b5f228a005aae59.
</commit_message>
<xml_diff>
--- a/hardware/SeeBoat_fullPartsList.xlsx
+++ b/hardware/SeeBoat_fullPartsList.xlsx
@@ -1,26 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\talia\Documents\GitHub\seeboat\hardware\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11478" windowHeight="8484"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <workbookPr/>
   <sheets>
-    <sheet name="final" sheetId="1" r:id="rId1"/>
-    <sheet name="scrap" sheetId="2" r:id="rId2"/>
+    <sheet state="visible" name="final" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="scrap" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="316">
   <si>
     <t>Parts list for SeeBoat &amp; full sensor suite</t>
   </si>
@@ -968,191 +960,130 @@
   </si>
   <si>
     <t>for waterproofing the electronics</t>
-  </si>
-  <si>
-    <t>6-32 1/2'' Phillips</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="mmmm\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="mmmm yyyy"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="26">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
       <i/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+    </font>
+    <font/>
+    <font>
+      <b/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <i/>
       <u/>
-      <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <i/>
       <u/>
-      <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <i/>
       <u/>
-      <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <i/>
       <u/>
-      <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <i/>
       <u/>
-      <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <i/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <i/>
-      <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <i/>
       <u/>
-      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1160,7 +1091,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1176,486 +1107,256 @@
     </fill>
   </fills>
   <borders count="10">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
-      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
-      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="59">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+  <cellXfs count="58">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="9" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="18" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="19" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="23" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="21.0"/>
+    <col customWidth="1" min="5" max="5" width="21.14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1668,15 +1369,15 @@
       <c r="H1" s="3"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3">
       <c r="A3" s="9">
-        <v>43221</v>
+        <v>43221.0</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -1687,13 +1388,13 @@
       <c r="H3" s="11"/>
       <c r="I3" s="12"/>
     </row>
-    <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="13"/>
     </row>
-    <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6">
       <c r="A6" s="14" t="s">
         <v>19</v>
       </c>
@@ -1737,7 +1438,7 @@
       <c r="AA6" s="16"/>
       <c r="AB6" s="16"/>
     </row>
-    <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7">
       <c r="A7" s="2" t="s">
         <v>39</v>
       </c>
@@ -1751,16 +1452,16 @@
         <v>46</v>
       </c>
       <c r="F7" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G7" s="23">
-        <v>230</v>
+        <v>230.0</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8">
       <c r="A8" s="2" t="s">
         <v>56</v>
       </c>
@@ -1771,16 +1472,16 @@
         <v>58</v>
       </c>
       <c r="F8" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G8" s="23">
-        <v>50</v>
+        <v>50.0</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9">
       <c r="A9" s="22" t="s">
         <v>60</v>
       </c>
@@ -1791,16 +1492,16 @@
         <v>62</v>
       </c>
       <c r="F9" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G9" s="23">
-        <v>7</v>
+        <v>7.0</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10">
       <c r="A10" s="2" t="s">
         <v>64</v>
       </c>
@@ -1811,16 +1512,16 @@
         <v>65</v>
       </c>
       <c r="F10" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G10" s="23">
-        <v>8</v>
+        <v>8.0</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11">
       <c r="A11" s="25" t="s">
         <v>68</v>
       </c>
@@ -1833,10 +1534,10 @@
         <v>69</v>
       </c>
       <c r="F11" s="29">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="G11" s="30">
-        <v>15</v>
+        <v>15.0</v>
       </c>
       <c r="H11" s="26" t="s">
         <v>72</v>
@@ -1862,7 +1563,7 @@
       <c r="AA11" s="16"/>
       <c r="AB11" s="16"/>
     </row>
-    <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12">
       <c r="A12" s="2" t="s">
         <v>77</v>
       </c>
@@ -1873,16 +1574,16 @@
         <v>62</v>
       </c>
       <c r="F12" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G12" s="23">
-        <v>10</v>
+        <v>10.0</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13">
       <c r="A13" s="2" t="s">
         <v>81</v>
       </c>
@@ -1893,16 +1594,16 @@
         <v>82</v>
       </c>
       <c r="F13" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G13" s="23">
-        <v>7</v>
+        <v>7.0</v>
       </c>
       <c r="H13" s="10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15">
       <c r="A15" s="22" t="s">
         <v>84</v>
       </c>
@@ -1913,16 +1614,16 @@
         <v>86</v>
       </c>
       <c r="F15" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G15" s="23">
-        <v>46</v>
+        <v>46.0</v>
       </c>
       <c r="H15" s="10" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16">
       <c r="A16" s="22" t="s">
         <v>88</v>
       </c>
@@ -1933,16 +1634,16 @@
         <v>86</v>
       </c>
       <c r="F16" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G16" s="23">
-        <v>126</v>
+        <v>126.0</v>
       </c>
       <c r="H16" s="10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17">
       <c r="A17" s="22" t="s">
         <v>90</v>
       </c>
@@ -1953,20 +1654,20 @@
         <v>91</v>
       </c>
       <c r="F17" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G17" s="23">
-        <v>160</v>
+        <v>160.0</v>
       </c>
       <c r="H17" s="10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18">
       <c r="A18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19">
       <c r="A19" s="32"/>
       <c r="B19" s="32"/>
       <c r="C19" s="32"/>
@@ -1996,13 +1697,13 @@
       <c r="AA19" s="32"/>
       <c r="AB19" s="32"/>
     </row>
-    <row r="20" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20">
       <c r="A20" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D20" s="13"/>
     </row>
-    <row r="21" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21">
       <c r="A21" s="14" t="s">
         <v>19</v>
       </c>
@@ -2046,7 +1747,7 @@
       <c r="AA21" s="16"/>
       <c r="AB21" s="16"/>
     </row>
-    <row r="22" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22">
       <c r="A22" s="25" t="s">
         <v>94</v>
       </c>
@@ -2059,10 +1760,10 @@
         <v>95</v>
       </c>
       <c r="F22" s="29">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G22" s="30">
-        <v>35</v>
+        <v>35.0</v>
       </c>
       <c r="H22" s="33" t="s">
         <v>96</v>
@@ -2088,7 +1789,7 @@
       <c r="AA22" s="16"/>
       <c r="AB22" s="16"/>
     </row>
-    <row r="23" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23">
       <c r="A23" s="25" t="s">
         <v>97</v>
       </c>
@@ -2101,10 +1802,10 @@
         <v>98</v>
       </c>
       <c r="F23" s="29">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G23" s="30">
-        <v>40</v>
+        <v>40.0</v>
       </c>
       <c r="H23" s="26" t="s">
         <v>99</v>
@@ -2130,7 +1831,7 @@
       <c r="AA23" s="16"/>
       <c r="AB23" s="16"/>
     </row>
-    <row r="24" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24">
       <c r="A24" s="25" t="s">
         <v>100</v>
       </c>
@@ -2143,10 +1844,10 @@
         <v>101</v>
       </c>
       <c r="F24" s="29">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G24" s="30">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H24" s="26" t="s">
         <v>102</v>
@@ -2172,7 +1873,7 @@
       <c r="AA24" s="16"/>
       <c r="AB24" s="16"/>
     </row>
-    <row r="25" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25">
       <c r="A25" s="25" t="s">
         <v>103</v>
       </c>
@@ -2185,10 +1886,10 @@
         <v>75</v>
       </c>
       <c r="F25" s="24">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="G25" s="31">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="H25" s="26" t="s">
         <v>104</v>
@@ -2214,7 +1915,7 @@
       <c r="AA25" s="16"/>
       <c r="AB25" s="16"/>
     </row>
-    <row r="26" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26">
       <c r="A26" s="25" t="s">
         <v>105</v>
       </c>
@@ -2227,7 +1928,7 @@
         <v>106</v>
       </c>
       <c r="F26" s="24">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="G26" s="31">
         <v>1.25</v>
@@ -2256,7 +1957,7 @@
       <c r="AA26" s="16"/>
       <c r="AB26" s="16"/>
     </row>
-    <row r="27" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="27">
       <c r="A27" s="25" t="s">
         <v>108</v>
       </c>
@@ -2269,10 +1970,10 @@
         <v>109</v>
       </c>
       <c r="F27" s="24">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="G27" s="31">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H27" s="26" t="s">
         <v>110</v>
@@ -2298,7 +1999,7 @@
       <c r="AA27" s="16"/>
       <c r="AB27" s="16"/>
     </row>
-    <row r="28" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="28">
       <c r="A28" s="25" t="s">
         <v>111</v>
       </c>
@@ -2311,7 +2012,7 @@
         <v>113</v>
       </c>
       <c r="F28" s="24">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G28" s="31">
         <v>5.59</v>
@@ -2340,7 +2041,7 @@
       <c r="AA28" s="16"/>
       <c r="AB28" s="16"/>
     </row>
-    <row r="29" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="29">
       <c r="A29" s="25" t="s">
         <v>115</v>
       </c>
@@ -2353,10 +2054,10 @@
         <v>116</v>
       </c>
       <c r="F29" s="34">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G29" s="30">
-        <v>15</v>
+        <v>15.0</v>
       </c>
       <c r="H29" s="26" t="s">
         <v>117</v>
@@ -2380,14 +2081,14 @@
       <c r="Y29" s="16"/>
       <c r="Z29" s="16"/>
     </row>
-    <row r="30" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="30">
       <c r="A30" s="35"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="31">
       <c r="A31" s="35" t="s">
         <v>118</v>
       </c>
@@ -2398,16 +2099,16 @@
         <v>120</v>
       </c>
       <c r="F31" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G31" s="23">
-        <v>5</v>
+        <v>5.0</v>
       </c>
       <c r="H31" s="10" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="32">
       <c r="A32" s="2" t="s">
         <v>122</v>
       </c>
@@ -2421,7 +2122,7 @@
         <v>125</v>
       </c>
       <c r="F32" s="2">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="G32" s="36">
         <v>0.1</v>
@@ -2430,7 +2131,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="33">
       <c r="A33" s="2" t="s">
         <v>127</v>
       </c>
@@ -2444,7 +2145,7 @@
         <v>129</v>
       </c>
       <c r="F33" s="2">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="G33" s="36">
         <v>0.1</v>
@@ -2453,7 +2154,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="34">
       <c r="A34" s="2" t="s">
         <v>131</v>
       </c>
@@ -2467,7 +2168,7 @@
         <v>133</v>
       </c>
       <c r="F34" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G34" s="37">
         <v>1.07</v>
@@ -2476,12 +2177,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="35">
       <c r="A35" s="2" t="s">
         <v>135</v>
       </c>
       <c r="C35" s="22">
-        <v>2343</v>
+        <v>2343.0</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>74</v>
@@ -2490,7 +2191,7 @@
         <v>136</v>
       </c>
       <c r="F35" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G35" s="36">
         <v>4.5</v>
@@ -2499,7 +2200,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="36" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="36">
       <c r="A36" s="2" t="s">
         <v>138</v>
       </c>
@@ -2513,7 +2214,7 @@
         <v>140</v>
       </c>
       <c r="F36" s="2">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="G36" s="36">
         <v>0.94</v>
@@ -2522,7 +2223,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="37" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="37">
       <c r="A37" s="2" t="s">
         <v>142</v>
       </c>
@@ -2536,7 +2237,7 @@
         <v>144</v>
       </c>
       <c r="F37" s="2">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="G37" s="36">
         <v>1.46</v>
@@ -2545,7 +2246,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="38" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="38">
       <c r="A38" s="2" t="s">
         <v>146</v>
       </c>
@@ -2559,7 +2260,7 @@
         <v>148</v>
       </c>
       <c r="F38" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G38" s="36">
         <v>0.87</v>
@@ -2568,7 +2269,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="39" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="39">
       <c r="A39" s="2" t="s">
         <v>150</v>
       </c>
@@ -2582,7 +2283,7 @@
         <v>152</v>
       </c>
       <c r="F39" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G39" s="36">
         <v>0.99</v>
@@ -2591,7 +2292,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="40" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="40">
       <c r="A40" s="2" t="s">
         <v>154</v>
       </c>
@@ -2605,7 +2306,7 @@
         <v>156</v>
       </c>
       <c r="F40" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G40" s="36">
         <v>95.15</v>
@@ -2617,7 +2318,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="41" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="41">
       <c r="A41" s="16" t="s">
         <v>159</v>
       </c>
@@ -2634,10 +2335,10 @@
         <v>161</v>
       </c>
       <c r="F41" s="24">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G41" s="38">
-        <v>16</v>
+        <v>16.0</v>
       </c>
       <c r="H41" s="26" t="s">
         <v>162</v>
@@ -2663,7 +2364,7 @@
       <c r="AA41" s="16"/>
       <c r="AB41" s="16"/>
     </row>
-    <row r="43" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="43">
       <c r="A43" s="32"/>
       <c r="B43" s="32"/>
       <c r="C43" s="32"/>
@@ -2693,13 +2394,13 @@
       <c r="AA43" s="32"/>
       <c r="AB43" s="32"/>
     </row>
-    <row r="44" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="44">
       <c r="A44" s="4" t="s">
         <v>163</v>
       </c>
       <c r="D44" s="13"/>
     </row>
-    <row r="45" spans="1:28" ht="12.6" x14ac:dyDescent="0.45">
+    <row r="45">
       <c r="A45" s="14" t="s">
         <v>19</v>
       </c>
@@ -2743,7 +2444,7 @@
       <c r="AA45" s="16"/>
       <c r="AB45" s="16"/>
     </row>
-    <row r="46" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="46">
       <c r="A46" s="39" t="s">
         <v>164</v>
       </c>
@@ -2756,10 +2457,10 @@
         <v>165</v>
       </c>
       <c r="F46" s="24">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G46" s="30">
-        <v>30</v>
+        <v>30.0</v>
       </c>
       <c r="H46" s="26" t="s">
         <v>166</v>
@@ -2784,7 +2485,7 @@
       <c r="AA46" s="16"/>
       <c r="AB46" s="16"/>
     </row>
-    <row r="47" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="47">
       <c r="A47" s="25" t="s">
         <v>167</v>
       </c>
@@ -2797,10 +2498,10 @@
         <v>168</v>
       </c>
       <c r="F47" s="24">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G47" s="38">
-        <v>31</v>
+        <v>31.0</v>
       </c>
       <c r="H47" s="26" t="s">
         <v>169</v>
@@ -2825,7 +2526,7 @@
       <c r="AA47" s="16"/>
       <c r="AB47" s="16"/>
     </row>
-    <row r="48" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="48">
       <c r="A48" s="35" t="s">
         <v>170</v>
       </c>
@@ -2836,16 +2537,16 @@
         <v>172</v>
       </c>
       <c r="F48" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G48" s="23">
-        <v>8</v>
+        <v>8.0</v>
       </c>
       <c r="H48" s="10" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="49" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="49">
       <c r="A49" s="2" t="s">
         <v>174</v>
       </c>
@@ -2856,16 +2557,16 @@
         <v>175</v>
       </c>
       <c r="F49" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G49" s="23">
-        <v>27</v>
+        <v>27.0</v>
       </c>
       <c r="H49" s="10" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="50" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="50">
       <c r="A50" s="35" t="s">
         <v>177</v>
       </c>
@@ -2876,16 +2577,16 @@
         <v>178</v>
       </c>
       <c r="F50" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G50" s="23">
-        <v>25</v>
+        <v>25.0</v>
       </c>
       <c r="H50" s="10" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="51">
       <c r="A51" s="35" t="s">
         <v>180</v>
       </c>
@@ -2896,13 +2597,13 @@
         <v>182</v>
       </c>
       <c r="F51" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G51" s="23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="52">
       <c r="A52" s="35" t="s">
         <v>183</v>
       </c>
@@ -2913,16 +2614,16 @@
         <v>184</v>
       </c>
       <c r="F52" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G52" s="23">
-        <v>10</v>
+        <v>10.0</v>
       </c>
       <c r="H52" s="10" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="53" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="53">
       <c r="A53" s="35" t="s">
         <v>186</v>
       </c>
@@ -2933,22 +2634,22 @@
         <v>188</v>
       </c>
       <c r="F53" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G53" s="23">
-        <v>10</v>
+        <v>10.0</v>
       </c>
       <c r="H53" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="54">
       <c r="A54" s="4"/>
     </row>
-    <row r="55" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="55">
       <c r="A55" s="4"/>
     </row>
-    <row r="56" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="56">
       <c r="A56" s="32"/>
       <c r="B56" s="32"/>
       <c r="C56" s="32"/>
@@ -2978,13 +2679,13 @@
       <c r="AA56" s="32"/>
       <c r="AB56" s="32"/>
     </row>
-    <row r="57" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="57">
       <c r="A57" s="4" t="s">
         <v>189</v>
       </c>
       <c r="D57" s="13"/>
     </row>
-    <row r="58" spans="1:28" ht="12.6" x14ac:dyDescent="0.45">
+    <row r="58">
       <c r="A58" s="14" t="s">
         <v>19</v>
       </c>
@@ -3028,7 +2729,7 @@
       <c r="AA58" s="16"/>
       <c r="AB58" s="16"/>
     </row>
-    <row r="59" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="59">
       <c r="A59" s="16" t="s">
         <v>190</v>
       </c>
@@ -3041,10 +2742,10 @@
         <v>192</v>
       </c>
       <c r="F59" s="24">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G59" s="30">
-        <v>38</v>
+        <v>38.0</v>
       </c>
       <c r="H59" s="26" t="s">
         <v>193</v>
@@ -3068,7 +2769,7 @@
       <c r="Y59" s="16"/>
       <c r="Z59" s="16"/>
     </row>
-    <row r="60" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="60">
       <c r="A60" s="25" t="s">
         <v>194</v>
       </c>
@@ -3081,10 +2782,10 @@
         <v>192</v>
       </c>
       <c r="F60" s="24">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G60" s="30">
-        <v>72</v>
+        <v>72.0</v>
       </c>
       <c r="H60" s="26" t="s">
         <v>195</v>
@@ -3108,7 +2809,7 @@
       <c r="Y60" s="16"/>
       <c r="Z60" s="16"/>
     </row>
-    <row r="61" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="61">
       <c r="A61" s="25" t="s">
         <v>196</v>
       </c>
@@ -3121,10 +2822,10 @@
         <v>197</v>
       </c>
       <c r="F61" s="24">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G61" s="38">
-        <v>40</v>
+        <v>40.0</v>
       </c>
       <c r="H61" s="26" t="s">
         <v>198</v>
@@ -3148,7 +2849,7 @@
       <c r="Y61" s="16"/>
       <c r="Z61" s="16"/>
     </row>
-    <row r="62" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="62">
       <c r="A62" s="2" t="s">
         <v>199</v>
       </c>
@@ -3159,16 +2860,16 @@
         <v>201</v>
       </c>
       <c r="F62" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G62" s="23">
-        <v>30</v>
+        <v>30.0</v>
       </c>
       <c r="H62" s="10" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="63" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="63">
       <c r="A63" s="2" t="s">
         <v>203</v>
       </c>
@@ -3179,19 +2880,19 @@
         <v>204</v>
       </c>
       <c r="F63" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G63" s="23">
-        <v>12</v>
+        <v>12.0</v>
       </c>
       <c r="H63" s="10" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="64" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="64">
       <c r="A64" s="2"/>
     </row>
-    <row r="65" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="65">
       <c r="A65" s="2" t="s">
         <v>206</v>
       </c>
@@ -3202,10 +2903,10 @@
         <v>208</v>
       </c>
     </row>
-    <row r="66" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="66">
       <c r="A66" s="2"/>
     </row>
-    <row r="67" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="67">
       <c r="A67" s="32"/>
       <c r="B67" s="32"/>
       <c r="C67" s="32"/>
@@ -3235,12 +2936,12 @@
       <c r="AA67" s="32"/>
       <c r="AB67" s="32"/>
     </row>
-    <row r="68" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="68">
       <c r="A68" s="4" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="69" spans="1:28" ht="12.6" x14ac:dyDescent="0.45">
+    <row r="69">
       <c r="A69" s="14" t="s">
         <v>19</v>
       </c>
@@ -3284,7 +2985,7 @@
       <c r="AA69" s="16"/>
       <c r="AB69" s="16"/>
     </row>
-    <row r="70" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="70">
       <c r="A70" s="2" t="s">
         <v>210</v>
       </c>
@@ -3293,16 +2994,16 @@
       </c>
       <c r="E70" s="40"/>
       <c r="F70" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G70" s="23">
-        <v>7</v>
+        <v>7.0</v>
       </c>
       <c r="H70" s="10" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="71" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="71">
       <c r="A71" s="2" t="s">
         <v>212</v>
       </c>
@@ -3313,7 +3014,7 @@
         <v>124</v>
       </c>
       <c r="F71" s="2">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="G71" s="36">
         <v>0.17</v>
@@ -3322,7 +3023,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="72" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="72">
       <c r="A72" s="27" t="s">
         <v>215</v>
       </c>
@@ -3335,7 +3036,7 @@
       </c>
       <c r="E72" s="27"/>
       <c r="F72" s="29">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G72" s="36">
         <v>0.1</v>
@@ -3364,7 +3065,7 @@
       <c r="AA72" s="16"/>
       <c r="AB72" s="16"/>
     </row>
-    <row r="73" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="73">
       <c r="A73" s="27" t="s">
         <v>217</v>
       </c>
@@ -3377,7 +3078,7 @@
       </c>
       <c r="E73" s="27"/>
       <c r="F73" s="29">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G73" s="37">
         <v>0.34</v>
@@ -3406,7 +3107,7 @@
       <c r="AA73" s="16"/>
       <c r="AB73" s="16"/>
     </row>
-    <row r="74" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="74">
       <c r="A74" s="27" t="s">
         <v>220</v>
       </c>
@@ -3419,7 +3120,7 @@
       </c>
       <c r="E74" s="27"/>
       <c r="F74" s="29">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="G74" s="36">
         <v>0.1</v>
@@ -3448,7 +3149,7 @@
       <c r="AA74" s="16"/>
       <c r="AB74" s="16"/>
     </row>
-    <row r="75" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="75">
       <c r="A75" s="27" t="s">
         <v>223</v>
       </c>
@@ -3461,7 +3162,7 @@
       </c>
       <c r="E75" s="27"/>
       <c r="F75" s="29">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G75" s="36">
         <v>0.34</v>
@@ -3490,7 +3191,7 @@
       <c r="AA75" s="16"/>
       <c r="AB75" s="16"/>
     </row>
-    <row r="76" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="76">
       <c r="A76" s="27" t="s">
         <v>226</v>
       </c>
@@ -3503,7 +3204,7 @@
       </c>
       <c r="E76" s="27"/>
       <c r="F76" s="29">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G76" s="37">
         <v>0.12</v>
@@ -3532,7 +3233,7 @@
       <c r="AA76" s="16"/>
       <c r="AB76" s="16"/>
     </row>
-    <row r="77" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="77">
       <c r="A77" s="27" t="s">
         <v>229</v>
       </c>
@@ -3544,7 +3245,7 @@
         <v>124</v>
       </c>
       <c r="F77" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G77" s="31">
         <v>0.32</v>
@@ -3573,7 +3274,7 @@
       <c r="AA77" s="16"/>
       <c r="AB77" s="16"/>
     </row>
-    <row r="78" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="78">
       <c r="A78" s="43" t="s">
         <v>232</v>
       </c>
@@ -3585,7 +3286,7 @@
       </c>
       <c r="E78" s="40"/>
       <c r="F78" s="44">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="G78" s="36">
         <v>0.37</v>
@@ -3594,7 +3295,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="79" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="79">
       <c r="A79" s="27" t="s">
         <v>235</v>
       </c>
@@ -3606,7 +3307,7 @@
         <v>124</v>
       </c>
       <c r="F79" s="29">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G79" s="30">
         <v>1.86</v>
@@ -3633,7 +3334,7 @@
       <c r="Y79" s="16"/>
       <c r="Z79" s="16"/>
     </row>
-    <row r="80" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="80">
       <c r="A80" s="27" t="s">
         <v>238</v>
       </c>
@@ -3645,7 +3346,7 @@
         <v>124</v>
       </c>
       <c r="F80" s="29">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G80" s="37">
         <v>2.64</v>
@@ -3672,7 +3373,7 @@
       <c r="Y80" s="16"/>
       <c r="Z80" s="16"/>
     </row>
-    <row r="81" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="81">
       <c r="A81" s="27" t="s">
         <v>238</v>
       </c>
@@ -3682,7 +3383,7 @@
       </c>
       <c r="E81" s="25"/>
       <c r="F81" s="29">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G81" s="30">
         <v>1.81</v>
@@ -3709,7 +3410,7 @@
       <c r="Y81" s="16"/>
       <c r="Z81" s="16"/>
     </row>
-    <row r="82" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="82">
       <c r="A82" s="2" t="s">
         <v>131</v>
       </c>
@@ -3723,7 +3424,7 @@
         <v>243</v>
       </c>
       <c r="F82" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G82" s="37">
         <v>1.07</v>
@@ -3732,7 +3433,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="83">
       <c r="A83" s="16"/>
       <c r="B83" s="16"/>
       <c r="C83" s="22"/>
@@ -3762,7 +3463,7 @@
       <c r="AA83" s="16"/>
       <c r="AB83" s="16"/>
     </row>
-    <row r="84" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="84">
       <c r="A84" s="16" t="s">
         <v>244</v>
       </c>
@@ -3779,10 +3480,10 @@
         <v>246</v>
       </c>
       <c r="F84" s="24">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G84" s="38">
-        <v>16</v>
+        <v>16.0</v>
       </c>
       <c r="H84" s="26" t="s">
         <v>247</v>
@@ -3808,7 +3509,7 @@
       <c r="AA84" s="16"/>
       <c r="AB84" s="16"/>
     </row>
-    <row r="85" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="85">
       <c r="A85" s="16" t="s">
         <v>159</v>
       </c>
@@ -3825,10 +3526,10 @@
         <v>246</v>
       </c>
       <c r="F85" s="24">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G85" s="38">
-        <v>16</v>
+        <v>16.0</v>
       </c>
       <c r="H85" s="26" t="s">
         <v>162</v>
@@ -3854,29 +3555,26 @@
       <c r="AA85" s="16"/>
       <c r="AB85" s="16"/>
     </row>
-    <row r="87" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="87">
       <c r="A87" s="2" t="s">
         <v>248</v>
       </c>
       <c r="F87" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="88">
       <c r="A88" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="C88" s="58" t="s">
-        <v>316</v>
-      </c>
       <c r="E88" s="2" t="s">
         <v>250</v>
       </c>
       <c r="F88" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="89">
       <c r="A89" s="2" t="s">
         <v>251</v>
       </c>
@@ -3884,10 +3582,10 @@
         <v>250</v>
       </c>
       <c r="F89" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:28" ht="12.6" x14ac:dyDescent="0.45">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="90">
       <c r="A90" s="48" t="s">
         <v>252</v>
       </c>
@@ -3930,7 +3628,7 @@
       <c r="AA90" s="49"/>
       <c r="AB90" s="49"/>
     </row>
-    <row r="91" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="91">
       <c r="A91" s="22" t="s">
         <v>255</v>
       </c>
@@ -3941,16 +3639,16 @@
         <v>201</v>
       </c>
       <c r="F91" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G91" s="23">
-        <v>17</v>
+        <v>17.0</v>
       </c>
       <c r="H91" s="10" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="92" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="92">
       <c r="A92" s="22" t="s">
         <v>257</v>
       </c>
@@ -3961,16 +3659,16 @@
         <v>201</v>
       </c>
       <c r="F92" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G92" s="23">
-        <v>17</v>
+        <v>17.0</v>
       </c>
       <c r="H92" s="10" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="94" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="94">
       <c r="A94" s="32"/>
       <c r="B94" s="32"/>
       <c r="C94" s="32"/>
@@ -4000,13 +3698,13 @@
       <c r="AA94" s="32"/>
       <c r="AB94" s="32"/>
     </row>
-    <row r="95" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="95">
       <c r="A95" s="4" t="s">
         <v>259</v>
       </c>
       <c r="D95" s="13"/>
     </row>
-    <row r="96" spans="1:28" ht="12.6" x14ac:dyDescent="0.45">
+    <row r="96">
       <c r="A96" s="14" t="s">
         <v>19</v>
       </c>
@@ -4049,7 +3747,7 @@
       <c r="AA96" s="16"/>
       <c r="AB96" s="16"/>
     </row>
-    <row r="97" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="97">
       <c r="A97" s="16" t="s">
         <v>260</v>
       </c>
@@ -4061,7 +3759,7 @@
       </c>
       <c r="E97" s="16"/>
       <c r="F97" s="22">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G97" s="31">
         <v>1.06</v>
@@ -4070,7 +3768,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="98" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="98">
       <c r="A98" s="16" t="s">
         <v>263</v>
       </c>
@@ -4082,7 +3780,7 @@
       </c>
       <c r="E98" s="16"/>
       <c r="F98" s="22">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G98" s="31">
         <v>5.31</v>
@@ -4091,7 +3789,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="99" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="99">
       <c r="A99" s="51" t="s">
         <v>266</v>
       </c>
@@ -4102,7 +3800,7 @@
         <v>124</v>
       </c>
       <c r="F99" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G99" s="31">
         <v>0.32</v>
@@ -4111,7 +3809,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="100" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="100">
       <c r="A100" s="16" t="s">
         <v>267</v>
       </c>
@@ -4122,7 +3820,7 @@
         <v>124</v>
       </c>
       <c r="F100" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G100" s="31">
         <v>0.12</v>
@@ -4131,7 +3829,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="101" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="101">
       <c r="A101" s="2" t="s">
         <v>270</v>
       </c>
@@ -4139,16 +3837,16 @@
         <v>119</v>
       </c>
       <c r="F101" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G101" s="23">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="H101" s="10" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="102" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="102">
       <c r="A102" s="2" t="s">
         <v>272</v>
       </c>
@@ -4156,16 +3854,16 @@
         <v>119</v>
       </c>
       <c r="F102" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G102" s="23">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="H102" s="10" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="103" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="103">
       <c r="A103" s="16" t="s">
         <v>274</v>
       </c>
@@ -4178,16 +3876,16 @@
       </c>
       <c r="E103" s="27"/>
       <c r="F103" s="24">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G103" s="38">
-        <v>25</v>
+        <v>25.0</v>
       </c>
       <c r="H103" s="26" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="104" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="104">
       <c r="A104" s="16" t="s">
         <v>277</v>
       </c>
@@ -4200,10 +3898,10 @@
       </c>
       <c r="E104" s="25"/>
       <c r="F104" s="24">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G104" s="38">
-        <v>25</v>
+        <v>25.0</v>
       </c>
       <c r="H104" s="26" t="s">
         <v>278</v>
@@ -4229,7 +3927,7 @@
       <c r="AA104" s="16"/>
       <c r="AB104" s="16"/>
     </row>
-    <row r="105" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="105">
       <c r="A105" s="16" t="s">
         <v>279</v>
       </c>
@@ -4242,10 +3940,10 @@
       </c>
       <c r="E105" s="25"/>
       <c r="F105" s="24">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G105" s="38">
-        <v>25</v>
+        <v>25.0</v>
       </c>
       <c r="H105" s="26" t="s">
         <v>280</v>
@@ -4271,7 +3969,7 @@
       <c r="AA105" s="16"/>
       <c r="AB105" s="16"/>
     </row>
-    <row r="106" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="106">
       <c r="A106" s="2" t="s">
         <v>281</v>
       </c>
@@ -4282,16 +3980,16 @@
         <v>282</v>
       </c>
       <c r="F106" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G106" s="23">
-        <v>13</v>
+        <v>13.0</v>
       </c>
       <c r="H106" s="10" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="107" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="107">
       <c r="A107" s="2" t="s">
         <v>284</v>
       </c>
@@ -4302,7 +4000,7 @@
         <v>285</v>
       </c>
       <c r="F107" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G107" s="36">
         <v>43.95</v>
@@ -4311,7 +4009,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="108" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="108">
       <c r="A108" s="2" t="s">
         <v>287</v>
       </c>
@@ -4322,16 +4020,16 @@
         <v>288</v>
       </c>
       <c r="F108" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G108" s="23">
-        <v>15</v>
+        <v>15.0</v>
       </c>
       <c r="H108" s="10" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="109" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="109">
       <c r="A109" s="2" t="s">
         <v>290</v>
       </c>
@@ -4342,16 +4040,16 @@
         <v>288</v>
       </c>
       <c r="F109" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G109" s="23">
-        <v>17</v>
+        <v>17.0</v>
       </c>
       <c r="H109" s="10" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="110" spans="1:28" ht="12.6" x14ac:dyDescent="0.45">
+    <row r="110">
       <c r="A110" s="52" t="s">
         <v>293</v>
       </c>
@@ -4364,10 +4062,10 @@
         <v>294</v>
       </c>
       <c r="F110" s="48">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G110" s="54">
-        <v>80</v>
+        <v>80.0</v>
       </c>
       <c r="H110" s="55" t="s">
         <v>295</v>
@@ -4393,10 +4091,10 @@
       <c r="AA110" s="49"/>
       <c r="AB110" s="49"/>
     </row>
-    <row r="111" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="111">
       <c r="A111" s="2"/>
     </row>
-    <row r="112" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="112">
       <c r="A112" s="32"/>
       <c r="B112" s="32"/>
       <c r="C112" s="32"/>
@@ -4426,13 +4124,13 @@
       <c r="AA112" s="32"/>
       <c r="AB112" s="32"/>
     </row>
-    <row r="113" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="113">
       <c r="A113" s="4" t="s">
         <v>296</v>
       </c>
       <c r="D113" s="13"/>
     </row>
-    <row r="114" spans="1:28" ht="12.6" x14ac:dyDescent="0.45">
+    <row r="114">
       <c r="A114" s="14" t="s">
         <v>19</v>
       </c>
@@ -4476,7 +4174,7 @@
       <c r="AA114" s="16"/>
       <c r="AB114" s="16"/>
     </row>
-    <row r="115" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="115">
       <c r="A115" s="2" t="s">
         <v>297</v>
       </c>
@@ -4487,16 +4185,16 @@
         <v>298</v>
       </c>
       <c r="F115" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G115" s="23">
-        <v>5</v>
+        <v>5.0</v>
       </c>
       <c r="H115" s="10" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="116" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="116">
       <c r="A116" s="2" t="s">
         <v>300</v>
       </c>
@@ -4510,7 +4208,7 @@
         <v>302</v>
       </c>
       <c r="F116" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G116" s="36">
         <v>0.6</v>
@@ -4519,7 +4217,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="117" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="117">
       <c r="A117" s="27" t="s">
         <v>304</v>
       </c>
@@ -4533,7 +4231,7 @@
         <v>306</v>
       </c>
       <c r="F117" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G117" s="36">
         <v>0.1</v>
@@ -4542,7 +4240,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="118" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="118">
       <c r="A118" s="27" t="s">
         <v>308</v>
       </c>
@@ -4553,7 +4251,7 @@
         <v>124</v>
       </c>
       <c r="F118" s="2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G118" s="36">
         <v>0.36</v>
@@ -4562,7 +4260,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="119" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="119">
       <c r="A119" s="27" t="s">
         <v>311</v>
       </c>
@@ -4579,10 +4277,10 @@
         <v>313</v>
       </c>
       <c r="F119" s="24">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G119" s="38">
-        <v>25</v>
+        <v>25.0</v>
       </c>
       <c r="H119" s="57" t="s">
         <v>314</v>
@@ -4608,7 +4306,7 @@
       <c r="AA119" s="16"/>
       <c r="AB119" s="16"/>
     </row>
-    <row r="120" spans="1:28" ht="12.6" x14ac:dyDescent="0.45">
+    <row r="120">
       <c r="A120" s="53" t="s">
         <v>274</v>
       </c>
@@ -4652,7 +4350,7 @@
       <c r="AA120" s="49"/>
       <c r="AB120" s="49"/>
     </row>
-    <row r="121" spans="1:28" ht="12.6" x14ac:dyDescent="0.45">
+    <row r="121">
       <c r="A121" s="53" t="s">
         <v>277</v>
       </c>
@@ -4675,7 +4373,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="122" spans="1:28" ht="12.6" x14ac:dyDescent="0.45">
+    <row r="122">
       <c r="A122" s="53" t="s">
         <v>279</v>
       </c>
@@ -4698,7 +4396,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="123" spans="1:28" ht="12.6" x14ac:dyDescent="0.45">
+    <row r="123">
       <c r="A123" s="48" t="s">
         <v>252</v>
       </c>
@@ -4741,7 +4439,7 @@
       <c r="AA123" s="49"/>
       <c r="AB123" s="49"/>
     </row>
-    <row r="126" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="126">
       <c r="A126" s="32"/>
       <c r="B126" s="32"/>
       <c r="C126" s="32"/>
@@ -4773,109 +4471,108 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H7" r:id="rId1"/>
-    <hyperlink ref="H8" r:id="rId2"/>
-    <hyperlink ref="H9" r:id="rId3"/>
-    <hyperlink ref="H10" r:id="rId4"/>
-    <hyperlink ref="H11" r:id="rId5"/>
-    <hyperlink ref="H12" r:id="rId6"/>
-    <hyperlink ref="H13" r:id="rId7"/>
-    <hyperlink ref="H15" r:id="rId8"/>
-    <hyperlink ref="H16" r:id="rId9"/>
-    <hyperlink ref="H17" r:id="rId10"/>
-    <hyperlink ref="H23" r:id="rId11"/>
-    <hyperlink ref="H24" r:id="rId12"/>
-    <hyperlink ref="H25" r:id="rId13"/>
-    <hyperlink ref="H26" r:id="rId14"/>
-    <hyperlink ref="H27" r:id="rId15"/>
-    <hyperlink ref="H28" r:id="rId16"/>
-    <hyperlink ref="H29" r:id="rId17"/>
-    <hyperlink ref="H31" r:id="rId18"/>
-    <hyperlink ref="H32" r:id="rId19"/>
-    <hyperlink ref="H33" r:id="rId20"/>
-    <hyperlink ref="H34" r:id="rId21"/>
-    <hyperlink ref="H35" r:id="rId22"/>
-    <hyperlink ref="H36" r:id="rId23"/>
-    <hyperlink ref="H37" r:id="rId24"/>
-    <hyperlink ref="H38" r:id="rId25"/>
-    <hyperlink ref="H39" r:id="rId26"/>
-    <hyperlink ref="H40" r:id="rId27"/>
-    <hyperlink ref="H41" r:id="rId28"/>
-    <hyperlink ref="H46" r:id="rId29"/>
-    <hyperlink ref="H47" r:id="rId30"/>
-    <hyperlink ref="H48" r:id="rId31"/>
-    <hyperlink ref="H49" r:id="rId32"/>
-    <hyperlink ref="H50" r:id="rId33"/>
-    <hyperlink ref="H52" r:id="rId34"/>
-    <hyperlink ref="H53" r:id="rId35"/>
-    <hyperlink ref="H59" r:id="rId36"/>
-    <hyperlink ref="H60" r:id="rId37"/>
-    <hyperlink ref="H61" r:id="rId38"/>
-    <hyperlink ref="H62" r:id="rId39"/>
-    <hyperlink ref="H63" r:id="rId40"/>
-    <hyperlink ref="H70" r:id="rId41"/>
-    <hyperlink ref="H71" r:id="rId42"/>
-    <hyperlink ref="H72" r:id="rId43"/>
-    <hyperlink ref="H73" r:id="rId44"/>
-    <hyperlink ref="H74" r:id="rId45"/>
-    <hyperlink ref="H75" r:id="rId46"/>
-    <hyperlink ref="H76" r:id="rId47"/>
-    <hyperlink ref="H77" r:id="rId48"/>
-    <hyperlink ref="H78" r:id="rId49"/>
-    <hyperlink ref="H79" r:id="rId50"/>
-    <hyperlink ref="H80" r:id="rId51"/>
-    <hyperlink ref="H81" r:id="rId52"/>
-    <hyperlink ref="H82" r:id="rId53"/>
-    <hyperlink ref="H84" r:id="rId54"/>
-    <hyperlink ref="H85" r:id="rId55"/>
-    <hyperlink ref="H91" r:id="rId56"/>
-    <hyperlink ref="H92" r:id="rId57"/>
-    <hyperlink ref="H97" r:id="rId58"/>
-    <hyperlink ref="H98" r:id="rId59"/>
-    <hyperlink ref="H99" r:id="rId60"/>
-    <hyperlink ref="H100" r:id="rId61"/>
-    <hyperlink ref="H101" r:id="rId62"/>
-    <hyperlink ref="H102" r:id="rId63"/>
-    <hyperlink ref="H103" r:id="rId64"/>
-    <hyperlink ref="H104" r:id="rId65"/>
-    <hyperlink ref="H105" r:id="rId66"/>
-    <hyperlink ref="H106" r:id="rId67"/>
-    <hyperlink ref="H107" r:id="rId68" location="product-description-iframe"/>
-    <hyperlink ref="H108" r:id="rId69"/>
-    <hyperlink ref="H109" r:id="rId70"/>
-    <hyperlink ref="H110" r:id="rId71"/>
-    <hyperlink ref="H115" r:id="rId72"/>
-    <hyperlink ref="H116" r:id="rId73"/>
-    <hyperlink ref="H117" r:id="rId74"/>
-    <hyperlink ref="H118" r:id="rId75"/>
-    <hyperlink ref="H119" r:id="rId76"/>
+    <hyperlink r:id="rId1" ref="H7"/>
+    <hyperlink r:id="rId2" ref="H8"/>
+    <hyperlink r:id="rId3" ref="H9"/>
+    <hyperlink r:id="rId4" ref="H10"/>
+    <hyperlink r:id="rId5" ref="H11"/>
+    <hyperlink r:id="rId6" ref="H12"/>
+    <hyperlink r:id="rId7" ref="H13"/>
+    <hyperlink r:id="rId8" ref="H15"/>
+    <hyperlink r:id="rId9" ref="H16"/>
+    <hyperlink r:id="rId10" ref="H17"/>
+    <hyperlink r:id="rId11" ref="H23"/>
+    <hyperlink r:id="rId12" ref="H24"/>
+    <hyperlink r:id="rId13" ref="H25"/>
+    <hyperlink r:id="rId14" ref="H26"/>
+    <hyperlink r:id="rId15" ref="H27"/>
+    <hyperlink r:id="rId16" ref="H28"/>
+    <hyperlink r:id="rId17" ref="H29"/>
+    <hyperlink r:id="rId18" ref="H31"/>
+    <hyperlink r:id="rId19" ref="H32"/>
+    <hyperlink r:id="rId20" ref="H33"/>
+    <hyperlink r:id="rId21" ref="H34"/>
+    <hyperlink r:id="rId22" ref="H35"/>
+    <hyperlink r:id="rId23" ref="H36"/>
+    <hyperlink r:id="rId24" ref="H37"/>
+    <hyperlink r:id="rId25" ref="H38"/>
+    <hyperlink r:id="rId26" ref="H39"/>
+    <hyperlink r:id="rId27" ref="H40"/>
+    <hyperlink r:id="rId28" ref="H41"/>
+    <hyperlink r:id="rId29" ref="H46"/>
+    <hyperlink r:id="rId30" ref="H47"/>
+    <hyperlink r:id="rId31" ref="H48"/>
+    <hyperlink r:id="rId32" ref="H49"/>
+    <hyperlink r:id="rId33" ref="H50"/>
+    <hyperlink r:id="rId34" ref="H52"/>
+    <hyperlink r:id="rId35" ref="H53"/>
+    <hyperlink r:id="rId36" ref="H59"/>
+    <hyperlink r:id="rId37" ref="H60"/>
+    <hyperlink r:id="rId38" ref="H61"/>
+    <hyperlink r:id="rId39" ref="H62"/>
+    <hyperlink r:id="rId40" ref="H63"/>
+    <hyperlink r:id="rId41" ref="H70"/>
+    <hyperlink r:id="rId42" ref="H71"/>
+    <hyperlink r:id="rId43" ref="H72"/>
+    <hyperlink r:id="rId44" ref="H73"/>
+    <hyperlink r:id="rId45" ref="H74"/>
+    <hyperlink r:id="rId46" ref="H75"/>
+    <hyperlink r:id="rId47" ref="H76"/>
+    <hyperlink r:id="rId48" ref="H77"/>
+    <hyperlink r:id="rId49" ref="H78"/>
+    <hyperlink r:id="rId50" ref="H79"/>
+    <hyperlink r:id="rId51" ref="H80"/>
+    <hyperlink r:id="rId52" ref="H81"/>
+    <hyperlink r:id="rId53" ref="H82"/>
+    <hyperlink r:id="rId54" ref="H84"/>
+    <hyperlink r:id="rId55" ref="H85"/>
+    <hyperlink r:id="rId56" ref="H91"/>
+    <hyperlink r:id="rId57" ref="H92"/>
+    <hyperlink r:id="rId58" ref="H97"/>
+    <hyperlink r:id="rId59" ref="H98"/>
+    <hyperlink r:id="rId60" ref="H99"/>
+    <hyperlink r:id="rId61" ref="H100"/>
+    <hyperlink r:id="rId62" ref="H101"/>
+    <hyperlink r:id="rId63" ref="H102"/>
+    <hyperlink r:id="rId64" ref="H103"/>
+    <hyperlink r:id="rId65" ref="H104"/>
+    <hyperlink r:id="rId66" ref="H105"/>
+    <hyperlink r:id="rId67" ref="H106"/>
+    <hyperlink r:id="rId68" location="product-description-iframe" ref="H107"/>
+    <hyperlink r:id="rId69" ref="H108"/>
+    <hyperlink r:id="rId70" ref="H109"/>
+    <hyperlink r:id="rId71" ref="H110"/>
+    <hyperlink r:id="rId72" ref="H115"/>
+    <hyperlink r:id="rId73" ref="H116"/>
+    <hyperlink r:id="rId74" ref="H117"/>
+    <hyperlink r:id="rId75" ref="H118"/>
+    <hyperlink r:id="rId76" ref="H119"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId77"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="4" max="4" width="21.83203125" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" customWidth="1"/>
-    <col min="7" max="7" width="64.83203125" customWidth="1"/>
+    <col customWidth="1" min="4" max="4" width="21.86"/>
+    <col customWidth="1" min="6" max="6" width="18.57"/>
+    <col customWidth="1" min="7" max="7" width="64.86"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -4883,17 +4580,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -4907,7 +4604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -4918,7 +4615,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -4935,7 +4632,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -4949,7 +4646,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -4966,7 +4663,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13">
       <c r="D13" s="10" t="s">
         <v>32</v>
       </c>
@@ -4974,7 +4671,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14">
       <c r="D14" s="10" t="s">
         <v>35</v>
       </c>
@@ -4982,7 +4679,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15">
       <c r="D15" s="10" t="s">
         <v>38</v>
       </c>
@@ -4990,11 +4687,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16">
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17">
       <c r="D17" s="10" t="s">
         <v>42</v>
       </c>
@@ -5002,17 +4699,17 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18">
       <c r="E18" s="22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19">
       <c r="E19" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20">
       <c r="A20" s="2" t="s">
         <v>48</v>
       </c>
@@ -5026,17 +4723,17 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24">
       <c r="A24" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="27">
       <c r="A27" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="28">
       <c r="A28" s="16" t="s">
         <v>55</v>
       </c>
@@ -5047,10 +4744,10 @@
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
       <c r="F28" s="24">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G28" s="24">
-        <v>16</v>
+        <v>16.0</v>
       </c>
       <c r="H28" s="26" t="s">
         <v>66</v>
@@ -5076,7 +4773,7 @@
       <c r="AA28" s="16"/>
       <c r="AB28" s="16"/>
     </row>
-    <row r="29" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="29">
       <c r="A29" s="16" t="s">
         <v>70</v>
       </c>
@@ -5087,10 +4784,10 @@
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
       <c r="F29" s="24">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="G29" s="24">
-        <v>16</v>
+        <v>16.0</v>
       </c>
       <c r="H29" s="26" t="s">
         <v>71</v>
@@ -5116,7 +4813,7 @@
       <c r="AA29" s="16"/>
       <c r="AB29" s="16"/>
     </row>
-    <row r="30" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="30">
       <c r="A30" s="25" t="s">
         <v>73</v>
       </c>
@@ -5129,7 +4826,7 @@
         <v>75</v>
       </c>
       <c r="F30" s="24">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="G30" s="31">
         <v>0.5</v>
@@ -5158,7 +4855,7 @@
       <c r="AA30" s="16"/>
       <c r="AB30" s="16"/>
     </row>
-    <row r="31" spans="1:28" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="31">
       <c r="A31" s="25" t="s">
         <v>78</v>
       </c>
@@ -5169,7 +4866,7 @@
       </c>
       <c r="E31" s="16"/>
       <c r="F31" s="24">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="G31" s="31">
         <v>1.5</v>
@@ -5200,22 +4897,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D7" r:id="rId1"/>
-    <hyperlink ref="D8" r:id="rId2"/>
-    <hyperlink ref="D9" r:id="rId3"/>
-    <hyperlink ref="G9" r:id="rId4"/>
-    <hyperlink ref="D10" r:id="rId5"/>
-    <hyperlink ref="D11" r:id="rId6"/>
-    <hyperlink ref="D13" r:id="rId7"/>
-    <hyperlink ref="D14" r:id="rId8"/>
-    <hyperlink ref="D15" r:id="rId9"/>
-    <hyperlink ref="D17" r:id="rId10"/>
-    <hyperlink ref="D20" r:id="rId11"/>
-    <hyperlink ref="H28" r:id="rId12"/>
-    <hyperlink ref="H29" r:id="rId13"/>
-    <hyperlink ref="H30" r:id="rId14"/>
-    <hyperlink ref="H31" r:id="rId15"/>
+    <hyperlink r:id="rId1" ref="D7"/>
+    <hyperlink r:id="rId2" ref="D8"/>
+    <hyperlink r:id="rId3" ref="D9"/>
+    <hyperlink r:id="rId4" ref="G9"/>
+    <hyperlink r:id="rId5" ref="D10"/>
+    <hyperlink r:id="rId6" ref="D11"/>
+    <hyperlink r:id="rId7" ref="D13"/>
+    <hyperlink r:id="rId8" ref="D14"/>
+    <hyperlink r:id="rId9" ref="D15"/>
+    <hyperlink r:id="rId10" ref="D17"/>
+    <hyperlink r:id="rId11" ref="D20"/>
+    <hyperlink r:id="rId12" ref="H28"/>
+    <hyperlink r:id="rId13" ref="H29"/>
+    <hyperlink r:id="rId14" ref="H30"/>
+    <hyperlink r:id="rId15" ref="H31"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
parts list diode update
</commit_message>
<xml_diff>
--- a/hardware/SeeBoat_fullPartsList.xlsx
+++ b/hardware/SeeBoat_fullPartsList.xlsx
@@ -536,10 +536,10 @@
     <t xml:space="preserve">diode</t>
   </si>
   <si>
-    <t xml:space="preserve">S1BBFDICTND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/product-detail/en/diodes-incorporated/S1GB-13-F/S1GB-FDICT-ND/815935</t>
+    <t xml:space="preserve">641-1331-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/products/en?keywords=641-1331-1-ND</t>
   </si>
   <si>
     <t xml:space="preserve">rail splitter</t>
@@ -990,7 +990,7 @@
     <numFmt numFmtId="166" formatCode="\$#,##0"/>
     <numFmt numFmtId="167" formatCode="\$#,##0.00"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1090,6 +1090,21 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1264,7 +1279,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1401,47 +1416,55 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1449,11 +1472,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1465,7 +1488,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1560,13 +1583,13 @@
   </sheetPr>
   <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A86" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F111" activeCellId="0" sqref="F111"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C73" activeCellId="0" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="14.43"/>
@@ -3425,7 +3448,7 @@
       <c r="AB71" s="13"/>
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="16" t="s">
+      <c r="A72" s="34" t="s">
         <v>167</v>
       </c>
       <c r="B72" s="13"/>
@@ -3467,10 +3490,10 @@
       <c r="AB72" s="13"/>
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="18" t="s">
+      <c r="A73" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="C73" s="16" t="s">
+      <c r="C73" s="34" t="s">
         <v>171</v>
       </c>
       <c r="D73" s="21" t="s">
@@ -3483,7 +3506,7 @@
       <c r="G73" s="30" t="n">
         <v>0.37</v>
       </c>
-      <c r="H73" s="20" t="s">
+      <c r="H73" s="35" t="s">
         <v>172</v>
       </c>
     </row>
@@ -3505,7 +3528,7 @@
       <c r="G74" s="23" t="n">
         <v>1.86</v>
       </c>
-      <c r="H74" s="34" t="s">
+      <c r="H74" s="36" t="s">
         <v>175</v>
       </c>
       <c r="I74" s="25"/>
@@ -3545,7 +3568,7 @@
       <c r="G75" s="29" t="n">
         <v>2.64</v>
       </c>
-      <c r="H75" s="34" t="s">
+      <c r="H75" s="36" t="s">
         <v>178</v>
       </c>
       <c r="I75" s="25"/>
@@ -3583,7 +3606,7 @@
       <c r="G76" s="23" t="n">
         <v>1.81</v>
       </c>
-      <c r="H76" s="34" t="s">
+      <c r="H76" s="36" t="s">
         <v>180</v>
       </c>
       <c r="I76" s="25"/>
@@ -3803,47 +3826,47 @@
       <c r="H84" s="17"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="35" t="s">
+      <c r="A85" s="37" t="s">
         <v>190</v>
       </c>
-      <c r="C85" s="35" t="s">
+      <c r="C85" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="D85" s="35" t="s">
+      <c r="D85" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="E85" s="35" t="s">
+      <c r="E85" s="37" t="s">
         <v>192</v>
       </c>
-      <c r="F85" s="35" t="s">
+      <c r="F85" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="G85" s="35" t="s">
+      <c r="G85" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="H85" s="35" t="s">
+      <c r="H85" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="I85" s="36"/>
-      <c r="J85" s="36"/>
-      <c r="K85" s="36"/>
-      <c r="L85" s="36"/>
-      <c r="M85" s="36"/>
-      <c r="N85" s="36"/>
-      <c r="O85" s="36"/>
-      <c r="P85" s="36"/>
-      <c r="Q85" s="36"/>
-      <c r="R85" s="36"/>
-      <c r="S85" s="36"/>
-      <c r="T85" s="36"/>
-      <c r="U85" s="36"/>
-      <c r="V85" s="36"/>
-      <c r="W85" s="36"/>
-      <c r="X85" s="36"/>
-      <c r="Y85" s="36"/>
-      <c r="Z85" s="36"/>
-      <c r="AA85" s="36"/>
-      <c r="AB85" s="36"/>
+      <c r="I85" s="38"/>
+      <c r="J85" s="38"/>
+      <c r="K85" s="38"/>
+      <c r="L85" s="38"/>
+      <c r="M85" s="38"/>
+      <c r="N85" s="38"/>
+      <c r="O85" s="38"/>
+      <c r="P85" s="38"/>
+      <c r="Q85" s="38"/>
+      <c r="R85" s="38"/>
+      <c r="S85" s="38"/>
+      <c r="T85" s="38"/>
+      <c r="U85" s="38"/>
+      <c r="V85" s="38"/>
+      <c r="W85" s="38"/>
+      <c r="X85" s="38"/>
+      <c r="Y85" s="38"/>
+      <c r="Z85" s="38"/>
+      <c r="AA85" s="38"/>
+      <c r="AB85" s="38"/>
     </row>
     <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="21" t="s">
@@ -3971,7 +3994,7 @@
         <v>198</v>
       </c>
       <c r="B92" s="17"/>
-      <c r="C92" s="37" t="s">
+      <c r="C92" s="39" t="s">
         <v>199</v>
       </c>
       <c r="D92" s="21" t="s">
@@ -3993,7 +4016,7 @@
         <v>201</v>
       </c>
       <c r="B93" s="17"/>
-      <c r="C93" s="37" t="s">
+      <c r="C93" s="39" t="s">
         <v>202</v>
       </c>
       <c r="D93" s="21" t="s">
@@ -4094,7 +4117,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="16" t="s">
         <v>212</v>
       </c>
@@ -4118,7 +4141,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="16" t="s">
         <v>216</v>
       </c>
@@ -4295,46 +4318,46 @@
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="35" t="s">
+      <c r="A105" s="37" t="s">
         <v>232</v>
       </c>
-      <c r="B105" s="38"/>
-      <c r="C105" s="35"/>
-      <c r="D105" s="35" t="s">
+      <c r="B105" s="40"/>
+      <c r="C105" s="37"/>
+      <c r="D105" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="E105" s="35" t="s">
+      <c r="E105" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="F105" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="G105" s="39" t="n">
+      <c r="F105" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="G105" s="41" t="n">
         <v>80</v>
       </c>
-      <c r="H105" s="40" t="s">
+      <c r="H105" s="42" t="s">
         <v>234</v>
       </c>
-      <c r="I105" s="41"/>
-      <c r="J105" s="42"/>
-      <c r="K105" s="42"/>
-      <c r="L105" s="42"/>
-      <c r="M105" s="42"/>
-      <c r="N105" s="42"/>
-      <c r="O105" s="42"/>
-      <c r="P105" s="42"/>
-      <c r="Q105" s="42"/>
-      <c r="R105" s="42"/>
-      <c r="S105" s="42"/>
-      <c r="T105" s="42"/>
-      <c r="U105" s="42"/>
-      <c r="V105" s="42"/>
-      <c r="W105" s="42"/>
-      <c r="X105" s="42"/>
-      <c r="Y105" s="42"/>
-      <c r="Z105" s="36"/>
-      <c r="AA105" s="36"/>
-      <c r="AB105" s="36"/>
+      <c r="I105" s="43"/>
+      <c r="J105" s="44"/>
+      <c r="K105" s="44"/>
+      <c r="L105" s="44"/>
+      <c r="M105" s="44"/>
+      <c r="N105" s="44"/>
+      <c r="O105" s="44"/>
+      <c r="P105" s="44"/>
+      <c r="Q105" s="44"/>
+      <c r="R105" s="44"/>
+      <c r="S105" s="44"/>
+      <c r="T105" s="44"/>
+      <c r="U105" s="44"/>
+      <c r="V105" s="44"/>
+      <c r="W105" s="44"/>
+      <c r="X105" s="44"/>
+      <c r="Y105" s="44"/>
+      <c r="Z105" s="38"/>
+      <c r="AA105" s="38"/>
+      <c r="AB105" s="38"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="26"/>
@@ -4511,91 +4534,91 @@
         <v>249</v>
       </c>
     </row>
-    <row r="114" s="44" customFormat="true" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="43" t="s">
+    <row r="114" s="46" customFormat="true" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="45" t="s">
         <v>106</v>
       </c>
-      <c r="C114" s="43" t="s">
+      <c r="C114" s="45" t="s">
         <v>250</v>
       </c>
-      <c r="D114" s="43" t="s">
+      <c r="D114" s="45" t="s">
         <v>250</v>
       </c>
-      <c r="E114" s="43" t="s">
+      <c r="E114" s="45" t="s">
         <v>251</v>
       </c>
-      <c r="F114" s="43" t="s">
+      <c r="F114" s="45" t="s">
         <v>250</v>
       </c>
-      <c r="G114" s="43" t="s">
+      <c r="G114" s="45" t="s">
         <v>250</v>
       </c>
-      <c r="H114" s="43" t="s">
+      <c r="H114" s="45" t="s">
         <v>250</v>
       </c>
-      <c r="J114" s="41"/>
-      <c r="K114" s="41"/>
-      <c r="L114" s="41"/>
-      <c r="M114" s="42"/>
-      <c r="N114" s="42"/>
-      <c r="O114" s="42"/>
-      <c r="P114" s="42"/>
-      <c r="Q114" s="42"/>
-      <c r="R114" s="42"/>
-      <c r="S114" s="42"/>
-      <c r="T114" s="42"/>
-      <c r="U114" s="42"/>
-      <c r="V114" s="42"/>
-      <c r="W114" s="42"/>
-      <c r="X114" s="42"/>
-      <c r="Y114" s="42"/>
-      <c r="Z114" s="42"/>
-      <c r="AA114" s="42"/>
-      <c r="AB114" s="42"/>
+      <c r="J114" s="43"/>
+      <c r="K114" s="43"/>
+      <c r="L114" s="43"/>
+      <c r="M114" s="44"/>
+      <c r="N114" s="44"/>
+      <c r="O114" s="44"/>
+      <c r="P114" s="44"/>
+      <c r="Q114" s="44"/>
+      <c r="R114" s="44"/>
+      <c r="S114" s="44"/>
+      <c r="T114" s="44"/>
+      <c r="U114" s="44"/>
+      <c r="V114" s="44"/>
+      <c r="W114" s="44"/>
+      <c r="X114" s="44"/>
+      <c r="Y114" s="44"/>
+      <c r="Z114" s="44"/>
+      <c r="AA114" s="44"/>
+      <c r="AB114" s="44"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="35" t="s">
+      <c r="A115" s="37" t="s">
         <v>190</v>
       </c>
       <c r="B115" s="17"/>
-      <c r="C115" s="35" t="s">
+      <c r="C115" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="D115" s="35" t="s">
+      <c r="D115" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="E115" s="35" t="s">
+      <c r="E115" s="37" t="s">
         <v>252</v>
       </c>
-      <c r="F115" s="35" t="s">
+      <c r="F115" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="G115" s="35" t="s">
+      <c r="G115" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="H115" s="35" t="s">
+      <c r="H115" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="I115" s="36"/>
-      <c r="J115" s="36"/>
-      <c r="K115" s="36"/>
-      <c r="L115" s="36"/>
-      <c r="M115" s="36"/>
-      <c r="N115" s="36"/>
-      <c r="O115" s="36"/>
-      <c r="P115" s="36"/>
-      <c r="Q115" s="36"/>
-      <c r="R115" s="36"/>
-      <c r="S115" s="36"/>
-      <c r="T115" s="36"/>
-      <c r="U115" s="36"/>
-      <c r="V115" s="36"/>
-      <c r="W115" s="36"/>
-      <c r="X115" s="36"/>
-      <c r="Y115" s="36"/>
-      <c r="Z115" s="36"/>
-      <c r="AA115" s="36"/>
-      <c r="AB115" s="36"/>
+      <c r="I115" s="38"/>
+      <c r="J115" s="38"/>
+      <c r="K115" s="38"/>
+      <c r="L115" s="38"/>
+      <c r="M115" s="38"/>
+      <c r="N115" s="38"/>
+      <c r="O115" s="38"/>
+      <c r="P115" s="38"/>
+      <c r="Q115" s="38"/>
+      <c r="R115" s="38"/>
+      <c r="S115" s="38"/>
+      <c r="T115" s="38"/>
+      <c r="U115" s="38"/>
+      <c r="V115" s="38"/>
+      <c r="W115" s="38"/>
+      <c r="X115" s="38"/>
+      <c r="Y115" s="38"/>
+      <c r="Z115" s="38"/>
+      <c r="AA115" s="38"/>
+      <c r="AB115" s="38"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="27"/>
@@ -4674,7 +4697,7 @@
     <hyperlink ref="H70" r:id="rId40" display="https://www.digikey.com/product-detail/en/yageo/RT0603BRD0742K2L/YAG4556CT-ND/6616712"/>
     <hyperlink ref="H71" r:id="rId41" display="https://www.digikey.com/product-detail/en/yageo/RT0603DRE071K2L/311-2461-1-ND/6128880"/>
     <hyperlink ref="H72" r:id="rId42" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X8R1H104K080AB/445-8818-1-ND/3248223"/>
-    <hyperlink ref="H73" r:id="rId43" display="https://www.digikey.com/product-detail/en/diodes-incorporated/S1GB-13-F/S1GB-FDICT-ND/815935"/>
+    <hyperlink ref="H73" r:id="rId43" display="https://www.digikey.com/products/en?keywords=641-1331-1-ND"/>
     <hyperlink ref="H74" r:id="rId44" display="https://www.digikey.com/product-detail/en/texas-instruments/TLE2426CD/296-6547-5-ND/371934"/>
     <hyperlink ref="H75" r:id="rId45" display="https://www.digikey.com/product-detail/en/analog-devices-inc/AD8655ARZ-REEL7/AD8655ARZ-REEL7CT-ND/3678589"/>
     <hyperlink ref="H76" r:id="rId46" display="https://www.digikey.com/product-detail/en/texas-instruments/TLV2374IDR/296-11967-1-ND/390435"/>
@@ -4742,7 +4765,7 @@
       <c r="A3" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="47" t="s">
         <v>255</v>
       </c>
     </row>
@@ -4760,7 +4783,7 @@
       <c r="A7" s="26" t="s">
         <v>258</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="48" t="s">
         <v>259</v>
       </c>
       <c r="E7" s="26" t="s">
@@ -4774,7 +4797,7 @@
       <c r="A8" s="26" t="s">
         <v>262</v>
       </c>
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="48" t="s">
         <v>263</v>
       </c>
       <c r="E8" s="26" t="s">
@@ -4785,7 +4808,7 @@
       <c r="A9" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="48" t="s">
         <v>266</v>
       </c>
       <c r="E9" s="26" t="s">
@@ -4794,7 +4817,7 @@
       <c r="F9" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="G9" s="47" t="s">
+      <c r="G9" s="49" t="s">
         <v>126</v>
       </c>
     </row>
@@ -4802,7 +4825,7 @@
       <c r="A10" s="26" t="s">
         <v>268</v>
       </c>
-      <c r="D10" s="46" t="s">
+      <c r="D10" s="48" t="s">
         <v>269</v>
       </c>
       <c r="E10" s="26" t="s">
@@ -4816,7 +4839,7 @@
       <c r="A11" s="26" t="s">
         <v>272</v>
       </c>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="48" t="s">
         <v>273</v>
       </c>
       <c r="E11" s="26" t="s">
@@ -4830,7 +4853,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="48" t="s">
         <v>276</v>
       </c>
       <c r="E13" s="26" t="s">
@@ -4838,7 +4861,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="46" t="s">
+      <c r="D14" s="48" t="s">
         <v>278</v>
       </c>
       <c r="E14" s="26" t="s">
@@ -4846,7 +4869,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="46" t="s">
+      <c r="D15" s="48" t="s">
         <v>280</v>
       </c>
       <c r="E15" s="26" t="s">
@@ -4858,7 +4881,7 @@
       <c r="E16" s="26"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="48" t="s">
         <v>282</v>
       </c>
       <c r="E17" s="26" t="s">
@@ -4866,7 +4889,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E18" s="48" t="s">
+      <c r="E18" s="50" t="s">
         <v>284</v>
       </c>
     </row>
@@ -4879,10 +4902,10 @@
       <c r="A20" s="26" t="s">
         <v>286</v>
       </c>
-      <c r="D20" s="46" t="s">
+      <c r="D20" s="48" t="s">
         <v>287</v>
       </c>
-      <c r="E20" s="48" t="s">
+      <c r="E20" s="50" t="s">
         <v>288</v>
       </c>
       <c r="F20" s="26" t="s">
@@ -4909,13 +4932,13 @@
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
-      <c r="F28" s="49" t="n">
-        <v>1</v>
-      </c>
-      <c r="G28" s="49" t="n">
+      <c r="F28" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="G28" s="51" t="n">
         <v>16</v>
       </c>
-      <c r="H28" s="50" t="s">
+      <c r="H28" s="52" t="s">
         <v>293</v>
       </c>
       <c r="I28" s="25"/>
@@ -4949,13 +4972,13 @@
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
-      <c r="F29" s="49" t="n">
-        <v>1</v>
-      </c>
-      <c r="G29" s="49" t="n">
+      <c r="F29" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="51" t="n">
         <v>16</v>
       </c>
-      <c r="H29" s="50" t="s">
+      <c r="H29" s="52" t="s">
         <v>295</v>
       </c>
       <c r="I29" s="25"/>
@@ -4991,13 +5014,13 @@
       <c r="E30" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F30" s="49" t="n">
+      <c r="F30" s="51" t="n">
         <v>4</v>
       </c>
-      <c r="G30" s="51" t="n">
+      <c r="G30" s="53" t="n">
         <v>0.5</v>
       </c>
-      <c r="H30" s="50" t="s">
+      <c r="H30" s="52" t="s">
         <v>297</v>
       </c>
       <c r="I30" s="25"/>
@@ -5031,13 +5054,13 @@
         <v>45</v>
       </c>
       <c r="E31" s="13"/>
-      <c r="F31" s="49" t="n">
+      <c r="F31" s="51" t="n">
         <v>4</v>
       </c>
-      <c r="G31" s="51" t="n">
+      <c r="G31" s="53" t="n">
         <v>1.5</v>
       </c>
-      <c r="H31" s="50" t="s">
+      <c r="H31" s="52" t="s">
         <v>299</v>
       </c>
       <c r="I31" s="25"/>
@@ -5073,13 +5096,13 @@
       <c r="E35" s="13" t="s">
         <v>301</v>
       </c>
-      <c r="F35" s="49" t="n">
-        <v>1</v>
-      </c>
-      <c r="G35" s="52" t="n">
+      <c r="F35" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" s="54" t="n">
         <v>31</v>
       </c>
-      <c r="H35" s="50" t="s">
+      <c r="H35" s="52" t="s">
         <v>302</v>
       </c>
       <c r="J35" s="25"/>
@@ -5115,10 +5138,10 @@
       <c r="F36" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="G36" s="53" t="n">
+      <c r="G36" s="55" t="n">
         <v>8</v>
       </c>
-      <c r="H36" s="46" t="s">
+      <c r="H36" s="48" t="s">
         <v>306</v>
       </c>
     </row>
@@ -5135,10 +5158,10 @@
       <c r="F37" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="G37" s="53" t="n">
+      <c r="G37" s="55" t="n">
         <v>27</v>
       </c>
-      <c r="H37" s="46" t="s">
+      <c r="H37" s="48" t="s">
         <v>309</v>
       </c>
     </row>
@@ -5155,10 +5178,10 @@
       <c r="F38" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="G38" s="53" t="n">
+      <c r="G38" s="55" t="n">
         <v>25</v>
       </c>
-      <c r="H38" s="46" t="s">
+      <c r="H38" s="48" t="s">
         <v>312</v>
       </c>
     </row>
@@ -5175,7 +5198,7 @@
       <c r="F39" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="G39" s="53" t="n">
+      <c r="G39" s="55" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5192,10 +5215,10 @@
       <c r="F40" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="G40" s="53" t="n">
+      <c r="G40" s="55" t="n">
         <v>10</v>
       </c>
-      <c r="H40" s="46" t="s">
+      <c r="H40" s="48" t="s">
         <v>318</v>
       </c>
     </row>

</xml_diff>

<commit_message>
parts list and boards update
</commit_message>
<xml_diff>
--- a/hardware/SeeBoat_fullPartsList.xlsx
+++ b/hardware/SeeBoat_fullPartsList.xlsx
@@ -242,7 +242,7 @@
     <t xml:space="preserve">connects to all sensors</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.dropbox.com/sh/u9hnaux5pfnx4as/AADP0RuAMPAJrF8vKR3xcZZMa?dl=0</t>
+    <t xml:space="preserve">https://www.dropbox.com/s/5kwn3nz447jgal9/controlBoard-0.5.brd?dl=0</t>
   </si>
   <si>
     <t xml:space="preserve">resistor SMD 0603 2.7K</t>
@@ -650,13 +650,13 @@
     <t xml:space="preserve">custom light to freq board</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.dropbox.com/sh/39q36secyieys02/AACOiOgjpHFcrkMj71UHTjf1a?dl=0</t>
+    <t xml:space="preserve">https://www.dropbox.com/s/5wtg2gff6oehxno/turbiditySensor.brd?dl=0</t>
   </si>
   <si>
     <t xml:space="preserve">custom LED board</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.dropbox.com/sh/17juos7x65yw1nq/AABGehwJ9LaHe85Q1wV3jjHMa?dl=0</t>
+    <t xml:space="preserve">https://www.dropbox.com/s/f1dnld6ux556wln/turbidityLED.brd?dl=0</t>
   </si>
   <si>
     <t xml:space="preserve">wire-black, stranded</t>
@@ -737,7 +737,7 @@
     <t xml:space="preserve">custom temperature board</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.dropbox.com/sh/mgy3ndqnzldy1xk/AABXH-txk6h3GChvCx_p5i7ma?dl=0</t>
+    <t xml:space="preserve">https://www.dropbox.com/s/a62454o26l9r3ev/temperatureSensor.brd?dl=0</t>
   </si>
   <si>
     <t xml:space="preserve">digital temperature sensor</t>
@@ -1583,8 +1583,8 @@
   </sheetPr>
   <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C73" activeCellId="0" sqref="C73"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2360,7 +2360,7 @@
       <c r="H30" s="16"/>
       <c r="I30" s="17"/>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="16" t="s">
         <v>70</v>
       </c>
@@ -4077,7 +4077,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="16" t="s">
         <v>208</v>
       </c>
@@ -4097,7 +4097,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="16" t="s">
         <v>210</v>
       </c>
@@ -4442,7 +4442,7 @@
       <c r="AA109" s="13"/>
       <c r="AB109" s="13"/>
     </row>
-    <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="16" t="s">
         <v>236</v>
       </c>
@@ -4672,58 +4672,54 @@
     <hyperlink ref="H27" r:id="rId15" display="https://www.adafruit.com/product/2886"/>
     <hyperlink ref="H28" r:id="rId16" display="https://www.amazon.com/gp/product/B00NH13O7K"/>
     <hyperlink ref="H29" r:id="rId17" display="https://www.adafruit.com/product/328"/>
-    <hyperlink ref="H31" r:id="rId18" display="https://www.dropbox.com/sh/u9hnaux5pfnx4as/AADP0RuAMPAJrF8vKR3xcZZMa?dl=0"/>
-    <hyperlink ref="H32" r:id="rId19" display="https://www.digikey.com/products/en?keywords=RNCP0603FTD2K74CT-ND"/>
-    <hyperlink ref="H33" r:id="rId20" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP0603FTD100R/RNCP0603FTD100RCT-ND/2240425"/>
-    <hyperlink ref="H34" r:id="rId21" display="https://www.digikey.com/product-detail/en/AYZ0202AGRLC/401-2013-1-ND/1640122"/>
-    <hyperlink ref="H35" r:id="rId22" display="https://www.adafruit.com/product/2343"/>
-    <hyperlink ref="H36" r:id="rId23" display="https://www.digikey.com/products/en?keywords=WM4802-ND"/>
-    <hyperlink ref="H37" r:id="rId24" display="https://www.digikey.com/products/en?keywords=WM9131-ND"/>
-    <hyperlink ref="H38" r:id="rId25" display="https://www.digikey.com/products/en?keywords=WM4801-ND"/>
-    <hyperlink ref="H39" r:id="rId26" display="https://www.digikey.com/products/en?keywords=WM10647-ND"/>
-    <hyperlink ref="H40" r:id="rId27" display="https://www.digikey.com/product-detail/en/3m/3302-16-300SF/MC16M-100-ND/145737"/>
-    <hyperlink ref="H41" r:id="rId28" display="https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2004A.12.02/C2004W-100-ND/57495"/>
-    <hyperlink ref="H46" r:id="rId29" display="https://www.adafruit.com/product/2240"/>
-    <hyperlink ref="H48" r:id="rId30" display="https://www.tapplastics.com/product/plastics/cut_to_size_plastic/satinice_white/655"/>
-    <hyperlink ref="H54" r:id="rId31" display="https://www.atlas-scientific.com/product_pages/circuits/ezo_ph.html"/>
-    <hyperlink ref="H55" r:id="rId32" display="https://www.atlas-scientific.com/product_pages/probes/ph_probe.html"/>
-    <hyperlink ref="H56" r:id="rId33" display="https://www.atlas-scientific.com/product_pages/components/single_carrier_iso.html"/>
-    <hyperlink ref="H57" r:id="rId34" display="https://www.hach.com/ph-buffer-solution-kit-color-coded-ph-4-01-ph-7-00-and-ph-10-01-500-ml-each/product?id=7640205069"/>
-    <hyperlink ref="H58" r:id="rId35" display="https://www.hach.com/electrolyte-solution-kcl-3m-50ml/product-parameter-reagent?id=7640207762"/>
-    <hyperlink ref="H66" r:id="rId36" display="https://www.digikey.com/product-detail/en/yageo/AT0603FRE0710KL/YAG2122CT-ND/5139570"/>
-    <hyperlink ref="H67" r:id="rId37" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP0603FTD2K74/RNCP0603FTD2K74CT-ND/2240457"/>
-    <hyperlink ref="H68" r:id="rId38" display="https://www.digikey.com/product-detail/en/yageo/RT0603BRD071ML/YAG4498CT-ND/6616654"/>
-    <hyperlink ref="H69" r:id="rId39" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP0603FTD1K00/RNCP0603FTD1K00CT-ND/2240445"/>
-    <hyperlink ref="H70" r:id="rId40" display="https://www.digikey.com/product-detail/en/yageo/RT0603BRD0742K2L/YAG4556CT-ND/6616712"/>
-    <hyperlink ref="H71" r:id="rId41" display="https://www.digikey.com/product-detail/en/yageo/RT0603DRE071K2L/311-2461-1-ND/6128880"/>
-    <hyperlink ref="H72" r:id="rId42" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X8R1H104K080AB/445-8818-1-ND/3248223"/>
-    <hyperlink ref="H73" r:id="rId43" display="https://www.digikey.com/products/en?keywords=641-1331-1-ND"/>
-    <hyperlink ref="H74" r:id="rId44" display="https://www.digikey.com/product-detail/en/texas-instruments/TLE2426CD/296-6547-5-ND/371934"/>
-    <hyperlink ref="H75" r:id="rId45" display="https://www.digikey.com/product-detail/en/analog-devices-inc/AD8655ARZ-REEL7/AD8655ARZ-REEL7CT-ND/3678589"/>
-    <hyperlink ref="H76" r:id="rId46" display="https://www.digikey.com/product-detail/en/texas-instruments/TLV2374IDR/296-11967-1-ND/390435"/>
-    <hyperlink ref="H77" r:id="rId47" display="https://www.digikey.com/product-detail/en/AYZ0202AGRLC/401-2013-1-ND/1640122"/>
-    <hyperlink ref="H79" r:id="rId48" display="https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2117A.12.06/C2117G-100-ND/16217"/>
-    <hyperlink ref="H80" r:id="rId49" display="https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2004A.12.02/C2004W-100-ND/57495"/>
-    <hyperlink ref="H86" r:id="rId50" display="https://www.amazon.com/gp/product/B01F2R2EPE/"/>
-    <hyperlink ref="H87" r:id="rId51" display="https://www.amazon.com/gp/product/B01F7L9QD8/"/>
-    <hyperlink ref="H92" r:id="rId52" display="https://www.digikey.com/product-detail/en/vishay-semiconductor-opto-division/VSMY2850G/VSMY2850GCT-ND/2615293"/>
-    <hyperlink ref="H93" r:id="rId53" display="https://www.digikey.com/product-detail/en/ams/TSL237T/TSL237-TCT-ND/3095287"/>
-    <hyperlink ref="H94" r:id="rId54" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X8R1H104K080AB/445-8818-1-ND/3248223"/>
-    <hyperlink ref="H95" r:id="rId55" display="https://www.digikey.com/product-detail/en/yageo/RT0603DRD07200RL/311-200DCT-ND/1035740"/>
-    <hyperlink ref="H96" r:id="rId56" display="https://www.dropbox.com/sh/39q36secyieys02/AACOiOgjpHFcrkMj71UHTjf1a?dl=0"/>
-    <hyperlink ref="H97" r:id="rId57" display="https://www.dropbox.com/sh/17juos7x65yw1nq/AABGehwJ9LaHe85Q1wV3jjHMa?dl=0"/>
-    <hyperlink ref="H98" r:id="rId58" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-BK005/422010-BK005-ND/3705786"/>
-    <hyperlink ref="H99" r:id="rId59" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-RD005/422010-RD005-ND/4935160"/>
-    <hyperlink ref="H100" r:id="rId60" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-SL005/422010-SL005-ND/4935161"/>
-    <hyperlink ref="H101" r:id="rId61" display="https://www.amazon.com/Source-One-LLC-Acrylic-Plexiglass/dp/B06XNXHKQN/"/>
-    <hyperlink ref="H102" r:id="rId62" location="product-description-iframe" display="https://www.amazon.com/MG-Chemicals-Thermally-Conductive-Encapsulating/dp/B008UH4CRM#product-description-iframe"/>
-    <hyperlink ref="H103" r:id="rId63" display="https://www.amazon.com/CRC-SL2512-Soluble-Oil-32/dp/B000M8O010/"/>
-    <hyperlink ref="H104" r:id="rId64" display="https://www.discountvials.com/6-dram-glass-vial-w-cap/"/>
-    <hyperlink ref="H105" r:id="rId65" display="http://www.hach.com/formazin-turbidity-standard-4000-ntu-500-ml/product?id=7640455437"/>
-    <hyperlink ref="H110" r:id="rId66" display="https://www.dropbox.com/sh/mgy3ndqnzldy1xk/AABXH-txk6h3GChvCx_p5i7ma?dl=0"/>
-    <hyperlink ref="H111" r:id="rId67" display="https://www.digikey.com/product-detail/en/microchip-technology/AT30TS750A-SS8M-T/1611-AT30TS750A-SS8M-TCT-ND/6831450"/>
-    <hyperlink ref="H112" r:id="rId68" display="http://www.digikey.com/product-detail/en/RC1206FR-0710KL/311-10.0KFRCT-ND/731430"/>
-    <hyperlink ref="H113" r:id="rId69" display="https://www.digikey.com/product-detail/en/avx-corporation/1206VC104KAT2A/478-5724-1-ND/2136332"/>
+    <hyperlink ref="H32" r:id="rId18" display="https://www.digikey.com/products/en?keywords=RNCP0603FTD2K74CT-ND"/>
+    <hyperlink ref="H33" r:id="rId19" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP0603FTD100R/RNCP0603FTD100RCT-ND/2240425"/>
+    <hyperlink ref="H34" r:id="rId20" display="https://www.digikey.com/product-detail/en/AYZ0202AGRLC/401-2013-1-ND/1640122"/>
+    <hyperlink ref="H35" r:id="rId21" display="https://www.adafruit.com/product/2343"/>
+    <hyperlink ref="H36" r:id="rId22" display="https://www.digikey.com/products/en?keywords=WM4802-ND"/>
+    <hyperlink ref="H37" r:id="rId23" display="https://www.digikey.com/products/en?keywords=WM9131-ND"/>
+    <hyperlink ref="H38" r:id="rId24" display="https://www.digikey.com/products/en?keywords=WM4801-ND"/>
+    <hyperlink ref="H39" r:id="rId25" display="https://www.digikey.com/products/en?keywords=WM10647-ND"/>
+    <hyperlink ref="H40" r:id="rId26" display="https://www.digikey.com/product-detail/en/3m/3302-16-300SF/MC16M-100-ND/145737"/>
+    <hyperlink ref="H41" r:id="rId27" display="https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2004A.12.02/C2004W-100-ND/57495"/>
+    <hyperlink ref="H46" r:id="rId28" display="https://www.adafruit.com/product/2240"/>
+    <hyperlink ref="H48" r:id="rId29" display="https://www.tapplastics.com/product/plastics/cut_to_size_plastic/satinice_white/655"/>
+    <hyperlink ref="H54" r:id="rId30" display="https://www.atlas-scientific.com/product_pages/circuits/ezo_ph.html"/>
+    <hyperlink ref="H55" r:id="rId31" display="https://www.atlas-scientific.com/product_pages/probes/ph_probe.html"/>
+    <hyperlink ref="H56" r:id="rId32" display="https://www.atlas-scientific.com/product_pages/components/single_carrier_iso.html"/>
+    <hyperlink ref="H57" r:id="rId33" display="https://www.hach.com/ph-buffer-solution-kit-color-coded-ph-4-01-ph-7-00-and-ph-10-01-500-ml-each/product?id=7640205069"/>
+    <hyperlink ref="H58" r:id="rId34" display="https://www.hach.com/electrolyte-solution-kcl-3m-50ml/product-parameter-reagent?id=7640207762"/>
+    <hyperlink ref="H66" r:id="rId35" display="https://www.digikey.com/product-detail/en/yageo/AT0603FRE0710KL/YAG2122CT-ND/5139570"/>
+    <hyperlink ref="H67" r:id="rId36" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP0603FTD2K74/RNCP0603FTD2K74CT-ND/2240457"/>
+    <hyperlink ref="H68" r:id="rId37" display="https://www.digikey.com/product-detail/en/yageo/RT0603BRD071ML/YAG4498CT-ND/6616654"/>
+    <hyperlink ref="H69" r:id="rId38" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP0603FTD1K00/RNCP0603FTD1K00CT-ND/2240445"/>
+    <hyperlink ref="H70" r:id="rId39" display="https://www.digikey.com/product-detail/en/yageo/RT0603BRD0742K2L/YAG4556CT-ND/6616712"/>
+    <hyperlink ref="H71" r:id="rId40" display="https://www.digikey.com/product-detail/en/yageo/RT0603DRE071K2L/311-2461-1-ND/6128880"/>
+    <hyperlink ref="H72" r:id="rId41" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X8R1H104K080AB/445-8818-1-ND/3248223"/>
+    <hyperlink ref="H73" r:id="rId42" display="https://www.digikey.com/products/en?keywords=641-1331-1-ND"/>
+    <hyperlink ref="H74" r:id="rId43" display="https://www.digikey.com/product-detail/en/texas-instruments/TLE2426CD/296-6547-5-ND/371934"/>
+    <hyperlink ref="H75" r:id="rId44" display="https://www.digikey.com/product-detail/en/analog-devices-inc/AD8655ARZ-REEL7/AD8655ARZ-REEL7CT-ND/3678589"/>
+    <hyperlink ref="H76" r:id="rId45" display="https://www.digikey.com/product-detail/en/texas-instruments/TLV2374IDR/296-11967-1-ND/390435"/>
+    <hyperlink ref="H77" r:id="rId46" display="https://www.digikey.com/product-detail/en/AYZ0202AGRLC/401-2013-1-ND/1640122"/>
+    <hyperlink ref="H79" r:id="rId47" display="https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2117A.12.06/C2117G-100-ND/16217"/>
+    <hyperlink ref="H80" r:id="rId48" display="https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2004A.12.02/C2004W-100-ND/57495"/>
+    <hyperlink ref="H86" r:id="rId49" display="https://www.amazon.com/gp/product/B01F2R2EPE/"/>
+    <hyperlink ref="H87" r:id="rId50" display="https://www.amazon.com/gp/product/B01F7L9QD8/"/>
+    <hyperlink ref="H92" r:id="rId51" display="https://www.digikey.com/product-detail/en/vishay-semiconductor-opto-division/VSMY2850G/VSMY2850GCT-ND/2615293"/>
+    <hyperlink ref="H93" r:id="rId52" display="https://www.digikey.com/product-detail/en/ams/TSL237T/TSL237-TCT-ND/3095287"/>
+    <hyperlink ref="H94" r:id="rId53" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X8R1H104K080AB/445-8818-1-ND/3248223"/>
+    <hyperlink ref="H95" r:id="rId54" display="https://www.digikey.com/product-detail/en/yageo/RT0603DRD07200RL/311-200DCT-ND/1035740"/>
+    <hyperlink ref="H98" r:id="rId55" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-BK005/422010-BK005-ND/3705786"/>
+    <hyperlink ref="H99" r:id="rId56" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-RD005/422010-RD005-ND/4935160"/>
+    <hyperlink ref="H100" r:id="rId57" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-SL005/422010-SL005-ND/4935161"/>
+    <hyperlink ref="H101" r:id="rId58" display="https://www.amazon.com/Source-One-LLC-Acrylic-Plexiglass/dp/B06XNXHKQN/"/>
+    <hyperlink ref="H102" r:id="rId59" location="product-description-iframe" display="https://www.amazon.com/MG-Chemicals-Thermally-Conductive-Encapsulating/dp/B008UH4CRM#product-description-iframe"/>
+    <hyperlink ref="H103" r:id="rId60" display="https://www.amazon.com/CRC-SL2512-Soluble-Oil-32/dp/B000M8O010/"/>
+    <hyperlink ref="H104" r:id="rId61" display="https://www.discountvials.com/6-dram-glass-vial-w-cap/"/>
+    <hyperlink ref="H105" r:id="rId62" display="http://www.hach.com/formazin-turbidity-standard-4000-ntu-500-ml/product?id=7640455437"/>
+    <hyperlink ref="H111" r:id="rId63" display="https://www.digikey.com/product-detail/en/microchip-technology/AT30TS750A-SS8M-T/1611-AT30TS750A-SS8M-TCT-ND/6831450"/>
+    <hyperlink ref="H112" r:id="rId64" display="http://www.digikey.com/product-detail/en/RC1206FR-0710KL/311-10.0KFRCT-ND/731430"/>
+    <hyperlink ref="H113" r:id="rId65" display="https://www.digikey.com/product-detail/en/avx-corporation/1206VC104KAT2A/478-5724-1-ND/2136332"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
parts list update with new attachers and conductivity code fix
</commit_message>
<xml_diff>
--- a/hardware/SeeBoat_fullPartsList.xlsx
+++ b/hardware/SeeBoat_fullPartsList.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="348">
   <si>
     <t xml:space="preserve">Parts list for SeeBoat &amp; full sensor suite</t>
   </si>
@@ -455,13 +455,49 @@
     <t xml:space="preserve">https://www.hach.com/electrolyte-solution-kcl-3m-50ml/product-parameter-reagent?id=7640207762</t>
   </si>
   <si>
-    <t xml:space="preserve">mounting materials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to attach the probe to the boat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TBD</t>
+    <t xml:space="preserve">3/4” 8-32 screws</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ace Hardware</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to attach the holder to the boat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8-32 nuts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/32 rubber washers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to attach the holder to the boat and water seal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plastic Expansion Routing Clamp, 5/8" ID, 2-7/16" Long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">McMaster Carr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">holder to attach the probe to the boat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mcmaster.com/8972T11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/2” inner diameter foam tubing, ~1” length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foam tubing to go around the probe so it securely attaches in the holder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mcmaster.com/4339T5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">small rubber band/o-ring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to make the foam tubing secure on the pH probe</t>
   </si>
   <si>
     <t xml:space="preserve">CONDUCTIVITY SENSOR</t>
@@ -581,7 +617,58 @@
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2117A.12.06/C2117G-100-ND/16217</t>
   </si>
   <si>
+    <t xml:space="preserve">Molex 2 pin header (female)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WM4800-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to connect the probe wires to the board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/products/en?keywords=%09WM4800-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molex 2 pin header (male)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WM2900-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/products/en?keywords=WM2900-ND%E2%80%8E</t>
+  </si>
+  <si>
     <t xml:space="preserve">3D printed probe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eden Vero White</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sensor probe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3D printed probe housing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">connects to the boat directly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plastic screws</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to connect the probe housing to the boat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plastic nuts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plastic to plastic epoxy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to glue the probe to the boat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/gp/product/B01IBOK7FE/</t>
   </si>
   <si>
     <t xml:space="preserve">screws</t>
@@ -984,13 +1071,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="MMMM\ YYYY"/>
     <numFmt numFmtId="166" formatCode="\$#,##0"/>
     <numFmt numFmtId="167" formatCode="\$#,##0.00"/>
+    <numFmt numFmtId="168" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1105,6 +1193,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1279,7 +1375,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="60">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1404,6 +1500,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1428,7 +1528,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1436,19 +1556,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1456,15 +1564,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1472,11 +1584,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1488,7 +1600,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1581,10 +1693,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB1048576"/>
+  <dimension ref="A1:AB130"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3105,242 +3217,182 @@
       </c>
       <c r="B60" s="17"/>
       <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="16" t="s">
+      <c r="D60" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="F60" s="17"/>
-      <c r="G60" s="17"/>
-      <c r="H60" s="16" t="s">
+      <c r="E60" s="17" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="26"/>
-    </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="27"/>
-      <c r="B62" s="27"/>
-      <c r="C62" s="27"/>
-      <c r="D62" s="27"/>
-      <c r="E62" s="27"/>
-      <c r="F62" s="27"/>
-      <c r="G62" s="27"/>
-      <c r="H62" s="27"/>
-      <c r="I62" s="27"/>
-      <c r="J62" s="27"/>
-      <c r="K62" s="27"/>
-      <c r="L62" s="27"/>
-      <c r="M62" s="27"/>
-      <c r="N62" s="27"/>
-      <c r="O62" s="27"/>
-      <c r="P62" s="27"/>
-      <c r="Q62" s="27"/>
-      <c r="R62" s="27"/>
-      <c r="S62" s="27"/>
-      <c r="T62" s="27"/>
-      <c r="U62" s="27"/>
-      <c r="V62" s="27"/>
-      <c r="W62" s="27"/>
-      <c r="X62" s="27"/>
-      <c r="Y62" s="27"/>
-      <c r="Z62" s="27"/>
-      <c r="AA62" s="27"/>
-      <c r="AB62" s="27"/>
-    </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="10" t="s">
+      <c r="F60" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="G60" s="19" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="H60" s="17"/>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="16" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="12" t="s">
+      <c r="B61" s="17"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E61" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="F61" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="G61" s="19" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="H61" s="17"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B62" s="17"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E62" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="F62" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="B64" s="13"/>
-      <c r="C64" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E64" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F64" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G64" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H64" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I64" s="13"/>
-      <c r="J64" s="13"/>
-      <c r="K64" s="13"/>
-      <c r="L64" s="13"/>
-      <c r="M64" s="13"/>
-      <c r="N64" s="13"/>
-      <c r="O64" s="13"/>
-      <c r="P64" s="13"/>
-      <c r="Q64" s="13"/>
-      <c r="R64" s="13"/>
-      <c r="S64" s="13"/>
-      <c r="T64" s="13"/>
-      <c r="U64" s="13"/>
-      <c r="V64" s="13"/>
-      <c r="W64" s="13"/>
-      <c r="X64" s="13"/>
-      <c r="Y64" s="13"/>
-      <c r="Z64" s="13"/>
-      <c r="AA64" s="13"/>
-      <c r="AB64" s="13"/>
+      <c r="G62" s="19" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="H62" s="17"/>
+    </row>
+    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B63" s="17"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="E63" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="F63" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="G63" s="19" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="H63" s="31" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B64" s="17"/>
+      <c r="C64" s="17"/>
+      <c r="D64" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="E64" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F64" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="G64" s="19" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="H64" s="31" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="16" t="s">
-        <v>148</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="B65" s="17"/>
       <c r="C65" s="17"/>
-      <c r="D65" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E65" s="31"/>
-      <c r="F65" s="16" t="n">
+      <c r="D65" s="17"/>
+      <c r="E65" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="F65" s="17" t="n">
         <v>1</v>
       </c>
       <c r="G65" s="19" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="H65" s="16"/>
+    </row>
+    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="26"/>
+    </row>
+    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="27"/>
+      <c r="B67" s="27"/>
+      <c r="C67" s="27"/>
+      <c r="D67" s="27"/>
+      <c r="E67" s="27"/>
+      <c r="F67" s="27"/>
+      <c r="G67" s="27"/>
+      <c r="H67" s="27"/>
+      <c r="I67" s="27"/>
+      <c r="J67" s="27"/>
+      <c r="K67" s="27"/>
+      <c r="L67" s="27"/>
+      <c r="M67" s="27"/>
+      <c r="N67" s="27"/>
+      <c r="O67" s="27"/>
+      <c r="P67" s="27"/>
+      <c r="Q67" s="27"/>
+      <c r="R67" s="27"/>
+      <c r="S67" s="27"/>
+      <c r="T67" s="27"/>
+      <c r="U67" s="27"/>
+      <c r="V67" s="27"/>
+      <c r="W67" s="27"/>
+      <c r="X67" s="27"/>
+      <c r="Y67" s="27"/>
+      <c r="Z67" s="27"/>
+      <c r="AA67" s="27"/>
+      <c r="AB67" s="27"/>
+    </row>
+    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B69" s="13"/>
+      <c r="C69" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H65" s="20" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="C66" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="D66" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E66" s="17"/>
-      <c r="F66" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="G66" s="30" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="H66" s="20" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="B67" s="13"/>
-      <c r="C67" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D67" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E67" s="16"/>
-      <c r="F67" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G67" s="30" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="H67" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="I67" s="13"/>
-      <c r="J67" s="13"/>
-      <c r="K67" s="13"/>
-      <c r="L67" s="13"/>
-      <c r="M67" s="13"/>
-      <c r="N67" s="13"/>
-      <c r="O67" s="13"/>
-      <c r="P67" s="13"/>
-      <c r="Q67" s="13"/>
-      <c r="R67" s="13"/>
-      <c r="S67" s="13"/>
-      <c r="T67" s="13"/>
-      <c r="U67" s="13"/>
-      <c r="V67" s="13"/>
-      <c r="W67" s="13"/>
-      <c r="X67" s="13"/>
-      <c r="Y67" s="13"/>
-      <c r="Z67" s="13"/>
-      <c r="AA67" s="13"/>
-      <c r="AB67" s="13"/>
-    </row>
-    <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="B68" s="13"/>
-      <c r="C68" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="D68" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E68" s="16"/>
-      <c r="F68" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G68" s="29" t="n">
-        <v>0.34</v>
-      </c>
-      <c r="H68" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="I68" s="13"/>
-      <c r="J68" s="13"/>
-      <c r="K68" s="13"/>
-      <c r="L68" s="13"/>
-      <c r="M68" s="13"/>
-      <c r="N68" s="13"/>
-      <c r="O68" s="13"/>
-      <c r="P68" s="13"/>
-      <c r="Q68" s="13"/>
-      <c r="R68" s="13"/>
-      <c r="S68" s="13"/>
-      <c r="T68" s="13"/>
-      <c r="U68" s="13"/>
-      <c r="V68" s="13"/>
-      <c r="W68" s="13"/>
-      <c r="X68" s="13"/>
-      <c r="Y68" s="13"/>
-      <c r="Z68" s="13"/>
-      <c r="AA68" s="13"/>
-      <c r="AB68" s="13"/>
-    </row>
-    <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="B69" s="13"/>
-      <c r="C69" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="D69" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E69" s="16"/>
-      <c r="F69" s="22" t="n">
-        <v>2</v>
-      </c>
-      <c r="G69" s="30" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="H69" s="33" t="s">
-        <v>160</v>
+      <c r="F69" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G69" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H69" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="I69" s="13"/>
       <c r="J69" s="13"/>
@@ -3363,110 +3415,66 @@
       <c r="AA69" s="13"/>
       <c r="AB69" s="13"/>
     </row>
-    <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C70" s="17"/>
+      <c r="D70" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E70" s="32"/>
+      <c r="F70" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G70" s="19" t="n">
+        <v>7</v>
+      </c>
+      <c r="H70" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="B70" s="13"/>
-      <c r="C70" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="D70" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E70" s="16"/>
-      <c r="F70" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G70" s="30" t="n">
-        <v>0.34</v>
-      </c>
-      <c r="H70" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="I70" s="13"/>
-      <c r="J70" s="13"/>
-      <c r="K70" s="13"/>
-      <c r="L70" s="13"/>
-      <c r="M70" s="13"/>
-      <c r="N70" s="13"/>
-      <c r="O70" s="13"/>
-      <c r="P70" s="13"/>
-      <c r="Q70" s="13"/>
-      <c r="R70" s="13"/>
-      <c r="S70" s="13"/>
-      <c r="T70" s="13"/>
-      <c r="U70" s="13"/>
-      <c r="V70" s="13"/>
-      <c r="W70" s="13"/>
-      <c r="X70" s="13"/>
-      <c r="Y70" s="13"/>
-      <c r="Z70" s="13"/>
-      <c r="AA70" s="13"/>
-      <c r="AB70" s="13"/>
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="B71" s="13"/>
+        <v>162</v>
+      </c>
       <c r="C71" s="21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D71" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="E71" s="16"/>
-      <c r="F71" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G71" s="29" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="H71" s="32" t="s">
+      <c r="E71" s="17"/>
+      <c r="F71" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="G71" s="30" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="H71" s="20" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B72" s="13"/>
+      <c r="C72" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D72" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E72" s="16"/>
+      <c r="F72" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G72" s="30" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H72" s="33" t="s">
         <v>166</v>
-      </c>
-      <c r="I71" s="13"/>
-      <c r="J71" s="13"/>
-      <c r="K71" s="13"/>
-      <c r="L71" s="13"/>
-      <c r="M71" s="13"/>
-      <c r="N71" s="13"/>
-      <c r="O71" s="13"/>
-      <c r="P71" s="13"/>
-      <c r="Q71" s="13"/>
-      <c r="R71" s="13"/>
-      <c r="S71" s="13"/>
-      <c r="T71" s="13"/>
-      <c r="U71" s="13"/>
-      <c r="V71" s="13"/>
-      <c r="W71" s="13"/>
-      <c r="X71" s="13"/>
-      <c r="Y71" s="13"/>
-      <c r="Z71" s="13"/>
-      <c r="AA71" s="13"/>
-      <c r="AB71" s="13"/>
-    </row>
-    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="34" t="s">
-        <v>167</v>
-      </c>
-      <c r="B72" s="13"/>
-      <c r="C72" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="D72" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="E72" s="17"/>
-      <c r="F72" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G72" s="29" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="H72" s="20" t="s">
-        <v>169</v>
       </c>
       <c r="I72" s="13"/>
       <c r="J72" s="13"/>
@@ -3490,50 +3498,71 @@
       <c r="AB72" s="13"/>
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="C73" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="D73" s="21" t="s">
+      <c r="A73" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="B73" s="13"/>
+      <c r="C73" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="D73" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="E73" s="31"/>
+      <c r="E73" s="16"/>
       <c r="F73" s="22" t="n">
-        <v>2</v>
-      </c>
-      <c r="G73" s="30" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="H73" s="35" t="s">
-        <v>172</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G73" s="29" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="H73" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="I73" s="13"/>
+      <c r="J73" s="13"/>
+      <c r="K73" s="13"/>
+      <c r="L73" s="13"/>
+      <c r="M73" s="13"/>
+      <c r="N73" s="13"/>
+      <c r="O73" s="13"/>
+      <c r="P73" s="13"/>
+      <c r="Q73" s="13"/>
+      <c r="R73" s="13"/>
+      <c r="S73" s="13"/>
+      <c r="T73" s="13"/>
+      <c r="U73" s="13"/>
+      <c r="V73" s="13"/>
+      <c r="W73" s="13"/>
+      <c r="X73" s="13"/>
+      <c r="Y73" s="13"/>
+      <c r="Z73" s="13"/>
+      <c r="AA73" s="13"/>
+      <c r="AB73" s="13"/>
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="16" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B74" s="13"/>
-      <c r="C74" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="D74" s="21" t="s">
+      <c r="C74" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="D74" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="E74" s="17"/>
+      <c r="E74" s="16"/>
       <c r="F74" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G74" s="23" t="n">
-        <v>1.86</v>
-      </c>
-      <c r="H74" s="36" t="s">
-        <v>175</v>
-      </c>
-      <c r="I74" s="25"/>
-      <c r="J74" s="25"/>
-      <c r="K74" s="25"/>
+        <v>2</v>
+      </c>
+      <c r="G74" s="30" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H74" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="I74" s="13"/>
+      <c r="J74" s="13"/>
+      <c r="K74" s="13"/>
       <c r="L74" s="13"/>
       <c r="M74" s="13"/>
       <c r="N74" s="13"/>
@@ -3549,32 +3578,34 @@
       <c r="X74" s="13"/>
       <c r="Y74" s="13"/>
       <c r="Z74" s="13"/>
+      <c r="AA74" s="13"/>
+      <c r="AB74" s="13"/>
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="16" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B75" s="13"/>
-      <c r="C75" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="D75" s="21" t="s">
+      <c r="C75" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="D75" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="E75" s="17"/>
+      <c r="E75" s="16"/>
       <c r="F75" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="G75" s="29" t="n">
-        <v>2.64</v>
-      </c>
-      <c r="H75" s="36" t="s">
-        <v>178</v>
-      </c>
-      <c r="I75" s="25"/>
-      <c r="J75" s="25"/>
-      <c r="K75" s="25"/>
-      <c r="L75" s="25"/>
+      <c r="G75" s="30" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="H75" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="I75" s="13"/>
+      <c r="J75" s="13"/>
+      <c r="K75" s="13"/>
+      <c r="L75" s="13"/>
       <c r="M75" s="13"/>
       <c r="N75" s="13"/>
       <c r="O75" s="13"/>
@@ -3589,29 +3620,33 @@
       <c r="X75" s="13"/>
       <c r="Y75" s="13"/>
       <c r="Z75" s="13"/>
+      <c r="AA75" s="13"/>
+      <c r="AB75" s="13"/>
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="16" t="s">
         <v>176</v>
       </c>
       <c r="B76" s="13"/>
-      <c r="C76" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="D76" s="17"/>
+      <c r="C76" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="D76" s="16" t="s">
+        <v>76</v>
+      </c>
       <c r="E76" s="16"/>
       <c r="F76" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="G76" s="23" t="n">
-        <v>1.81</v>
-      </c>
-      <c r="H76" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="I76" s="25"/>
-      <c r="J76" s="25"/>
-      <c r="K76" s="25"/>
+      <c r="G76" s="29" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="H76" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="I76" s="13"/>
+      <c r="J76" s="13"/>
+      <c r="K76" s="13"/>
       <c r="L76" s="13"/>
       <c r="M76" s="13"/>
       <c r="N76" s="13"/>
@@ -3627,90 +3662,98 @@
       <c r="X76" s="13"/>
       <c r="Y76" s="13"/>
       <c r="Z76" s="13"/>
+      <c r="AA76" s="13"/>
+      <c r="AB76" s="13"/>
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="C77" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="D77" s="16" t="s">
+      <c r="A77" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="B77" s="13"/>
+      <c r="C77" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="D77" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="E77" s="16" t="s">
+      <c r="E77" s="17"/>
+      <c r="F77" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G77" s="29" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="H77" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="F77" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G77" s="29" t="n">
-        <v>1.07</v>
-      </c>
-      <c r="H77" s="20" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="16"/>
-      <c r="B78" s="13"/>
-      <c r="C78" s="21"/>
-      <c r="D78" s="16"/>
-      <c r="E78" s="16"/>
-      <c r="F78" s="22"/>
-      <c r="G78" s="23"/>
-      <c r="H78" s="32"/>
-      <c r="I78" s="13"/>
-      <c r="J78" s="13"/>
-      <c r="K78" s="13"/>
-      <c r="L78" s="13"/>
-      <c r="M78" s="13"/>
-      <c r="N78" s="13"/>
-      <c r="O78" s="13"/>
-      <c r="P78" s="13"/>
-      <c r="Q78" s="13"/>
-      <c r="R78" s="13"/>
-      <c r="S78" s="13"/>
-      <c r="T78" s="13"/>
-      <c r="U78" s="13"/>
-      <c r="V78" s="13"/>
-      <c r="W78" s="13"/>
-      <c r="X78" s="13"/>
-      <c r="Y78" s="13"/>
-      <c r="Z78" s="13"/>
-      <c r="AA78" s="13"/>
-      <c r="AB78" s="13"/>
+      <c r="I77" s="13"/>
+      <c r="J77" s="13"/>
+      <c r="K77" s="13"/>
+      <c r="L77" s="13"/>
+      <c r="M77" s="13"/>
+      <c r="N77" s="13"/>
+      <c r="O77" s="13"/>
+      <c r="P77" s="13"/>
+      <c r="Q77" s="13"/>
+      <c r="R77" s="13"/>
+      <c r="S77" s="13"/>
+      <c r="T77" s="13"/>
+      <c r="U77" s="13"/>
+      <c r="V77" s="13"/>
+      <c r="W77" s="13"/>
+      <c r="X77" s="13"/>
+      <c r="Y77" s="13"/>
+      <c r="Z77" s="13"/>
+      <c r="AA77" s="13"/>
+      <c r="AB77" s="13"/>
+    </row>
+    <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="C78" s="35" t="s">
+        <v>183</v>
+      </c>
+      <c r="D78" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E78" s="32"/>
+      <c r="F78" s="22" t="n">
+        <v>2</v>
+      </c>
+      <c r="G78" s="30" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="H78" s="36" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="B79" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="C79" s="21" t="s">
-        <v>183</v>
-      </c>
-      <c r="D79" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="B79" s="13"/>
+      <c r="C79" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="D79" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="E79" s="16" t="s">
-        <v>184</v>
-      </c>
+      <c r="E79" s="17"/>
       <c r="F79" s="22" t="n">
         <v>1</v>
       </c>
       <c r="G79" s="23" t="n">
-        <v>16</v>
-      </c>
-      <c r="H79" s="24" t="s">
-        <v>185</v>
+        <v>1.86</v>
+      </c>
+      <c r="H79" s="37" t="s">
+        <v>187</v>
       </c>
       <c r="I79" s="25"/>
       <c r="J79" s="25"/>
       <c r="K79" s="25"/>
-      <c r="L79" s="25"/>
-      <c r="M79" s="25"/>
+      <c r="L79" s="13"/>
+      <c r="M79" s="13"/>
       <c r="N79" s="13"/>
       <c r="O79" s="13"/>
       <c r="P79" s="13"/>
@@ -3724,39 +3767,33 @@
       <c r="X79" s="13"/>
       <c r="Y79" s="13"/>
       <c r="Z79" s="13"/>
-      <c r="AA79" s="13"/>
-      <c r="AB79" s="13"/>
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="B80" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="C80" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="D80" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="B80" s="13"/>
+      <c r="C80" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="D80" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="E80" s="16" t="s">
-        <v>184</v>
-      </c>
+      <c r="E80" s="17"/>
       <c r="F80" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="G80" s="23" t="n">
-        <v>16</v>
-      </c>
-      <c r="H80" s="24" t="s">
-        <v>115</v>
+      <c r="G80" s="29" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="H80" s="37" t="s">
+        <v>190</v>
       </c>
       <c r="I80" s="25"/>
       <c r="J80" s="25"/>
       <c r="K80" s="25"/>
       <c r="L80" s="25"/>
-      <c r="M80" s="25"/>
+      <c r="M80" s="13"/>
       <c r="N80" s="13"/>
       <c r="O80" s="13"/>
       <c r="P80" s="13"/>
@@ -3770,889 +3807,1236 @@
       <c r="X80" s="13"/>
       <c r="Y80" s="13"/>
       <c r="Z80" s="13"/>
-      <c r="AA80" s="13"/>
-      <c r="AB80" s="13"/>
-    </row>
-    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="17"/>
-      <c r="C81" s="17"/>
+    </row>
+    <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="B81" s="13"/>
+      <c r="C81" s="18" t="s">
+        <v>191</v>
+      </c>
       <c r="D81" s="17"/>
-      <c r="E81" s="17"/>
-      <c r="F81" s="17"/>
-      <c r="G81" s="17"/>
-      <c r="H81" s="17"/>
-    </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E81" s="16"/>
+      <c r="F81" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G81" s="23" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="H81" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="I81" s="25"/>
+      <c r="J81" s="25"/>
+      <c r="K81" s="25"/>
+      <c r="L81" s="13"/>
+      <c r="M81" s="13"/>
+      <c r="N81" s="13"/>
+      <c r="O81" s="13"/>
+      <c r="P81" s="13"/>
+      <c r="Q81" s="13"/>
+      <c r="R81" s="13"/>
+      <c r="S81" s="13"/>
+      <c r="T81" s="13"/>
+      <c r="U81" s="13"/>
+      <c r="V81" s="13"/>
+      <c r="W81" s="13"/>
+      <c r="X81" s="13"/>
+      <c r="Y81" s="13"/>
+      <c r="Z81" s="13"/>
+    </row>
+    <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="C82" s="17"/>
-      <c r="D82" s="17"/>
-      <c r="E82" s="17"/>
+        <v>83</v>
+      </c>
+      <c r="C82" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D82" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E82" s="16" t="s">
+        <v>193</v>
+      </c>
       <c r="F82" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="G82" s="17"/>
-      <c r="H82" s="17"/>
+      <c r="G82" s="29" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="H82" s="20" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="C83" s="17"/>
-      <c r="D83" s="17"/>
-      <c r="E83" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="F83" s="16" t="n">
+      <c r="A83" s="16"/>
+      <c r="B83" s="13"/>
+      <c r="C83" s="21"/>
+      <c r="D83" s="16"/>
+      <c r="E83" s="16"/>
+      <c r="F83" s="22"/>
+      <c r="G83" s="23"/>
+      <c r="H83" s="33"/>
+      <c r="I83" s="13"/>
+      <c r="J83" s="13"/>
+      <c r="K83" s="13"/>
+      <c r="L83" s="13"/>
+      <c r="M83" s="13"/>
+      <c r="N83" s="13"/>
+      <c r="O83" s="13"/>
+      <c r="P83" s="13"/>
+      <c r="Q83" s="13"/>
+      <c r="R83" s="13"/>
+      <c r="S83" s="13"/>
+      <c r="T83" s="13"/>
+      <c r="U83" s="13"/>
+      <c r="V83" s="13"/>
+      <c r="W83" s="13"/>
+      <c r="X83" s="13"/>
+      <c r="Y83" s="13"/>
+      <c r="Z83" s="13"/>
+      <c r="AA83" s="13"/>
+      <c r="AB83" s="13"/>
+    </row>
+    <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="B84" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C84" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="D84" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E84" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="F84" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G84" s="23" t="n">
+        <v>16</v>
+      </c>
+      <c r="H84" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="I84" s="25"/>
+      <c r="J84" s="25"/>
+      <c r="K84" s="25"/>
+      <c r="L84" s="25"/>
+      <c r="M84" s="25"/>
+      <c r="N84" s="13"/>
+      <c r="O84" s="13"/>
+      <c r="P84" s="13"/>
+      <c r="Q84" s="13"/>
+      <c r="R84" s="13"/>
+      <c r="S84" s="13"/>
+      <c r="T84" s="13"/>
+      <c r="U84" s="13"/>
+      <c r="V84" s="13"/>
+      <c r="W84" s="13"/>
+      <c r="X84" s="13"/>
+      <c r="Y84" s="13"/>
+      <c r="Z84" s="13"/>
+      <c r="AA84" s="13"/>
+      <c r="AB84" s="13"/>
+    </row>
+    <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B85" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C85" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D85" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E85" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="F85" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G85" s="23" t="n">
+        <v>16</v>
+      </c>
+      <c r="H85" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="I85" s="25"/>
+      <c r="J85" s="25"/>
+      <c r="K85" s="25"/>
+      <c r="L85" s="25"/>
+      <c r="M85" s="25"/>
+      <c r="N85" s="13"/>
+      <c r="O85" s="13"/>
+      <c r="P85" s="13"/>
+      <c r="Q85" s="13"/>
+      <c r="R85" s="13"/>
+      <c r="S85" s="13"/>
+      <c r="T85" s="13"/>
+      <c r="U85" s="13"/>
+      <c r="V85" s="13"/>
+      <c r="W85" s="13"/>
+      <c r="X85" s="13"/>
+      <c r="Y85" s="13"/>
+      <c r="Z85" s="13"/>
+      <c r="AA85" s="13"/>
+      <c r="AB85" s="13"/>
+    </row>
+    <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="B86" s="13"/>
+      <c r="C86" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="D86" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E86" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="F86" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G86" s="23" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="H86" s="39" t="s">
+        <v>201</v>
+      </c>
+      <c r="I86" s="25"/>
+      <c r="J86" s="25"/>
+      <c r="K86" s="25"/>
+      <c r="L86" s="25"/>
+      <c r="M86" s="25"/>
+      <c r="N86" s="13"/>
+      <c r="O86" s="13"/>
+      <c r="P86" s="13"/>
+      <c r="Q86" s="13"/>
+      <c r="R86" s="13"/>
+      <c r="S86" s="13"/>
+      <c r="T86" s="13"/>
+      <c r="U86" s="13"/>
+      <c r="V86" s="13"/>
+      <c r="W86" s="13"/>
+      <c r="X86" s="13"/>
+      <c r="Y86" s="13"/>
+      <c r="Z86" s="13"/>
+      <c r="AA86" s="13"/>
+      <c r="AB86" s="13"/>
+    </row>
+    <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="B87" s="13"/>
+      <c r="C87" s="38" t="s">
+        <v>203</v>
+      </c>
+      <c r="D87" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E87" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="F87" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G87" s="23" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="H87" s="39" t="s">
+        <v>204</v>
+      </c>
+      <c r="I87" s="25"/>
+      <c r="J87" s="25"/>
+      <c r="K87" s="25"/>
+      <c r="L87" s="25"/>
+      <c r="M87" s="25"/>
+      <c r="N87" s="13"/>
+      <c r="O87" s="13"/>
+      <c r="P87" s="13"/>
+      <c r="Q87" s="13"/>
+      <c r="R87" s="13"/>
+      <c r="S87" s="13"/>
+      <c r="T87" s="13"/>
+      <c r="U87" s="13"/>
+      <c r="V87" s="13"/>
+      <c r="W87" s="13"/>
+      <c r="X87" s="13"/>
+      <c r="Y87" s="13"/>
+      <c r="Z87" s="13"/>
+      <c r="AA87" s="13"/>
+      <c r="AB87" s="13"/>
+    </row>
+    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="17"/>
+      <c r="C88" s="17"/>
+      <c r="D88" s="17"/>
+      <c r="E88" s="17"/>
+      <c r="F88" s="17"/>
+      <c r="G88" s="17"/>
+      <c r="H88" s="17"/>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="C89" s="17"/>
+      <c r="D89" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="E89" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="F89" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G89" s="17"/>
+      <c r="H89" s="17"/>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C90" s="17"/>
+      <c r="D90" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="E90" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="F90" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G90" s="17"/>
+      <c r="H90" s="17"/>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="C91" s="17"/>
+      <c r="D91" s="17"/>
+      <c r="E91" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="F91" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="G83" s="17"/>
-      <c r="H83" s="17"/>
-    </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="C84" s="17"/>
-      <c r="D84" s="17"/>
-      <c r="E84" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="F84" s="16" t="n">
+      <c r="G91" s="17"/>
+      <c r="H91" s="17"/>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="C92" s="17"/>
+      <c r="D92" s="17"/>
+      <c r="E92" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="F92" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="G84" s="17"/>
-      <c r="H84" s="17"/>
-    </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="37" t="s">
-        <v>190</v>
-      </c>
-      <c r="C85" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="D85" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="E85" s="37" t="s">
-        <v>192</v>
-      </c>
-      <c r="F85" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="G85" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="H85" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="I85" s="38"/>
-      <c r="J85" s="38"/>
-      <c r="K85" s="38"/>
-      <c r="L85" s="38"/>
-      <c r="M85" s="38"/>
-      <c r="N85" s="38"/>
-      <c r="O85" s="38"/>
-      <c r="P85" s="38"/>
-      <c r="Q85" s="38"/>
-      <c r="R85" s="38"/>
-      <c r="S85" s="38"/>
-      <c r="T85" s="38"/>
-      <c r="U85" s="38"/>
-      <c r="V85" s="38"/>
-      <c r="W85" s="38"/>
-      <c r="X85" s="38"/>
-      <c r="Y85" s="38"/>
-      <c r="Z85" s="38"/>
-      <c r="AA85" s="38"/>
-      <c r="AB85" s="38"/>
-    </row>
-    <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="C86" s="17"/>
-      <c r="D86" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E86" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="F86" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G86" s="19" t="n">
-        <v>17</v>
-      </c>
-      <c r="H86" s="20" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="21" t="s">
-        <v>195</v>
-      </c>
-      <c r="C87" s="17"/>
-      <c r="D87" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E87" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="F87" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G87" s="19" t="n">
-        <v>17</v>
-      </c>
-      <c r="H87" s="20" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="27"/>
-      <c r="B89" s="27"/>
-      <c r="C89" s="27"/>
-      <c r="D89" s="27"/>
-      <c r="E89" s="27"/>
-      <c r="F89" s="27"/>
-      <c r="G89" s="27"/>
-      <c r="H89" s="27"/>
-      <c r="I89" s="27"/>
-      <c r="J89" s="27"/>
-      <c r="K89" s="27"/>
-      <c r="L89" s="27"/>
-      <c r="M89" s="27"/>
-      <c r="N89" s="27"/>
-      <c r="O89" s="27"/>
-      <c r="P89" s="27"/>
-      <c r="Q89" s="27"/>
-      <c r="R89" s="27"/>
-      <c r="S89" s="27"/>
-      <c r="T89" s="27"/>
-      <c r="U89" s="27"/>
-      <c r="V89" s="27"/>
-      <c r="W89" s="27"/>
-      <c r="X89" s="27"/>
-      <c r="Y89" s="27"/>
-      <c r="Z89" s="27"/>
-      <c r="AA89" s="27"/>
-      <c r="AB89" s="27"/>
-    </row>
-    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="D90" s="11"/>
-    </row>
-    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C91" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D91" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E91" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F91" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G91" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H91" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I91" s="13"/>
-      <c r="J91" s="13"/>
-      <c r="K91" s="13"/>
-      <c r="L91" s="13"/>
-      <c r="M91" s="13"/>
-      <c r="N91" s="13"/>
-      <c r="O91" s="13"/>
-      <c r="P91" s="13"/>
-      <c r="Q91" s="13"/>
-      <c r="R91" s="13"/>
-      <c r="S91" s="13"/>
-      <c r="T91" s="13"/>
-      <c r="U91" s="13"/>
-      <c r="V91" s="13"/>
-      <c r="W91" s="13"/>
-      <c r="X91" s="13"/>
-      <c r="Y91" s="13"/>
-      <c r="Z91" s="13"/>
-      <c r="AA91" s="13"/>
-      <c r="AB91" s="13"/>
-    </row>
-    <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="B92" s="17"/>
-      <c r="C92" s="39" t="s">
-        <v>199</v>
-      </c>
-      <c r="D92" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="E92" s="16"/>
-      <c r="F92" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="G92" s="29" t="n">
-        <v>1.06</v>
-      </c>
-      <c r="H92" s="20" t="s">
-        <v>200</v>
-      </c>
+      <c r="G92" s="17"/>
+      <c r="H92" s="17"/>
     </row>
     <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="B93" s="17"/>
-      <c r="C93" s="39" t="s">
-        <v>202</v>
-      </c>
-      <c r="D93" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="E93" s="16"/>
-      <c r="F93" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="G93" s="29" t="n">
-        <v>5.31</v>
-      </c>
-      <c r="H93" s="20" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="B94" s="17"/>
-      <c r="C94" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="D94" s="21" t="s">
-        <v>76</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="C93" s="17"/>
+      <c r="D93" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E93" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="F93" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G93" s="40" t="n">
+        <v>7.12</v>
+      </c>
+      <c r="H93" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="16"/>
+      <c r="C94" s="17"/>
+      <c r="D94" s="17"/>
       <c r="E94" s="17"/>
-      <c r="F94" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G94" s="29" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="H94" s="20" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="B95" s="17"/>
-      <c r="C95" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="D95" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="E95" s="17"/>
+      <c r="F94" s="16"/>
+      <c r="G94" s="17"/>
+      <c r="H94" s="17"/>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="C95" s="17"/>
+      <c r="D95" s="17"/>
+      <c r="E95" s="16" t="s">
+        <v>217</v>
+      </c>
       <c r="F95" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G95" s="29" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="H95" s="20" t="s">
-        <v>207</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G95" s="17"/>
+      <c r="H95" s="17"/>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="B96" s="17"/>
+        <v>218</v>
+      </c>
       <c r="C96" s="17"/>
-      <c r="D96" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E96" s="17"/>
+      <c r="D96" s="17"/>
+      <c r="E96" s="16" t="s">
+        <v>217</v>
+      </c>
       <c r="F96" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G96" s="19" t="n">
-        <v>3</v>
-      </c>
-      <c r="H96" s="20" t="s">
-        <v>209</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G96" s="17"/>
+      <c r="H96" s="17"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="B97" s="17"/>
-      <c r="C97" s="17"/>
-      <c r="D97" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E97" s="17"/>
-      <c r="F97" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G97" s="19" t="n">
-        <v>3</v>
-      </c>
-      <c r="H97" s="20" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="B98" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="C98" s="16"/>
+      <c r="A97" s="41" t="s">
+        <v>219</v>
+      </c>
+      <c r="C97" s="41" t="s">
+        <v>220</v>
+      </c>
+      <c r="D97" s="41" t="s">
+        <v>220</v>
+      </c>
+      <c r="E97" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="F97" s="41" t="s">
+        <v>220</v>
+      </c>
+      <c r="G97" s="41" t="s">
+        <v>220</v>
+      </c>
+      <c r="H97" s="41" t="s">
+        <v>220</v>
+      </c>
+      <c r="I97" s="42"/>
+      <c r="J97" s="42"/>
+      <c r="K97" s="42"/>
+      <c r="L97" s="42"/>
+      <c r="M97" s="42"/>
+      <c r="N97" s="42"/>
+      <c r="O97" s="42"/>
+      <c r="P97" s="42"/>
+      <c r="Q97" s="42"/>
+      <c r="R97" s="42"/>
+      <c r="S97" s="42"/>
+      <c r="T97" s="42"/>
+      <c r="U97" s="42"/>
+      <c r="V97" s="42"/>
+      <c r="W97" s="42"/>
+      <c r="X97" s="42"/>
+      <c r="Y97" s="42"/>
+      <c r="Z97" s="42"/>
+      <c r="AA97" s="42"/>
+      <c r="AB97" s="42"/>
+    </row>
+    <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C98" s="17"/>
       <c r="D98" s="16" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E98" s="16" t="s">
-        <v>214</v>
-      </c>
-      <c r="F98" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G98" s="23" t="n">
-        <v>25</v>
-      </c>
-      <c r="H98" s="24" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="B99" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="C99" s="16"/>
+        <v>139</v>
+      </c>
+      <c r="F98" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G98" s="19" t="n">
+        <v>17</v>
+      </c>
+      <c r="H98" s="20" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="C99" s="17"/>
       <c r="D99" s="16" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E99" s="16" t="s">
-        <v>214</v>
-      </c>
-      <c r="F99" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G99" s="23" t="n">
-        <v>25</v>
-      </c>
-      <c r="H99" s="24" t="s">
-        <v>217</v>
-      </c>
-      <c r="I99" s="25"/>
-      <c r="J99" s="25"/>
-      <c r="K99" s="25"/>
-      <c r="L99" s="25"/>
-      <c r="M99" s="13"/>
-      <c r="N99" s="13"/>
-      <c r="O99" s="13"/>
-      <c r="P99" s="13"/>
-      <c r="Q99" s="13"/>
-      <c r="R99" s="13"/>
-      <c r="S99" s="13"/>
-      <c r="T99" s="13"/>
-      <c r="U99" s="13"/>
-      <c r="V99" s="13"/>
-      <c r="W99" s="13"/>
-      <c r="X99" s="13"/>
-      <c r="Y99" s="13"/>
-      <c r="Z99" s="13"/>
-      <c r="AA99" s="13"/>
-      <c r="AB99" s="13"/>
-    </row>
-    <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="16" t="s">
-        <v>218</v>
-      </c>
-      <c r="B100" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="C100" s="16"/>
-      <c r="D100" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E100" s="16" t="s">
-        <v>214</v>
-      </c>
-      <c r="F100" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G100" s="23" t="n">
-        <v>25</v>
-      </c>
-      <c r="H100" s="24" t="s">
-        <v>219</v>
-      </c>
-      <c r="I100" s="25"/>
-      <c r="J100" s="25"/>
-      <c r="K100" s="25"/>
-      <c r="L100" s="25"/>
-      <c r="M100" s="13"/>
-      <c r="N100" s="13"/>
-      <c r="O100" s="13"/>
-      <c r="P100" s="13"/>
-      <c r="Q100" s="13"/>
-      <c r="R100" s="13"/>
-      <c r="S100" s="13"/>
-      <c r="T100" s="13"/>
-      <c r="U100" s="13"/>
-      <c r="V100" s="13"/>
-      <c r="W100" s="13"/>
-      <c r="X100" s="13"/>
-      <c r="Y100" s="13"/>
-      <c r="Z100" s="13"/>
-      <c r="AA100" s="13"/>
-      <c r="AB100" s="13"/>
-    </row>
-    <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="B101" s="17"/>
-      <c r="C101" s="17"/>
-      <c r="D101" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E101" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="F101" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G101" s="19" t="n">
-        <v>13</v>
-      </c>
-      <c r="H101" s="20" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="16" t="s">
-        <v>223</v>
-      </c>
-      <c r="B102" s="17"/>
-      <c r="C102" s="17"/>
-      <c r="D102" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E102" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="F102" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G102" s="30" t="n">
-        <v>43.95</v>
-      </c>
-      <c r="H102" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="F99" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G99" s="19" t="n">
+        <v>17</v>
+      </c>
+      <c r="H99" s="20" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="16" t="s">
+    <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="27"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
+      <c r="D101" s="27"/>
+      <c r="E101" s="27"/>
+      <c r="F101" s="27"/>
+      <c r="G101" s="27"/>
+      <c r="H101" s="27"/>
+      <c r="I101" s="27"/>
+      <c r="J101" s="27"/>
+      <c r="K101" s="27"/>
+      <c r="L101" s="27"/>
+      <c r="M101" s="27"/>
+      <c r="N101" s="27"/>
+      <c r="O101" s="27"/>
+      <c r="P101" s="27"/>
+      <c r="Q101" s="27"/>
+      <c r="R101" s="27"/>
+      <c r="S101" s="27"/>
+      <c r="T101" s="27"/>
+      <c r="U101" s="27"/>
+      <c r="V101" s="27"/>
+      <c r="W101" s="27"/>
+      <c r="X101" s="27"/>
+      <c r="Y101" s="27"/>
+      <c r="Z101" s="27"/>
+      <c r="AA101" s="27"/>
+      <c r="AB101" s="27"/>
+    </row>
+    <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="B103" s="17"/>
-      <c r="C103" s="17"/>
-      <c r="D103" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E103" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="F103" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G103" s="19" t="n">
-        <v>15</v>
-      </c>
-      <c r="H103" s="20" t="s">
-        <v>228</v>
-      </c>
+      <c r="D102" s="11"/>
+    </row>
+    <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C103" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D103" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E103" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F103" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G103" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H103" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I103" s="13"/>
+      <c r="J103" s="13"/>
+      <c r="K103" s="13"/>
+      <c r="L103" s="13"/>
+      <c r="M103" s="13"/>
+      <c r="N103" s="13"/>
+      <c r="O103" s="13"/>
+      <c r="P103" s="13"/>
+      <c r="Q103" s="13"/>
+      <c r="R103" s="13"/>
+      <c r="S103" s="13"/>
+      <c r="T103" s="13"/>
+      <c r="U103" s="13"/>
+      <c r="V103" s="13"/>
+      <c r="W103" s="13"/>
+      <c r="X103" s="13"/>
+      <c r="Y103" s="13"/>
+      <c r="Z103" s="13"/>
+      <c r="AA103" s="13"/>
+      <c r="AB103" s="13"/>
     </row>
     <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="B104" s="17"/>
+      <c r="C104" s="43" t="s">
+        <v>228</v>
+      </c>
+      <c r="D104" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E104" s="16"/>
+      <c r="F104" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="G104" s="29" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="H104" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="B104" s="17"/>
-      <c r="C104" s="17"/>
-      <c r="D104" s="16" t="s">
+    </row>
+    <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="E104" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="F104" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G104" s="19" t="n">
-        <v>17</v>
-      </c>
-      <c r="H104" s="20" t="s">
+      <c r="B105" s="17"/>
+      <c r="C105" s="43" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="37" t="s">
+      <c r="D105" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E105" s="16"/>
+      <c r="F105" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="G105" s="29" t="n">
+        <v>5.31</v>
+      </c>
+      <c r="H105" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="B105" s="40"/>
-      <c r="C105" s="37"/>
-      <c r="D105" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="E105" s="37" t="s">
+    </row>
+    <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="17" t="s">
         <v>233</v>
       </c>
-      <c r="F105" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="G105" s="41" t="n">
-        <v>80</v>
-      </c>
-      <c r="H105" s="42" t="s">
+      <c r="B106" s="17"/>
+      <c r="C106" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="D106" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E106" s="17"/>
+      <c r="F106" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G106" s="29" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="H106" s="20" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="I105" s="43"/>
-      <c r="J105" s="44"/>
-      <c r="K105" s="44"/>
-      <c r="L105" s="44"/>
-      <c r="M105" s="44"/>
-      <c r="N105" s="44"/>
-      <c r="O105" s="44"/>
-      <c r="P105" s="44"/>
-      <c r="Q105" s="44"/>
-      <c r="R105" s="44"/>
-      <c r="S105" s="44"/>
-      <c r="T105" s="44"/>
-      <c r="U105" s="44"/>
-      <c r="V105" s="44"/>
-      <c r="W105" s="44"/>
-      <c r="X105" s="44"/>
-      <c r="Y105" s="44"/>
-      <c r="Z105" s="38"/>
-      <c r="AA105" s="38"/>
-      <c r="AB105" s="38"/>
-    </row>
-    <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="26"/>
-    </row>
-    <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="27"/>
-      <c r="B107" s="27"/>
-      <c r="C107" s="27"/>
-      <c r="D107" s="27"/>
-      <c r="E107" s="27"/>
-      <c r="F107" s="27"/>
-      <c r="G107" s="27"/>
-      <c r="H107" s="27"/>
-      <c r="I107" s="27"/>
-      <c r="J107" s="27"/>
-      <c r="K107" s="27"/>
-      <c r="L107" s="27"/>
-      <c r="M107" s="27"/>
-      <c r="N107" s="27"/>
-      <c r="O107" s="27"/>
-      <c r="P107" s="27"/>
-      <c r="Q107" s="27"/>
-      <c r="R107" s="27"/>
-      <c r="S107" s="27"/>
-      <c r="T107" s="27"/>
-      <c r="U107" s="27"/>
-      <c r="V107" s="27"/>
-      <c r="W107" s="27"/>
-      <c r="X107" s="27"/>
-      <c r="Y107" s="27"/>
-      <c r="Z107" s="27"/>
-      <c r="AA107" s="27"/>
-      <c r="AB107" s="27"/>
-    </row>
-    <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="10" t="s">
+      <c r="B107" s="17"/>
+      <c r="C107" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="D108" s="11"/>
-    </row>
-    <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B109" s="13"/>
-      <c r="C109" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D109" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E109" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F109" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G109" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H109" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I109" s="13"/>
-      <c r="J109" s="13"/>
-      <c r="K109" s="13"/>
-      <c r="L109" s="13"/>
-      <c r="M109" s="13"/>
-      <c r="N109" s="13"/>
-      <c r="O109" s="13"/>
-      <c r="P109" s="13"/>
-      <c r="Q109" s="13"/>
-      <c r="R109" s="13"/>
-      <c r="S109" s="13"/>
-      <c r="T109" s="13"/>
-      <c r="U109" s="13"/>
-      <c r="V109" s="13"/>
-      <c r="W109" s="13"/>
-      <c r="X109" s="13"/>
-      <c r="Y109" s="13"/>
-      <c r="Z109" s="13"/>
-      <c r="AA109" s="13"/>
-      <c r="AB109" s="13"/>
-    </row>
-    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D107" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E107" s="17"/>
+      <c r="F107" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G107" s="29" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="H107" s="20" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="B108" s="17"/>
+      <c r="C108" s="17"/>
+      <c r="D108" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E108" s="17"/>
+      <c r="F108" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G108" s="19" t="n">
+        <v>3</v>
+      </c>
+      <c r="H108" s="20" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="B109" s="17"/>
+      <c r="C109" s="17"/>
+      <c r="D109" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E109" s="17"/>
+      <c r="F109" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G109" s="19" t="n">
+        <v>3</v>
+      </c>
+      <c r="H109" s="20" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="16" t="s">
-        <v>236</v>
-      </c>
-      <c r="B110" s="17"/>
-      <c r="C110" s="17"/>
+        <v>241</v>
+      </c>
+      <c r="B110" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="C110" s="16"/>
       <c r="D110" s="16" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E110" s="16" t="s">
-        <v>237</v>
-      </c>
-      <c r="F110" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G110" s="19" t="n">
-        <v>5</v>
-      </c>
-      <c r="H110" s="20" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>243</v>
+      </c>
+      <c r="F110" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G110" s="23" t="n">
+        <v>25</v>
+      </c>
+      <c r="H110" s="24" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="B111" s="17"/>
-      <c r="C111" s="21" t="s">
-        <v>240</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="B111" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="C111" s="16"/>
       <c r="D111" s="16" t="s">
         <v>76</v>
       </c>
       <c r="E111" s="16" t="s">
-        <v>241</v>
-      </c>
-      <c r="F111" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G111" s="30" t="n">
-        <v>0.6</v>
+        <v>243</v>
+      </c>
+      <c r="F111" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G111" s="23" t="n">
+        <v>25</v>
       </c>
       <c r="H111" s="24" t="s">
-        <v>242</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="I111" s="25"/>
+      <c r="J111" s="25"/>
+      <c r="K111" s="25"/>
+      <c r="L111" s="25"/>
+      <c r="M111" s="13"/>
+      <c r="N111" s="13"/>
+      <c r="O111" s="13"/>
+      <c r="P111" s="13"/>
+      <c r="Q111" s="13"/>
+      <c r="R111" s="13"/>
+      <c r="S111" s="13"/>
+      <c r="T111" s="13"/>
+      <c r="U111" s="13"/>
+      <c r="V111" s="13"/>
+      <c r="W111" s="13"/>
+      <c r="X111" s="13"/>
+      <c r="Y111" s="13"/>
+      <c r="Z111" s="13"/>
+      <c r="AA111" s="13"/>
+      <c r="AB111" s="13"/>
     </row>
     <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="B112" s="17"/>
-      <c r="C112" s="21" t="s">
-        <v>244</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="B112" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="C112" s="16"/>
       <c r="D112" s="16" t="s">
         <v>76</v>
       </c>
       <c r="E112" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="F112" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G112" s="30" t="n">
-        <v>0.1</v>
+        <v>243</v>
+      </c>
+      <c r="F112" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G112" s="23" t="n">
+        <v>25</v>
       </c>
       <c r="H112" s="24" t="s">
-        <v>246</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="I112" s="25"/>
+      <c r="J112" s="25"/>
+      <c r="K112" s="25"/>
+      <c r="L112" s="25"/>
+      <c r="M112" s="13"/>
+      <c r="N112" s="13"/>
+      <c r="O112" s="13"/>
+      <c r="P112" s="13"/>
+      <c r="Q112" s="13"/>
+      <c r="R112" s="13"/>
+      <c r="S112" s="13"/>
+      <c r="T112" s="13"/>
+      <c r="U112" s="13"/>
+      <c r="V112" s="13"/>
+      <c r="W112" s="13"/>
+      <c r="X112" s="13"/>
+      <c r="Y112" s="13"/>
+      <c r="Z112" s="13"/>
+      <c r="AA112" s="13"/>
+      <c r="AB112" s="13"/>
     </row>
     <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="16" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B113" s="17"/>
-      <c r="C113" s="21" t="s">
-        <v>248</v>
-      </c>
+      <c r="C113" s="17"/>
       <c r="D113" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E113" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="F113" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G113" s="19" t="n">
+        <v>13</v>
+      </c>
+      <c r="H113" s="20" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="B114" s="17"/>
+      <c r="C114" s="17"/>
+      <c r="D114" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E114" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="F114" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G114" s="30" t="n">
+        <v>43.95</v>
+      </c>
+      <c r="H114" s="20" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="B115" s="17"/>
+      <c r="C115" s="17"/>
+      <c r="D115" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E115" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="F115" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G115" s="19" t="n">
+        <v>15</v>
+      </c>
+      <c r="H115" s="20" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="B116" s="17"/>
+      <c r="C116" s="17"/>
+      <c r="D116" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="E116" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="F116" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G116" s="19" t="n">
+        <v>17</v>
+      </c>
+      <c r="H116" s="20" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="41" t="s">
+        <v>261</v>
+      </c>
+      <c r="B117" s="44"/>
+      <c r="C117" s="41"/>
+      <c r="D117" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="E117" s="41" t="s">
+        <v>262</v>
+      </c>
+      <c r="F117" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="G117" s="45" t="n">
+        <v>80</v>
+      </c>
+      <c r="H117" s="46" t="s">
+        <v>263</v>
+      </c>
+      <c r="I117" s="47"/>
+      <c r="J117" s="48"/>
+      <c r="K117" s="48"/>
+      <c r="L117" s="48"/>
+      <c r="M117" s="48"/>
+      <c r="N117" s="48"/>
+      <c r="O117" s="48"/>
+      <c r="P117" s="48"/>
+      <c r="Q117" s="48"/>
+      <c r="R117" s="48"/>
+      <c r="S117" s="48"/>
+      <c r="T117" s="48"/>
+      <c r="U117" s="48"/>
+      <c r="V117" s="48"/>
+      <c r="W117" s="48"/>
+      <c r="X117" s="48"/>
+      <c r="Y117" s="48"/>
+      <c r="Z117" s="42"/>
+      <c r="AA117" s="42"/>
+      <c r="AB117" s="42"/>
+    </row>
+    <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="26"/>
+    </row>
+    <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="27"/>
+      <c r="B119" s="27"/>
+      <c r="C119" s="27"/>
+      <c r="D119" s="27"/>
+      <c r="E119" s="27"/>
+      <c r="F119" s="27"/>
+      <c r="G119" s="27"/>
+      <c r="H119" s="27"/>
+      <c r="I119" s="27"/>
+      <c r="J119" s="27"/>
+      <c r="K119" s="27"/>
+      <c r="L119" s="27"/>
+      <c r="M119" s="27"/>
+      <c r="N119" s="27"/>
+      <c r="O119" s="27"/>
+      <c r="P119" s="27"/>
+      <c r="Q119" s="27"/>
+      <c r="R119" s="27"/>
+      <c r="S119" s="27"/>
+      <c r="T119" s="27"/>
+      <c r="U119" s="27"/>
+      <c r="V119" s="27"/>
+      <c r="W119" s="27"/>
+      <c r="X119" s="27"/>
+      <c r="Y119" s="27"/>
+      <c r="Z119" s="27"/>
+      <c r="AA119" s="27"/>
+      <c r="AB119" s="27"/>
+    </row>
+    <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="D120" s="11"/>
+    </row>
+    <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B121" s="13"/>
+      <c r="C121" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D121" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E121" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F121" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G121" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H121" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I121" s="13"/>
+      <c r="J121" s="13"/>
+      <c r="K121" s="13"/>
+      <c r="L121" s="13"/>
+      <c r="M121" s="13"/>
+      <c r="N121" s="13"/>
+      <c r="O121" s="13"/>
+      <c r="P121" s="13"/>
+      <c r="Q121" s="13"/>
+      <c r="R121" s="13"/>
+      <c r="S121" s="13"/>
+      <c r="T121" s="13"/>
+      <c r="U121" s="13"/>
+      <c r="V121" s="13"/>
+      <c r="W121" s="13"/>
+      <c r="X121" s="13"/>
+      <c r="Y121" s="13"/>
+      <c r="Z121" s="13"/>
+      <c r="AA121" s="13"/>
+      <c r="AB121" s="13"/>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="B122" s="17"/>
+      <c r="C122" s="17"/>
+      <c r="D122" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E122" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="F122" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G122" s="19" t="n">
+        <v>5</v>
+      </c>
+      <c r="H122" s="20" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="B123" s="17"/>
+      <c r="C123" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="D123" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="E113" s="17"/>
-      <c r="F113" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G113" s="30" t="n">
+      <c r="E123" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="F123" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G123" s="30" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="H123" s="24" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="B124" s="17"/>
+      <c r="C124" s="21" t="s">
+        <v>273</v>
+      </c>
+      <c r="D124" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E124" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="F124" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G124" s="30" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H124" s="24" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="B125" s="17"/>
+      <c r="C125" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="D125" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E125" s="17"/>
+      <c r="F125" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G125" s="30" t="n">
         <v>0.36</v>
       </c>
-      <c r="H113" s="24" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="114" s="46" customFormat="true" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="45" t="s">
+      <c r="H125" s="24" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="126" s="50" customFormat="true" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="C114" s="45" t="s">
-        <v>250</v>
-      </c>
-      <c r="D114" s="45" t="s">
-        <v>250</v>
-      </c>
-      <c r="E114" s="45" t="s">
-        <v>251</v>
-      </c>
-      <c r="F114" s="45" t="s">
-        <v>250</v>
-      </c>
-      <c r="G114" s="45" t="s">
-        <v>250</v>
-      </c>
-      <c r="H114" s="45" t="s">
-        <v>250</v>
-      </c>
-      <c r="J114" s="43"/>
-      <c r="K114" s="43"/>
-      <c r="L114" s="43"/>
-      <c r="M114" s="44"/>
-      <c r="N114" s="44"/>
-      <c r="O114" s="44"/>
-      <c r="P114" s="44"/>
-      <c r="Q114" s="44"/>
-      <c r="R114" s="44"/>
-      <c r="S114" s="44"/>
-      <c r="T114" s="44"/>
-      <c r="U114" s="44"/>
-      <c r="V114" s="44"/>
-      <c r="W114" s="44"/>
-      <c r="X114" s="44"/>
-      <c r="Y114" s="44"/>
-      <c r="Z114" s="44"/>
-      <c r="AA114" s="44"/>
-      <c r="AB114" s="44"/>
-    </row>
-    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="37" t="s">
-        <v>190</v>
-      </c>
-      <c r="B115" s="17"/>
-      <c r="C115" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="D115" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="E115" s="37" t="s">
-        <v>252</v>
-      </c>
-      <c r="F115" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="G115" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="H115" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="I115" s="38"/>
-      <c r="J115" s="38"/>
-      <c r="K115" s="38"/>
-      <c r="L115" s="38"/>
-      <c r="M115" s="38"/>
-      <c r="N115" s="38"/>
-      <c r="O115" s="38"/>
-      <c r="P115" s="38"/>
-      <c r="Q115" s="38"/>
-      <c r="R115" s="38"/>
-      <c r="S115" s="38"/>
-      <c r="T115" s="38"/>
-      <c r="U115" s="38"/>
-      <c r="V115" s="38"/>
-      <c r="W115" s="38"/>
-      <c r="X115" s="38"/>
-      <c r="Y115" s="38"/>
-      <c r="Z115" s="38"/>
-      <c r="AA115" s="38"/>
-      <c r="AB115" s="38"/>
-    </row>
-    <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="27"/>
-      <c r="B118" s="27"/>
-      <c r="C118" s="27"/>
-      <c r="D118" s="27"/>
-      <c r="E118" s="27"/>
-      <c r="F118" s="27"/>
-      <c r="G118" s="27"/>
-      <c r="H118" s="27"/>
-      <c r="I118" s="27"/>
-      <c r="J118" s="27"/>
-      <c r="K118" s="27"/>
-      <c r="L118" s="27"/>
-      <c r="M118" s="27"/>
-      <c r="N118" s="27"/>
-      <c r="O118" s="27"/>
-      <c r="P118" s="27"/>
-      <c r="Q118" s="27"/>
-      <c r="R118" s="27"/>
-      <c r="S118" s="27"/>
-      <c r="T118" s="27"/>
-      <c r="U118" s="27"/>
-      <c r="V118" s="27"/>
-      <c r="W118" s="27"/>
-      <c r="X118" s="27"/>
-      <c r="Y118" s="27"/>
-      <c r="Z118" s="27"/>
-      <c r="AA118" s="27"/>
-      <c r="AB118" s="27"/>
-    </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="C126" s="49" t="s">
+        <v>279</v>
+      </c>
+      <c r="D126" s="49" t="s">
+        <v>279</v>
+      </c>
+      <c r="E126" s="49" t="s">
+        <v>280</v>
+      </c>
+      <c r="F126" s="49" t="s">
+        <v>279</v>
+      </c>
+      <c r="G126" s="49" t="s">
+        <v>279</v>
+      </c>
+      <c r="H126" s="49" t="s">
+        <v>279</v>
+      </c>
+      <c r="J126" s="47"/>
+      <c r="K126" s="47"/>
+      <c r="L126" s="47"/>
+      <c r="M126" s="48"/>
+      <c r="N126" s="48"/>
+      <c r="O126" s="48"/>
+      <c r="P126" s="48"/>
+      <c r="Q126" s="48"/>
+      <c r="R126" s="48"/>
+      <c r="S126" s="48"/>
+      <c r="T126" s="48"/>
+      <c r="U126" s="48"/>
+      <c r="V126" s="48"/>
+      <c r="W126" s="48"/>
+      <c r="X126" s="48"/>
+      <c r="Y126" s="48"/>
+      <c r="Z126" s="48"/>
+      <c r="AA126" s="48"/>
+      <c r="AB126" s="48"/>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="41" t="s">
+        <v>219</v>
+      </c>
+      <c r="B127" s="17"/>
+      <c r="C127" s="41" t="s">
+        <v>220</v>
+      </c>
+      <c r="D127" s="41" t="s">
+        <v>220</v>
+      </c>
+      <c r="E127" s="41" t="s">
+        <v>281</v>
+      </c>
+      <c r="F127" s="41" t="s">
+        <v>220</v>
+      </c>
+      <c r="G127" s="41" t="s">
+        <v>220</v>
+      </c>
+      <c r="H127" s="41" t="s">
+        <v>220</v>
+      </c>
+      <c r="I127" s="42"/>
+      <c r="J127" s="42"/>
+      <c r="K127" s="42"/>
+      <c r="L127" s="42"/>
+      <c r="M127" s="42"/>
+      <c r="N127" s="42"/>
+      <c r="O127" s="42"/>
+      <c r="P127" s="42"/>
+      <c r="Q127" s="42"/>
+      <c r="R127" s="42"/>
+      <c r="S127" s="42"/>
+      <c r="T127" s="42"/>
+      <c r="U127" s="42"/>
+      <c r="V127" s="42"/>
+      <c r="W127" s="42"/>
+      <c r="X127" s="42"/>
+      <c r="Y127" s="42"/>
+      <c r="Z127" s="42"/>
+      <c r="AA127" s="42"/>
+      <c r="AB127" s="42"/>
+    </row>
+    <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="27"/>
+      <c r="B130" s="27"/>
+      <c r="C130" s="27"/>
+      <c r="D130" s="27"/>
+      <c r="E130" s="27"/>
+      <c r="F130" s="27"/>
+      <c r="G130" s="27"/>
+      <c r="H130" s="27"/>
+      <c r="I130" s="27"/>
+      <c r="J130" s="27"/>
+      <c r="K130" s="27"/>
+      <c r="L130" s="27"/>
+      <c r="M130" s="27"/>
+      <c r="N130" s="27"/>
+      <c r="O130" s="27"/>
+      <c r="P130" s="27"/>
+      <c r="Q130" s="27"/>
+      <c r="R130" s="27"/>
+      <c r="S130" s="27"/>
+      <c r="T130" s="27"/>
+      <c r="U130" s="27"/>
+      <c r="V130" s="27"/>
+      <c r="W130" s="27"/>
+      <c r="X130" s="27"/>
+      <c r="Y130" s="27"/>
+      <c r="Z130" s="27"/>
+      <c r="AA130" s="27"/>
+      <c r="AB130" s="27"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H7" r:id="rId1" display="https://www.horizonhobby.com/blackjack-24-inch-catamaran-brushless%3A-rtr-prb08007"/>
@@ -4689,37 +5073,42 @@
     <hyperlink ref="H56" r:id="rId32" display="https://www.atlas-scientific.com/product_pages/components/single_carrier_iso.html"/>
     <hyperlink ref="H57" r:id="rId33" display="https://www.hach.com/ph-buffer-solution-kit-color-coded-ph-4-01-ph-7-00-and-ph-10-01-500-ml-each/product?id=7640205069"/>
     <hyperlink ref="H58" r:id="rId34" display="https://www.hach.com/electrolyte-solution-kcl-3m-50ml/product-parameter-reagent?id=7640207762"/>
-    <hyperlink ref="H66" r:id="rId35" display="https://www.digikey.com/product-detail/en/yageo/AT0603FRE0710KL/YAG2122CT-ND/5139570"/>
-    <hyperlink ref="H67" r:id="rId36" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP0603FTD2K74/RNCP0603FTD2K74CT-ND/2240457"/>
-    <hyperlink ref="H68" r:id="rId37" display="https://www.digikey.com/product-detail/en/yageo/RT0603BRD071ML/YAG4498CT-ND/6616654"/>
-    <hyperlink ref="H69" r:id="rId38" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP0603FTD1K00/RNCP0603FTD1K00CT-ND/2240445"/>
-    <hyperlink ref="H70" r:id="rId39" display="https://www.digikey.com/product-detail/en/yageo/RT0603BRD0742K2L/YAG4556CT-ND/6616712"/>
-    <hyperlink ref="H71" r:id="rId40" display="https://www.digikey.com/product-detail/en/yageo/RT0603DRE071K2L/311-2461-1-ND/6128880"/>
-    <hyperlink ref="H72" r:id="rId41" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X8R1H104K080AB/445-8818-1-ND/3248223"/>
-    <hyperlink ref="H73" r:id="rId42" display="https://www.digikey.com/products/en?keywords=641-1331-1-ND"/>
-    <hyperlink ref="H74" r:id="rId43" display="https://www.digikey.com/product-detail/en/texas-instruments/TLE2426CD/296-6547-5-ND/371934"/>
-    <hyperlink ref="H75" r:id="rId44" display="https://www.digikey.com/product-detail/en/analog-devices-inc/AD8655ARZ-REEL7/AD8655ARZ-REEL7CT-ND/3678589"/>
-    <hyperlink ref="H76" r:id="rId45" display="https://www.digikey.com/product-detail/en/texas-instruments/TLV2374IDR/296-11967-1-ND/390435"/>
-    <hyperlink ref="H77" r:id="rId46" display="https://www.digikey.com/product-detail/en/AYZ0202AGRLC/401-2013-1-ND/1640122"/>
-    <hyperlink ref="H79" r:id="rId47" display="https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2117A.12.06/C2117G-100-ND/16217"/>
-    <hyperlink ref="H80" r:id="rId48" display="https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2004A.12.02/C2004W-100-ND/57495"/>
-    <hyperlink ref="H86" r:id="rId49" display="https://www.amazon.com/gp/product/B01F2R2EPE/"/>
-    <hyperlink ref="H87" r:id="rId50" display="https://www.amazon.com/gp/product/B01F7L9QD8/"/>
-    <hyperlink ref="H92" r:id="rId51" display="https://www.digikey.com/product-detail/en/vishay-semiconductor-opto-division/VSMY2850G/VSMY2850GCT-ND/2615293"/>
-    <hyperlink ref="H93" r:id="rId52" display="https://www.digikey.com/product-detail/en/ams/TSL237T/TSL237-TCT-ND/3095287"/>
-    <hyperlink ref="H94" r:id="rId53" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X8R1H104K080AB/445-8818-1-ND/3248223"/>
-    <hyperlink ref="H95" r:id="rId54" display="https://www.digikey.com/product-detail/en/yageo/RT0603DRD07200RL/311-200DCT-ND/1035740"/>
-    <hyperlink ref="H98" r:id="rId55" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-BK005/422010-BK005-ND/3705786"/>
-    <hyperlink ref="H99" r:id="rId56" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-RD005/422010-RD005-ND/4935160"/>
-    <hyperlink ref="H100" r:id="rId57" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-SL005/422010-SL005-ND/4935161"/>
-    <hyperlink ref="H101" r:id="rId58" display="https://www.amazon.com/Source-One-LLC-Acrylic-Plexiglass/dp/B06XNXHKQN/"/>
-    <hyperlink ref="H102" r:id="rId59" location="product-description-iframe" display="https://www.amazon.com/MG-Chemicals-Thermally-Conductive-Encapsulating/dp/B008UH4CRM#product-description-iframe"/>
-    <hyperlink ref="H103" r:id="rId60" display="https://www.amazon.com/CRC-SL2512-Soluble-Oil-32/dp/B000M8O010/"/>
-    <hyperlink ref="H104" r:id="rId61" display="https://www.discountvials.com/6-dram-glass-vial-w-cap/"/>
-    <hyperlink ref="H105" r:id="rId62" display="http://www.hach.com/formazin-turbidity-standard-4000-ntu-500-ml/product?id=7640455437"/>
-    <hyperlink ref="H111" r:id="rId63" display="https://www.digikey.com/product-detail/en/microchip-technology/AT30TS750A-SS8M-T/1611-AT30TS750A-SS8M-TCT-ND/6831450"/>
-    <hyperlink ref="H112" r:id="rId64" display="http://www.digikey.com/product-detail/en/RC1206FR-0710KL/311-10.0KFRCT-ND/731430"/>
-    <hyperlink ref="H113" r:id="rId65" display="https://www.digikey.com/product-detail/en/avx-corporation/1206VC104KAT2A/478-5724-1-ND/2136332"/>
+    <hyperlink ref="H63" r:id="rId35" display="https://www.mcmaster.com/8972T11"/>
+    <hyperlink ref="H64" r:id="rId36" display="https://www.mcmaster.com/4339T5"/>
+    <hyperlink ref="H71" r:id="rId37" display="https://www.digikey.com/product-detail/en/yageo/AT0603FRE0710KL/YAG2122CT-ND/5139570"/>
+    <hyperlink ref="H72" r:id="rId38" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP0603FTD2K74/RNCP0603FTD2K74CT-ND/2240457"/>
+    <hyperlink ref="H73" r:id="rId39" display="https://www.digikey.com/product-detail/en/yageo/RT0603BRD071ML/YAG4498CT-ND/6616654"/>
+    <hyperlink ref="H74" r:id="rId40" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP0603FTD1K00/RNCP0603FTD1K00CT-ND/2240445"/>
+    <hyperlink ref="H75" r:id="rId41" display="https://www.digikey.com/product-detail/en/yageo/RT0603BRD0742K2L/YAG4556CT-ND/6616712"/>
+    <hyperlink ref="H76" r:id="rId42" display="https://www.digikey.com/product-detail/en/yageo/RT0603DRE071K2L/311-2461-1-ND/6128880"/>
+    <hyperlink ref="H77" r:id="rId43" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X8R1H104K080AB/445-8818-1-ND/3248223"/>
+    <hyperlink ref="H78" r:id="rId44" display="https://www.digikey.com/products/en?keywords=641-1331-1-ND"/>
+    <hyperlink ref="H79" r:id="rId45" display="https://www.digikey.com/product-detail/en/texas-instruments/TLE2426CD/296-6547-5-ND/371934"/>
+    <hyperlink ref="H80" r:id="rId46" display="https://www.digikey.com/product-detail/en/analog-devices-inc/AD8655ARZ-REEL7/AD8655ARZ-REEL7CT-ND/3678589"/>
+    <hyperlink ref="H81" r:id="rId47" display="https://www.digikey.com/product-detail/en/texas-instruments/TLV2374IDR/296-11967-1-ND/390435"/>
+    <hyperlink ref="H82" r:id="rId48" display="https://www.digikey.com/product-detail/en/AYZ0202AGRLC/401-2013-1-ND/1640122"/>
+    <hyperlink ref="H84" r:id="rId49" display="https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2117A.12.06/C2117G-100-ND/16217"/>
+    <hyperlink ref="H85" r:id="rId50" display="https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2004A.12.02/C2004W-100-ND/57495"/>
+    <hyperlink ref="H86" r:id="rId51" display="https://www.digikey.com/products/en?keywords=%09WM4800-ND"/>
+    <hyperlink ref="H87" r:id="rId52" display="https://www.digikey.com/products/en?keywords=WM2900-ND%E2%80%8E"/>
+    <hyperlink ref="H93" r:id="rId53" display="https://www.amazon.com/gp/product/B01IBOK7FE/"/>
+    <hyperlink ref="H98" r:id="rId54" display="https://www.amazon.com/gp/product/B01F2R2EPE/"/>
+    <hyperlink ref="H99" r:id="rId55" display="https://www.amazon.com/gp/product/B01F7L9QD8/"/>
+    <hyperlink ref="H104" r:id="rId56" display="https://www.digikey.com/product-detail/en/vishay-semiconductor-opto-division/VSMY2850G/VSMY2850GCT-ND/2615293"/>
+    <hyperlink ref="H105" r:id="rId57" display="https://www.digikey.com/product-detail/en/ams/TSL237T/TSL237-TCT-ND/3095287"/>
+    <hyperlink ref="H106" r:id="rId58" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X8R1H104K080AB/445-8818-1-ND/3248223"/>
+    <hyperlink ref="H107" r:id="rId59" display="https://www.digikey.com/product-detail/en/yageo/RT0603DRD07200RL/311-200DCT-ND/1035740"/>
+    <hyperlink ref="H110" r:id="rId60" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-BK005/422010-BK005-ND/3705786"/>
+    <hyperlink ref="H111" r:id="rId61" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-RD005/422010-RD005-ND/4935160"/>
+    <hyperlink ref="H112" r:id="rId62" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-SL005/422010-SL005-ND/4935161"/>
+    <hyperlink ref="H113" r:id="rId63" display="https://www.amazon.com/Source-One-LLC-Acrylic-Plexiglass/dp/B06XNXHKQN/"/>
+    <hyperlink ref="H114" r:id="rId64" location="product-description-iframe" display="https://www.amazon.com/MG-Chemicals-Thermally-Conductive-Encapsulating/dp/B008UH4CRM#product-description-iframe"/>
+    <hyperlink ref="H115" r:id="rId65" display="https://www.amazon.com/CRC-SL2512-Soluble-Oil-32/dp/B000M8O010/"/>
+    <hyperlink ref="H116" r:id="rId66" display="https://www.discountvials.com/6-dram-glass-vial-w-cap/"/>
+    <hyperlink ref="H117" r:id="rId67" display="http://www.hach.com/formazin-turbidity-standard-4000-ntu-500-ml/product?id=7640455437"/>
+    <hyperlink ref="H123" r:id="rId68" display="https://www.digikey.com/product-detail/en/microchip-technology/AT30TS750A-SS8M-T/1611-AT30TS750A-SS8M-TCT-ND/6831450"/>
+    <hyperlink ref="H124" r:id="rId69" display="http://www.digikey.com/product-detail/en/RC1206FR-0710KL/311-10.0KFRCT-ND/731430"/>
+    <hyperlink ref="H125" r:id="rId70" display="https://www.digikey.com/product-detail/en/avx-corporation/1206VC104KAT2A/478-5724-1-ND/2136332"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4754,122 +5143,122 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="26" t="s">
-        <v>253</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="G3" s="47" t="s">
-        <v>255</v>
+        <v>283</v>
+      </c>
+      <c r="G3" s="51" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>256</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="26" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="26" t="s">
-        <v>258</v>
-      </c>
-      <c r="D7" s="48" t="s">
-        <v>259</v>
+        <v>287</v>
+      </c>
+      <c r="D7" s="52" t="s">
+        <v>288</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>260</v>
+        <v>289</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>261</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="26" t="s">
-        <v>262</v>
-      </c>
-      <c r="D8" s="48" t="s">
-        <v>263</v>
+        <v>291</v>
+      </c>
+      <c r="D8" s="52" t="s">
+        <v>292</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>264</v>
+        <v>293</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="26" t="s">
-        <v>265</v>
-      </c>
-      <c r="D9" s="48" t="s">
-        <v>266</v>
+        <v>294</v>
+      </c>
+      <c r="D9" s="52" t="s">
+        <v>295</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>264</v>
+        <v>293</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>267</v>
-      </c>
-      <c r="G9" s="49" t="s">
+        <v>296</v>
+      </c>
+      <c r="G9" s="53" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="26" t="s">
-        <v>268</v>
-      </c>
-      <c r="D10" s="48" t="s">
-        <v>269</v>
+        <v>297</v>
+      </c>
+      <c r="D10" s="52" t="s">
+        <v>298</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>270</v>
+        <v>299</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>271</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="26" t="s">
-        <v>272</v>
-      </c>
-      <c r="D11" s="48" t="s">
-        <v>273</v>
+        <v>301</v>
+      </c>
+      <c r="D11" s="52" t="s">
+        <v>302</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>260</v>
+        <v>289</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>274</v>
+        <v>303</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>275</v>
+        <v>304</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="48" t="s">
-        <v>276</v>
+      <c r="D13" s="52" t="s">
+        <v>305</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>277</v>
+        <v>306</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="48" t="s">
-        <v>278</v>
+      <c r="D14" s="52" t="s">
+        <v>307</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>279</v>
+        <v>308</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="48" t="s">
-        <v>280</v>
+      <c r="D15" s="52" t="s">
+        <v>309</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>281</v>
+        <v>310</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4877,50 +5266,50 @@
       <c r="E16" s="26"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="48" t="s">
-        <v>282</v>
+      <c r="D17" s="52" t="s">
+        <v>311</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>283</v>
+        <v>312</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E18" s="50" t="s">
-        <v>284</v>
+      <c r="E18" s="54" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E19" s="26" t="s">
-        <v>285</v>
+        <v>314</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="26" t="s">
-        <v>286</v>
-      </c>
-      <c r="D20" s="48" t="s">
-        <v>287</v>
-      </c>
-      <c r="E20" s="50" t="s">
-        <v>288</v>
+        <v>315</v>
+      </c>
+      <c r="D20" s="52" t="s">
+        <v>316</v>
+      </c>
+      <c r="E20" s="54" t="s">
+        <v>317</v>
       </c>
       <c r="F20" s="26" t="s">
-        <v>289</v>
+        <v>318</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>290</v>
+        <v>319</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="s">
-        <v>291</v>
+        <v>320</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="13" t="s">
-        <v>292</v>
+        <v>321</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>112</v>
@@ -4928,14 +5317,14 @@
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
-      <c r="F28" s="51" t="n">
-        <v>1</v>
-      </c>
-      <c r="G28" s="51" t="n">
+      <c r="F28" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="G28" s="55" t="n">
         <v>16</v>
       </c>
-      <c r="H28" s="52" t="s">
-        <v>293</v>
+      <c r="H28" s="56" t="s">
+        <v>322</v>
       </c>
       <c r="I28" s="25"/>
       <c r="J28" s="25"/>
@@ -4960,7 +5349,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="13" t="s">
-        <v>294</v>
+        <v>323</v>
       </c>
       <c r="B29" s="13" t="s">
         <v>112</v>
@@ -4968,14 +5357,14 @@
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
-      <c r="F29" s="51" t="n">
-        <v>1</v>
-      </c>
-      <c r="G29" s="51" t="n">
+      <c r="F29" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="55" t="n">
         <v>16</v>
       </c>
-      <c r="H29" s="52" t="s">
-        <v>295</v>
+      <c r="H29" s="56" t="s">
+        <v>324</v>
       </c>
       <c r="I29" s="25"/>
       <c r="J29" s="25"/>
@@ -5000,7 +5389,7 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="13" t="s">
-        <v>296</v>
+        <v>325</v>
       </c>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -5010,14 +5399,14 @@
       <c r="E30" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F30" s="51" t="n">
+      <c r="F30" s="55" t="n">
         <v>4</v>
       </c>
-      <c r="G30" s="53" t="n">
+      <c r="G30" s="57" t="n">
         <v>0.5</v>
       </c>
-      <c r="H30" s="52" t="s">
-        <v>297</v>
+      <c r="H30" s="56" t="s">
+        <v>326</v>
       </c>
       <c r="I30" s="25"/>
       <c r="J30" s="13"/>
@@ -5042,7 +5431,7 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="13" t="s">
-        <v>298</v>
+        <v>327</v>
       </c>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -5050,14 +5439,14 @@
         <v>45</v>
       </c>
       <c r="E31" s="13"/>
-      <c r="F31" s="51" t="n">
+      <c r="F31" s="55" t="n">
         <v>4</v>
       </c>
-      <c r="G31" s="53" t="n">
+      <c r="G31" s="57" t="n">
         <v>1.5</v>
       </c>
-      <c r="H31" s="52" t="s">
-        <v>299</v>
+      <c r="H31" s="56" t="s">
+        <v>328</v>
       </c>
       <c r="I31" s="25"/>
       <c r="J31" s="13"/>
@@ -5082,7 +5471,7 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="13" t="s">
-        <v>300</v>
+        <v>329</v>
       </c>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -5090,16 +5479,16 @@
         <v>64</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>301</v>
-      </c>
-      <c r="F35" s="51" t="n">
-        <v>1</v>
-      </c>
-      <c r="G35" s="54" t="n">
+        <v>330</v>
+      </c>
+      <c r="F35" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" s="58" t="n">
         <v>31</v>
       </c>
-      <c r="H35" s="52" t="s">
-        <v>302</v>
+      <c r="H35" s="56" t="s">
+        <v>331</v>
       </c>
       <c r="J35" s="25"/>
       <c r="K35" s="25"/>
@@ -5123,99 +5512,99 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="26" t="s">
-        <v>303</v>
+        <v>332</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>304</v>
+        <v>333</v>
       </c>
       <c r="E36" s="26" t="s">
-        <v>305</v>
+        <v>334</v>
       </c>
       <c r="F36" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="G36" s="55" t="n">
+      <c r="G36" s="59" t="n">
         <v>8</v>
       </c>
-      <c r="H36" s="48" t="s">
-        <v>306</v>
+      <c r="H36" s="52" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="26" t="s">
-        <v>307</v>
+        <v>336</v>
       </c>
       <c r="D37" s="26" t="s">
         <v>64</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>308</v>
+        <v>337</v>
       </c>
       <c r="F37" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="G37" s="55" t="n">
+      <c r="G37" s="59" t="n">
         <v>27</v>
       </c>
-      <c r="H37" s="48" t="s">
-        <v>309</v>
+      <c r="H37" s="52" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="26" t="s">
-        <v>310</v>
+        <v>339</v>
       </c>
       <c r="D38" s="26" t="s">
         <v>64</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>311</v>
+        <v>340</v>
       </c>
       <c r="F38" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="G38" s="55" t="n">
+      <c r="G38" s="59" t="n">
         <v>25</v>
       </c>
-      <c r="H38" s="48" t="s">
-        <v>312</v>
+      <c r="H38" s="52" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="26" t="s">
-        <v>313</v>
+        <v>342</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>314</v>
+        <v>343</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>315</v>
+        <v>344</v>
       </c>
       <c r="F39" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="G39" s="55" t="n">
+      <c r="G39" s="59" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="26" t="s">
-        <v>316</v>
+        <v>345</v>
       </c>
       <c r="D40" s="26" t="s">
         <v>64</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>317</v>
+        <v>346</v>
       </c>
       <c r="F40" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="G40" s="55" t="n">
+      <c r="G40" s="59" t="n">
         <v>10</v>
       </c>
-      <c r="H40" s="48" t="s">
-        <v>318</v>
+      <c r="H40" s="52" t="s">
+        <v>347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update conductivity headers, add 3D print parts and laser cut parts
</commit_message>
<xml_diff>
--- a/hardware/SeeBoat_fullPartsList.xlsx
+++ b/hardware/SeeBoat_fullPartsList.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="349">
   <si>
     <t xml:space="preserve">Parts list for SeeBoat &amp; full sensor suite</t>
   </si>
@@ -32,6 +32,9 @@
     <t xml:space="preserve">updated June 2019</t>
   </si>
   <si>
+    <t xml:space="preserve">updated July 2019</t>
+  </si>
+  <si>
     <t xml:space="preserve">BOAT</t>
   </si>
   <si>
@@ -242,7 +245,7 @@
     <t xml:space="preserve">connects to all sensors</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.dropbox.com/s/5kwn3nz447jgal9/controlBoard-0.5.brd?dl=0</t>
+    <t xml:space="preserve">https://github.com/lperovich/seeboat/tree/master/hardware/controlBoard</t>
   </si>
   <si>
     <t xml:space="preserve">resistor SMD 0603 2.7K</t>
@@ -506,7 +509,7 @@
     <t xml:space="preserve">custom conductivity board</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.dropbox.com/s/1nyp3by1tbcasan/conductivity.brd?dl=0</t>
+    <t xml:space="preserve">https://github.com/lperovich/seeboat/tree/master/hardware/conductivity</t>
   </si>
   <si>
     <t xml:space="preserve">resistor 10K, 0603</t>
@@ -632,10 +635,10 @@
     <t xml:space="preserve">Molex 2 pin header (male)</t>
   </si>
   <si>
-    <t xml:space="preserve">WM2900-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/products/en?keywords=WM2900-ND%E2%80%8E</t>
+    <t xml:space="preserve">WM24819-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/products/en?keywords=WM24819-ND</t>
   </si>
   <si>
     <t xml:space="preserve">3D printed probe</t>
@@ -737,13 +740,13 @@
     <t xml:space="preserve">custom light to freq board</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.dropbox.com/s/5wtg2gff6oehxno/turbiditySensor.brd?dl=0</t>
+    <t xml:space="preserve">https://github.com/lperovich/seeboat/tree/master/hardware/turbiditySensor</t>
   </si>
   <si>
     <t xml:space="preserve">custom LED board</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.dropbox.com/s/f1dnld6ux556wln/turbidityLED.brd?dl=0</t>
+    <t xml:space="preserve">https://github.com/lperovich/seeboat/tree/master/hardware/turbidityLED</t>
   </si>
   <si>
     <t xml:space="preserve">wire-black, stranded</t>
@@ -824,7 +827,7 @@
     <t xml:space="preserve">custom temperature board</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.dropbox.com/s/a62454o26l9r3ev/temperatureSensor.brd?dl=0</t>
+    <t xml:space="preserve">https://github.com/lperovich/seeboat/tree/master/hardware/temperatureSensor</t>
   </si>
   <si>
     <t xml:space="preserve">digital temperature sensor</t>
@@ -1174,6 +1177,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
@@ -1181,14 +1192,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -1496,6 +1499,10 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1504,7 +1511,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1516,19 +1523,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1696,7 +1699,7 @@
   <dimension ref="A1:AB130"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1734,7 +1737,9 @@
         <v>2</v>
       </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="D3" s="8" t="s">
+        <v>3</v>
+      </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -1743,32 +1748,32 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
@@ -1793,17 +1798,17 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F7" s="16" t="n">
         <v>1</v>
@@ -1812,20 +1817,20 @@
         <v>230</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F8" s="16" t="n">
         <v>1</v>
@@ -1834,20 +1839,20 @@
         <v>50</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F9" s="16" t="n">
         <v>1</v>
@@ -1856,20 +1861,20 @@
         <v>7</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F10" s="16" t="n">
         <v>1</v>
@@ -1878,20 +1883,20 @@
         <v>8</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F11" s="22" t="n">
         <v>3</v>
@@ -1900,7 +1905,7 @@
         <v>15</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I11" s="25"/>
       <c r="J11" s="25"/>
@@ -1925,15 +1930,15 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
       <c r="D12" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F12" s="16" t="n">
         <v>1</v>
@@ -1942,20 +1947,20 @@
         <v>10</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
       <c r="D13" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F13" s="16" t="n">
         <v>1</v>
@@ -1964,7 +1969,7 @@
         <v>7</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1979,15 +1984,15 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
       <c r="D15" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F15" s="16" t="n">
         <v>1</v>
@@ -1996,20 +2001,20 @@
         <v>46</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="D16" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F16" s="16" t="n">
         <v>1</v>
@@ -2018,20 +2023,20 @@
         <v>126</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F17" s="16" t="n">
         <v>1</v>
@@ -2040,7 +2045,7 @@
         <v>160</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2079,32 +2084,32 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D20" s="11"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
@@ -2129,15 +2134,15 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F22" s="22" t="n">
         <v>1</v>
@@ -2146,7 +2151,7 @@
         <v>35</v>
       </c>
       <c r="H22" s="28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I22" s="28"/>
       <c r="J22" s="13"/>
@@ -2171,15 +2176,15 @@
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F23" s="22" t="n">
         <v>1</v>
@@ -2188,7 +2193,7 @@
         <v>40</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I23" s="28"/>
       <c r="J23" s="13"/>
@@ -2213,15 +2218,15 @@
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F24" s="22" t="n">
         <v>1</v>
@@ -2230,7 +2235,7 @@
         <v>1</v>
       </c>
       <c r="H24" s="24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I24" s="28"/>
       <c r="J24" s="13"/>
@@ -2255,15 +2260,15 @@
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F25" s="22" t="n">
         <v>1</v>
@@ -2272,7 +2277,7 @@
         <v>3</v>
       </c>
       <c r="H25" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I25" s="28"/>
       <c r="J25" s="13"/>
@@ -2297,15 +2302,15 @@
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F26" s="22" t="n">
         <v>4</v>
@@ -2314,7 +2319,7 @@
         <v>1.25</v>
       </c>
       <c r="H26" s="24" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I26" s="28"/>
       <c r="J26" s="13"/>
@@ -2339,15 +2344,15 @@
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F27" s="22" t="n">
         <v>4</v>
@@ -2356,7 +2361,7 @@
         <v>1</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I27" s="28"/>
       <c r="J27" s="13"/>
@@ -2381,15 +2386,15 @@
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
       <c r="D28" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F28" s="22" t="n">
         <v>1</v>
@@ -2398,7 +2403,7 @@
         <v>5.59</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I28" s="28"/>
       <c r="J28" s="13"/>
@@ -2423,15 +2428,15 @@
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
       <c r="D29" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F29" s="22" t="n">
         <v>1</v>
@@ -2440,7 +2445,7 @@
         <v>15</v>
       </c>
       <c r="H29" s="24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I29" s="16"/>
       <c r="J29" s="13"/>
@@ -2472,17 +2477,17 @@
       <c r="H30" s="16"/>
       <c r="I30" s="17"/>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
       <c r="D31" s="16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F31" s="16" t="n">
         <v>1</v>
@@ -2490,74 +2495,74 @@
       <c r="G31" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="H31" s="20" t="s">
-        <v>73</v>
+      <c r="H31" s="30" t="s">
+        <v>74</v>
       </c>
       <c r="I31" s="17"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B32" s="17"/>
       <c r="C32" s="21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F32" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="G32" s="30" t="n">
+      <c r="G32" s="31" t="n">
         <v>0.1</v>
       </c>
       <c r="H32" s="20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I32" s="17"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B33" s="17"/>
       <c r="C33" s="21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F33" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="G33" s="30" t="n">
+      <c r="G33" s="31" t="n">
         <v>0.1</v>
       </c>
       <c r="H33" s="20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I33" s="17"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F34" s="16" t="n">
         <v>1</v>
@@ -2566,177 +2571,177 @@
         <v>1.07</v>
       </c>
       <c r="H34" s="20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I34" s="17"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B35" s="17"/>
       <c r="C35" s="21" t="n">
         <v>2343</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F35" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="G35" s="30" t="n">
+      <c r="G35" s="31" t="n">
         <v>4.5</v>
       </c>
       <c r="H35" s="20" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I35" s="17"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B36" s="17"/>
       <c r="C36" s="21" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F36" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="G36" s="30" t="n">
+      <c r="G36" s="31" t="n">
         <v>0.94</v>
       </c>
       <c r="H36" s="20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I36" s="17"/>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="16" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B37" s="17"/>
       <c r="C37" s="21" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F37" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="G37" s="30" t="n">
+      <c r="G37" s="31" t="n">
         <v>1.46</v>
       </c>
       <c r="H37" s="20" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I37" s="17"/>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B38" s="17"/>
       <c r="C38" s="21" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F38" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="G38" s="30" t="n">
+      <c r="G38" s="31" t="n">
         <v>0.87</v>
       </c>
       <c r="H38" s="20" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I38" s="17"/>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="16" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B39" s="17"/>
       <c r="C39" s="21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F39" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="G39" s="30" t="n">
+      <c r="G39" s="31" t="n">
         <v>0.99</v>
       </c>
       <c r="H39" s="20" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I39" s="17"/>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B40" s="17"/>
       <c r="C40" s="21" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F40" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="G40" s="30" t="n">
+      <c r="G40" s="31" t="n">
         <v>95.15</v>
       </c>
       <c r="H40" s="20" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F41" s="22" t="n">
         <v>1</v>
@@ -2745,7 +2750,7 @@
         <v>16</v>
       </c>
       <c r="H41" s="24" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I41" s="28"/>
       <c r="J41" s="25"/>
@@ -2800,32 +2805,32 @@
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D44" s="11"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B45" s="13"/>
       <c r="C45" s="12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H45" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I45" s="13"/>
       <c r="J45" s="13"/>
@@ -2850,15 +2855,15 @@
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="28" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B46" s="28"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F46" s="22" t="n">
         <v>1</v>
@@ -2867,7 +2872,7 @@
         <v>30</v>
       </c>
       <c r="H46" s="24" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J46" s="13"/>
       <c r="K46" s="13"/>
@@ -2891,15 +2896,15 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="28" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B47" s="28"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F47" s="22" t="n">
         <v>1</v>
@@ -2931,15 +2936,15 @@
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="16" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
       <c r="D48" s="16" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F48" s="16" t="n">
         <v>1</v>
@@ -2948,7 +2953,7 @@
         <v>10</v>
       </c>
       <c r="H48" s="20" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2989,32 +2994,32 @@
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D52" s="11"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B53" s="13"/>
       <c r="C53" s="12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G53" s="15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H53" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I53" s="13"/>
       <c r="J53" s="13"/>
@@ -3039,15 +3044,15 @@
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="16" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B54" s="16"/>
       <c r="C54" s="16"/>
       <c r="D54" s="16" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F54" s="22" t="n">
         <v>1</v>
@@ -3056,7 +3061,7 @@
         <v>38</v>
       </c>
       <c r="H54" s="24" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I54" s="25"/>
       <c r="J54" s="13"/>
@@ -3079,15 +3084,15 @@
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="16" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B55" s="16"/>
       <c r="C55" s="16"/>
       <c r="D55" s="16" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E55" s="16" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F55" s="22" t="n">
         <v>1</v>
@@ -3096,7 +3101,7 @@
         <v>72</v>
       </c>
       <c r="H55" s="24" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I55" s="25"/>
       <c r="J55" s="13"/>
@@ -3119,15 +3124,15 @@
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="16" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B56" s="16"/>
       <c r="C56" s="16"/>
       <c r="D56" s="16" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F56" s="22" t="n">
         <v>1</v>
@@ -3136,7 +3141,7 @@
         <v>40</v>
       </c>
       <c r="H56" s="24" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I56" s="25"/>
       <c r="J56" s="25"/>
@@ -3159,15 +3164,15 @@
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="16" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B57" s="17"/>
       <c r="C57" s="17"/>
       <c r="D57" s="16" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E57" s="16" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F57" s="16" t="n">
         <v>1</v>
@@ -3176,20 +3181,20 @@
         <v>30</v>
       </c>
       <c r="H57" s="20" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="16" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B58" s="17"/>
       <c r="C58" s="17"/>
       <c r="D58" s="16" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E58" s="16" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F58" s="16" t="n">
         <v>1</v>
@@ -3198,7 +3203,7 @@
         <v>12</v>
       </c>
       <c r="H58" s="20" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3213,15 +3218,15 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="16" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B60" s="17"/>
       <c r="C60" s="17"/>
       <c r="D60" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E60" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F60" s="17" t="n">
         <v>2</v>
@@ -3233,15 +3238,15 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="16" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B61" s="17"/>
       <c r="C61" s="17"/>
       <c r="D61" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E61" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F61" s="17" t="n">
         <v>2</v>
@@ -3253,15 +3258,15 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B62" s="17"/>
       <c r="C62" s="17"/>
       <c r="D62" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E62" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F62" s="17" t="n">
         <v>4</v>
@@ -3273,15 +3278,15 @@
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="16" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B63" s="17"/>
       <c r="C63" s="17"/>
       <c r="D63" s="17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E63" s="17" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F63" s="17" t="n">
         <v>1</v>
@@ -3289,21 +3294,21 @@
       <c r="G63" s="19" t="n">
         <v>0.55</v>
       </c>
-      <c r="H63" s="31" t="s">
-        <v>153</v>
+      <c r="H63" s="32" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="16" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B64" s="17"/>
       <c r="C64" s="17"/>
       <c r="D64" s="17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E64" s="17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F64" s="17" t="n">
         <v>1</v>
@@ -3311,19 +3316,19 @@
       <c r="G64" s="19" t="n">
         <v>0.9</v>
       </c>
-      <c r="H64" s="31" t="s">
-        <v>156</v>
+      <c r="H64" s="32" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="16" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B65" s="17"/>
       <c r="C65" s="17"/>
       <c r="D65" s="17"/>
       <c r="E65" s="17" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F65" s="17" t="n">
         <v>1</v>
@@ -3368,31 +3373,31 @@
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="10" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B69" s="13"/>
       <c r="C69" s="12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E69" s="12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F69" s="14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G69" s="15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H69" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I69" s="13"/>
       <c r="J69" s="13"/>
@@ -3415,66 +3420,66 @@
       <c r="AA69" s="13"/>
       <c r="AB69" s="13"/>
     </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="16" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C70" s="17"/>
       <c r="D70" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E70" s="32"/>
+        <v>72</v>
+      </c>
+      <c r="E70" s="33"/>
       <c r="F70" s="16" t="n">
         <v>1</v>
       </c>
       <c r="G70" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="H70" s="20" t="s">
-        <v>161</v>
+      <c r="H70" s="30" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C71" s="21" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D71" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E71" s="17"/>
       <c r="F71" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="G71" s="30" t="n">
+      <c r="G71" s="31" t="n">
         <v>0.17</v>
       </c>
       <c r="H71" s="20" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B72" s="13"/>
       <c r="C72" s="21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D72" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E72" s="16"/>
       <c r="F72" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="G72" s="30" t="n">
+      <c r="G72" s="31" t="n">
         <v>0.1</v>
       </c>
-      <c r="H72" s="33" t="s">
-        <v>166</v>
+      <c r="H72" s="34" t="s">
+        <v>167</v>
       </c>
       <c r="I72" s="13"/>
       <c r="J72" s="13"/>
@@ -3499,14 +3504,14 @@
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="16" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B73" s="13"/>
       <c r="C73" s="21" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D73" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E73" s="16"/>
       <c r="F73" s="22" t="n">
@@ -3515,8 +3520,8 @@
       <c r="G73" s="29" t="n">
         <v>0.34</v>
       </c>
-      <c r="H73" s="33" t="s">
-        <v>169</v>
+      <c r="H73" s="34" t="s">
+        <v>170</v>
       </c>
       <c r="I73" s="13"/>
       <c r="J73" s="13"/>
@@ -3541,24 +3546,24 @@
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="16" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B74" s="13"/>
       <c r="C74" s="21" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D74" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E74" s="16"/>
       <c r="F74" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="G74" s="30" t="n">
+      <c r="G74" s="31" t="n">
         <v>0.1</v>
       </c>
-      <c r="H74" s="34" t="s">
-        <v>172</v>
+      <c r="H74" s="35" t="s">
+        <v>173</v>
       </c>
       <c r="I74" s="13"/>
       <c r="J74" s="13"/>
@@ -3583,24 +3588,24 @@
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="16" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B75" s="13"/>
       <c r="C75" s="21" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E75" s="16"/>
       <c r="F75" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="G75" s="30" t="n">
+      <c r="G75" s="31" t="n">
         <v>0.34</v>
       </c>
-      <c r="H75" s="33" t="s">
-        <v>175</v>
+      <c r="H75" s="34" t="s">
+        <v>176</v>
       </c>
       <c r="I75" s="13"/>
       <c r="J75" s="13"/>
@@ -3625,14 +3630,14 @@
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="16" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B76" s="13"/>
       <c r="C76" s="21" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D76" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E76" s="16"/>
       <c r="F76" s="22" t="n">
@@ -3641,8 +3646,8 @@
       <c r="G76" s="29" t="n">
         <v>0.12</v>
       </c>
-      <c r="H76" s="33" t="s">
-        <v>178</v>
+      <c r="H76" s="34" t="s">
+        <v>179</v>
       </c>
       <c r="I76" s="13"/>
       <c r="J76" s="13"/>
@@ -3666,15 +3671,15 @@
       <c r="AB76" s="13"/>
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="35" t="s">
-        <v>179</v>
+      <c r="A77" s="36" t="s">
+        <v>180</v>
       </c>
       <c r="B77" s="13"/>
       <c r="C77" s="16" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D77" s="21" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E77" s="17"/>
       <c r="F77" s="16" t="n">
@@ -3684,7 +3689,7 @@
         <v>0.32</v>
       </c>
       <c r="H77" s="20" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="I77" s="13"/>
       <c r="J77" s="13"/>
@@ -3708,36 +3713,36 @@
       <c r="AB77" s="13"/>
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="35" t="s">
-        <v>182</v>
-      </c>
-      <c r="C78" s="35" t="s">
+      <c r="A78" s="36" t="s">
         <v>183</v>
       </c>
+      <c r="C78" s="36" t="s">
+        <v>184</v>
+      </c>
       <c r="D78" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="E78" s="32"/>
+        <v>77</v>
+      </c>
+      <c r="E78" s="33"/>
       <c r="F78" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="G78" s="30" t="n">
+      <c r="G78" s="31" t="n">
         <v>0.37</v>
       </c>
-      <c r="H78" s="36" t="s">
-        <v>184</v>
+      <c r="H78" s="30" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="16" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B79" s="13"/>
       <c r="C79" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D79" s="21" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E79" s="17"/>
       <c r="F79" s="22" t="n">
@@ -3747,7 +3752,7 @@
         <v>1.86</v>
       </c>
       <c r="H79" s="37" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="I79" s="25"/>
       <c r="J79" s="25"/>
@@ -3770,14 +3775,14 @@
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="16" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B80" s="13"/>
       <c r="C80" s="18" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D80" s="21" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E80" s="17"/>
       <c r="F80" s="22" t="n">
@@ -3787,7 +3792,7 @@
         <v>2.64</v>
       </c>
       <c r="H80" s="37" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I80" s="25"/>
       <c r="J80" s="25"/>
@@ -3810,11 +3815,11 @@
     </row>
     <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="16" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B81" s="13"/>
       <c r="C81" s="18" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D81" s="17"/>
       <c r="E81" s="16"/>
@@ -3825,7 +3830,7 @@
         <v>1.81</v>
       </c>
       <c r="H81" s="37" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I81" s="25"/>
       <c r="J81" s="25"/>
@@ -3848,16 +3853,16 @@
     </row>
     <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C82" s="21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D82" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E82" s="16" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F82" s="16" t="n">
         <v>1</v>
@@ -3866,7 +3871,7 @@
         <v>1.07</v>
       </c>
       <c r="H82" s="20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3877,7 +3882,7 @@
       <c r="E83" s="16"/>
       <c r="F83" s="22"/>
       <c r="G83" s="23"/>
-      <c r="H83" s="33"/>
+      <c r="H83" s="34"/>
       <c r="I83" s="13"/>
       <c r="J83" s="13"/>
       <c r="K83" s="13"/>
@@ -3901,19 +3906,19 @@
     </row>
     <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="16" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C84" s="21" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D84" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E84" s="16" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F84" s="22" t="n">
         <v>1</v>
@@ -3922,7 +3927,7 @@
         <v>16</v>
       </c>
       <c r="H84" s="24" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I84" s="25"/>
       <c r="J84" s="25"/>
@@ -3947,19 +3952,19 @@
     </row>
     <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C85" s="21" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D85" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E85" s="16" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F85" s="22" t="n">
         <v>1</v>
@@ -3968,7 +3973,7 @@
         <v>16</v>
       </c>
       <c r="H85" s="24" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I85" s="25"/>
       <c r="J85" s="25"/>
@@ -3993,17 +3998,17 @@
     </row>
     <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="16" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B86" s="13"/>
       <c r="C86" s="38" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D86" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E86" s="16" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F86" s="22" t="n">
         <v>1</v>
@@ -4012,7 +4017,7 @@
         <v>0.84</v>
       </c>
       <c r="H86" s="39" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I86" s="25"/>
       <c r="J86" s="25"/>
@@ -4037,26 +4042,26 @@
     </row>
     <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="16" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B87" s="13"/>
       <c r="C87" s="38" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D87" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E87" s="16" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F87" s="22" t="n">
         <v>1</v>
       </c>
       <c r="G87" s="23" t="n">
-        <v>0.27</v>
+        <v>0.78</v>
       </c>
       <c r="H87" s="39" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="I87" s="25"/>
       <c r="J87" s="25"/>
@@ -4090,14 +4095,14 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="16" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C89" s="17"/>
       <c r="D89" s="17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E89" s="17" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F89" s="16" t="n">
         <v>1</v>
@@ -4107,14 +4112,14 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="16" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C90" s="17"/>
       <c r="D90" s="17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E90" s="17" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F90" s="16" t="n">
         <v>1</v>
@@ -4124,12 +4129,12 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="16" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C91" s="17"/>
       <c r="D91" s="17"/>
       <c r="E91" s="17" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F91" s="16" t="n">
         <v>2</v>
@@ -4139,12 +4144,12 @@
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="16" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C92" s="17"/>
       <c r="D92" s="17"/>
       <c r="E92" s="17" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F92" s="16" t="n">
         <v>2</v>
@@ -4154,14 +4159,14 @@
     </row>
     <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="16" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C93" s="17"/>
       <c r="D93" s="17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E93" s="17" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F93" s="16" t="n">
         <v>1</v>
@@ -4169,8 +4174,8 @@
       <c r="G93" s="40" t="n">
         <v>7.12</v>
       </c>
-      <c r="H93" s="31" t="s">
-        <v>215</v>
+      <c r="H93" s="32" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4184,12 +4189,12 @@
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="16" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C95" s="17"/>
       <c r="D95" s="17"/>
       <c r="E95" s="16" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F95" s="16" t="n">
         <v>2</v>
@@ -4199,12 +4204,12 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="16" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C96" s="17"/>
       <c r="D96" s="17"/>
       <c r="E96" s="16" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F96" s="16" t="n">
         <v>2</v>
@@ -4214,25 +4219,25 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="41" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C97" s="41" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D97" s="41" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E97" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="F97" s="41" t="s">
         <v>221</v>
       </c>
-      <c r="F97" s="41" t="s">
-        <v>220</v>
-      </c>
       <c r="G97" s="41" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H97" s="41" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I97" s="42"/>
       <c r="J97" s="42"/>
@@ -4257,14 +4262,14 @@
     </row>
     <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="21" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C98" s="17"/>
       <c r="D98" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E98" s="16" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F98" s="16" t="n">
         <v>1</v>
@@ -4273,19 +4278,19 @@
         <v>17</v>
       </c>
       <c r="H98" s="20" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="21" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C99" s="17"/>
       <c r="D99" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E99" s="16" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F99" s="16" t="n">
         <v>1</v>
@@ -4294,7 +4299,7 @@
         <v>17</v>
       </c>
       <c r="H99" s="20" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4329,31 +4334,31 @@
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="10" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D102" s="11"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D103" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E103" s="12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F103" s="14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G103" s="15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H103" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I103" s="13"/>
       <c r="J103" s="13"/>
@@ -4378,14 +4383,14 @@
     </row>
     <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="16" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B104" s="17"/>
       <c r="C104" s="43" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D104" s="21" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E104" s="16"/>
       <c r="F104" s="21" t="n">
@@ -4395,19 +4400,19 @@
         <v>1.06</v>
       </c>
       <c r="H104" s="20" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="16" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B105" s="17"/>
       <c r="C105" s="43" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D105" s="21" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E105" s="16"/>
       <c r="F105" s="21" t="n">
@@ -4417,19 +4422,19 @@
         <v>5.31</v>
       </c>
       <c r="H105" s="20" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="17" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B106" s="17"/>
       <c r="C106" s="16" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D106" s="21" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E106" s="17"/>
       <c r="F106" s="16" t="n">
@@ -4439,19 +4444,19 @@
         <v>0.32</v>
       </c>
       <c r="H106" s="20" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="17" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B107" s="17"/>
       <c r="C107" s="16" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D107" s="21" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E107" s="17"/>
       <c r="F107" s="16" t="n">
@@ -4461,17 +4466,17 @@
         <v>0.12</v>
       </c>
       <c r="H107" s="20" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="16" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B108" s="17"/>
       <c r="C108" s="17"/>
       <c r="D108" s="16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E108" s="17"/>
       <c r="F108" s="16" t="n">
@@ -4481,17 +4486,17 @@
         <v>3</v>
       </c>
       <c r="H108" s="20" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="16" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B109" s="17"/>
       <c r="C109" s="17"/>
       <c r="D109" s="16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E109" s="17"/>
       <c r="F109" s="16" t="n">
@@ -4501,22 +4506,22 @@
         <v>3</v>
       </c>
       <c r="H109" s="20" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="16" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B110" s="16" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C110" s="16"/>
       <c r="D110" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E110" s="16" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F110" s="22" t="n">
         <v>1</v>
@@ -4525,22 +4530,22 @@
         <v>25</v>
       </c>
       <c r="H110" s="24" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="16" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B111" s="16" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C111" s="16"/>
       <c r="D111" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E111" s="16" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F111" s="22" t="n">
         <v>1</v>
@@ -4549,7 +4554,7 @@
         <v>25</v>
       </c>
       <c r="H111" s="24" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="I111" s="25"/>
       <c r="J111" s="25"/>
@@ -4574,17 +4579,17 @@
     </row>
     <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="16" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B112" s="16" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C112" s="16"/>
       <c r="D112" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E112" s="16" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F112" s="22" t="n">
         <v>1</v>
@@ -4593,7 +4598,7 @@
         <v>25</v>
       </c>
       <c r="H112" s="24" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="I112" s="25"/>
       <c r="J112" s="25"/>
@@ -4618,15 +4623,15 @@
     </row>
     <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="16" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B113" s="17"/>
       <c r="C113" s="17"/>
       <c r="D113" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E113" s="16" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F113" s="16" t="n">
         <v>1</v>
@@ -4635,42 +4640,42 @@
         <v>13</v>
       </c>
       <c r="H113" s="20" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="16" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B114" s="17"/>
       <c r="C114" s="17"/>
       <c r="D114" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E114" s="16" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F114" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="G114" s="30" t="n">
+      <c r="G114" s="31" t="n">
         <v>43.95</v>
       </c>
       <c r="H114" s="20" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="16" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B115" s="17"/>
       <c r="C115" s="17"/>
       <c r="D115" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E115" s="16" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F115" s="16" t="n">
         <v>1</v>
@@ -4679,20 +4684,20 @@
         <v>15</v>
       </c>
       <c r="H115" s="20" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="16" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B116" s="17"/>
       <c r="C116" s="17"/>
       <c r="D116" s="16" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E116" s="16" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F116" s="16" t="n">
         <v>1</v>
@@ -4701,20 +4706,20 @@
         <v>17</v>
       </c>
       <c r="H116" s="20" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="41" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B117" s="44"/>
       <c r="C117" s="41"/>
       <c r="D117" s="41" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E117" s="41" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F117" s="41" t="n">
         <v>1</v>
@@ -4723,7 +4728,7 @@
         <v>80</v>
       </c>
       <c r="H117" s="46" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="I117" s="47"/>
       <c r="J117" s="48"/>
@@ -4781,32 +4786,32 @@
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D120" s="11"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B121" s="13"/>
       <c r="C121" s="12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D121" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E121" s="12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F121" s="14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G121" s="15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H121" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I121" s="13"/>
       <c r="J121" s="13"/>
@@ -4829,17 +4834,17 @@
       <c r="AA121" s="13"/>
       <c r="AB121" s="13"/>
     </row>
-    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="16" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B122" s="17"/>
       <c r="C122" s="17"/>
       <c r="D122" s="16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E122" s="16" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F122" s="16" t="n">
         <v>1</v>
@@ -4848,100 +4853,100 @@
         <v>5</v>
       </c>
       <c r="H122" s="20" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="16" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B123" s="17"/>
       <c r="C123" s="21" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D123" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E123" s="16" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F123" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="G123" s="30" t="n">
+      <c r="G123" s="31" t="n">
         <v>0.6</v>
       </c>
       <c r="H123" s="24" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="16" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B124" s="17"/>
       <c r="C124" s="21" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D124" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E124" s="16" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F124" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="G124" s="30" t="n">
+      <c r="G124" s="31" t="n">
         <v>0.1</v>
       </c>
       <c r="H124" s="24" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="16" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B125" s="17"/>
       <c r="C125" s="21" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D125" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E125" s="17"/>
       <c r="F125" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="G125" s="30" t="n">
+      <c r="G125" s="31" t="n">
         <v>0.36</v>
       </c>
       <c r="H125" s="24" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="126" s="50" customFormat="true" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="49" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C126" s="49" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D126" s="49" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E126" s="49" t="s">
+        <v>281</v>
+      </c>
+      <c r="F126" s="49" t="s">
         <v>280</v>
       </c>
-      <c r="F126" s="49" t="s">
-        <v>279</v>
-      </c>
       <c r="G126" s="49" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H126" s="49" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="J126" s="47"/>
       <c r="K126" s="47"/>
@@ -4965,26 +4970,26 @@
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="41" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B127" s="17"/>
       <c r="C127" s="41" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D127" s="41" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E127" s="41" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F127" s="41" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G127" s="41" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H127" s="41" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I127" s="42"/>
       <c r="J127" s="42"/>
@@ -5056,59 +5061,64 @@
     <hyperlink ref="H27" r:id="rId15" display="https://www.adafruit.com/product/2886"/>
     <hyperlink ref="H28" r:id="rId16" display="https://www.amazon.com/gp/product/B00NH13O7K"/>
     <hyperlink ref="H29" r:id="rId17" display="https://www.adafruit.com/product/328"/>
-    <hyperlink ref="H32" r:id="rId18" display="https://www.digikey.com/products/en?keywords=RNCP0603FTD2K74CT-ND"/>
-    <hyperlink ref="H33" r:id="rId19" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP0603FTD100R/RNCP0603FTD100RCT-ND/2240425"/>
-    <hyperlink ref="H34" r:id="rId20" display="https://www.digikey.com/product-detail/en/AYZ0202AGRLC/401-2013-1-ND/1640122"/>
-    <hyperlink ref="H35" r:id="rId21" display="https://www.adafruit.com/product/2343"/>
-    <hyperlink ref="H36" r:id="rId22" display="https://www.digikey.com/products/en?keywords=WM4802-ND"/>
-    <hyperlink ref="H37" r:id="rId23" display="https://www.digikey.com/products/en?keywords=WM9131-ND"/>
-    <hyperlink ref="H38" r:id="rId24" display="https://www.digikey.com/products/en?keywords=WM4801-ND"/>
-    <hyperlink ref="H39" r:id="rId25" display="https://www.digikey.com/products/en?keywords=WM10647-ND"/>
-    <hyperlink ref="H40" r:id="rId26" display="https://www.digikey.com/product-detail/en/3m/3302-16-300SF/MC16M-100-ND/145737"/>
-    <hyperlink ref="H41" r:id="rId27" display="https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2004A.12.02/C2004W-100-ND/57495"/>
-    <hyperlink ref="H46" r:id="rId28" display="https://www.adafruit.com/product/2240"/>
-    <hyperlink ref="H48" r:id="rId29" display="https://www.tapplastics.com/product/plastics/cut_to_size_plastic/satinice_white/655"/>
-    <hyperlink ref="H54" r:id="rId30" display="https://www.atlas-scientific.com/product_pages/circuits/ezo_ph.html"/>
-    <hyperlink ref="H55" r:id="rId31" display="https://www.atlas-scientific.com/product_pages/probes/ph_probe.html"/>
-    <hyperlink ref="H56" r:id="rId32" display="https://www.atlas-scientific.com/product_pages/components/single_carrier_iso.html"/>
-    <hyperlink ref="H57" r:id="rId33" display="https://www.hach.com/ph-buffer-solution-kit-color-coded-ph-4-01-ph-7-00-and-ph-10-01-500-ml-each/product?id=7640205069"/>
-    <hyperlink ref="H58" r:id="rId34" display="https://www.hach.com/electrolyte-solution-kcl-3m-50ml/product-parameter-reagent?id=7640207762"/>
-    <hyperlink ref="H63" r:id="rId35" display="https://www.mcmaster.com/8972T11"/>
-    <hyperlink ref="H64" r:id="rId36" display="https://www.mcmaster.com/4339T5"/>
-    <hyperlink ref="H71" r:id="rId37" display="https://www.digikey.com/product-detail/en/yageo/AT0603FRE0710KL/YAG2122CT-ND/5139570"/>
-    <hyperlink ref="H72" r:id="rId38" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP0603FTD2K74/RNCP0603FTD2K74CT-ND/2240457"/>
-    <hyperlink ref="H73" r:id="rId39" display="https://www.digikey.com/product-detail/en/yageo/RT0603BRD071ML/YAG4498CT-ND/6616654"/>
-    <hyperlink ref="H74" r:id="rId40" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP0603FTD1K00/RNCP0603FTD1K00CT-ND/2240445"/>
-    <hyperlink ref="H75" r:id="rId41" display="https://www.digikey.com/product-detail/en/yageo/RT0603BRD0742K2L/YAG4556CT-ND/6616712"/>
-    <hyperlink ref="H76" r:id="rId42" display="https://www.digikey.com/product-detail/en/yageo/RT0603DRE071K2L/311-2461-1-ND/6128880"/>
-    <hyperlink ref="H77" r:id="rId43" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X8R1H104K080AB/445-8818-1-ND/3248223"/>
-    <hyperlink ref="H78" r:id="rId44" display="https://www.digikey.com/products/en?keywords=641-1331-1-ND"/>
-    <hyperlink ref="H79" r:id="rId45" display="https://www.digikey.com/product-detail/en/texas-instruments/TLE2426CD/296-6547-5-ND/371934"/>
-    <hyperlink ref="H80" r:id="rId46" display="https://www.digikey.com/product-detail/en/analog-devices-inc/AD8655ARZ-REEL7/AD8655ARZ-REEL7CT-ND/3678589"/>
-    <hyperlink ref="H81" r:id="rId47" display="https://www.digikey.com/product-detail/en/texas-instruments/TLV2374IDR/296-11967-1-ND/390435"/>
-    <hyperlink ref="H82" r:id="rId48" display="https://www.digikey.com/product-detail/en/AYZ0202AGRLC/401-2013-1-ND/1640122"/>
-    <hyperlink ref="H84" r:id="rId49" display="https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2117A.12.06/C2117G-100-ND/16217"/>
-    <hyperlink ref="H85" r:id="rId50" display="https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2004A.12.02/C2004W-100-ND/57495"/>
-    <hyperlink ref="H86" r:id="rId51" display="https://www.digikey.com/products/en?keywords=%09WM4800-ND"/>
-    <hyperlink ref="H87" r:id="rId52" display="https://www.digikey.com/products/en?keywords=WM2900-ND%E2%80%8E"/>
-    <hyperlink ref="H93" r:id="rId53" display="https://www.amazon.com/gp/product/B01IBOK7FE/"/>
-    <hyperlink ref="H98" r:id="rId54" display="https://www.amazon.com/gp/product/B01F2R2EPE/"/>
-    <hyperlink ref="H99" r:id="rId55" display="https://www.amazon.com/gp/product/B01F7L9QD8/"/>
-    <hyperlink ref="H104" r:id="rId56" display="https://www.digikey.com/product-detail/en/vishay-semiconductor-opto-division/VSMY2850G/VSMY2850GCT-ND/2615293"/>
-    <hyperlink ref="H105" r:id="rId57" display="https://www.digikey.com/product-detail/en/ams/TSL237T/TSL237-TCT-ND/3095287"/>
-    <hyperlink ref="H106" r:id="rId58" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X8R1H104K080AB/445-8818-1-ND/3248223"/>
-    <hyperlink ref="H107" r:id="rId59" display="https://www.digikey.com/product-detail/en/yageo/RT0603DRD07200RL/311-200DCT-ND/1035740"/>
-    <hyperlink ref="H110" r:id="rId60" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-BK005/422010-BK005-ND/3705786"/>
-    <hyperlink ref="H111" r:id="rId61" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-RD005/422010-RD005-ND/4935160"/>
-    <hyperlink ref="H112" r:id="rId62" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-SL005/422010-SL005-ND/4935161"/>
-    <hyperlink ref="H113" r:id="rId63" display="https://www.amazon.com/Source-One-LLC-Acrylic-Plexiglass/dp/B06XNXHKQN/"/>
-    <hyperlink ref="H114" r:id="rId64" location="product-description-iframe" display="https://www.amazon.com/MG-Chemicals-Thermally-Conductive-Encapsulating/dp/B008UH4CRM#product-description-iframe"/>
-    <hyperlink ref="H115" r:id="rId65" display="https://www.amazon.com/CRC-SL2512-Soluble-Oil-32/dp/B000M8O010/"/>
-    <hyperlink ref="H116" r:id="rId66" display="https://www.discountvials.com/6-dram-glass-vial-w-cap/"/>
-    <hyperlink ref="H117" r:id="rId67" display="http://www.hach.com/formazin-turbidity-standard-4000-ntu-500-ml/product?id=7640455437"/>
-    <hyperlink ref="H123" r:id="rId68" display="https://www.digikey.com/product-detail/en/microchip-technology/AT30TS750A-SS8M-T/1611-AT30TS750A-SS8M-TCT-ND/6831450"/>
-    <hyperlink ref="H124" r:id="rId69" display="http://www.digikey.com/product-detail/en/RC1206FR-0710KL/311-10.0KFRCT-ND/731430"/>
-    <hyperlink ref="H125" r:id="rId70" display="https://www.digikey.com/product-detail/en/avx-corporation/1206VC104KAT2A/478-5724-1-ND/2136332"/>
+    <hyperlink ref="H31" r:id="rId18" display="https://github.com/lperovich/seeboat/tree/master/hardware/controlBoard"/>
+    <hyperlink ref="H32" r:id="rId19" display="https://www.digikey.com/products/en?keywords=RNCP0603FTD2K74CT-ND"/>
+    <hyperlink ref="H33" r:id="rId20" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP0603FTD100R/RNCP0603FTD100RCT-ND/2240425"/>
+    <hyperlink ref="H34" r:id="rId21" display="https://www.digikey.com/product-detail/en/AYZ0202AGRLC/401-2013-1-ND/1640122"/>
+    <hyperlink ref="H35" r:id="rId22" display="https://www.adafruit.com/product/2343"/>
+    <hyperlink ref="H36" r:id="rId23" display="https://www.digikey.com/products/en?keywords=WM4802-ND"/>
+    <hyperlink ref="H37" r:id="rId24" display="https://www.digikey.com/products/en?keywords=WM9131-ND"/>
+    <hyperlink ref="H38" r:id="rId25" display="https://www.digikey.com/products/en?keywords=WM4801-ND"/>
+    <hyperlink ref="H39" r:id="rId26" display="https://www.digikey.com/products/en?keywords=WM10647-ND"/>
+    <hyperlink ref="H40" r:id="rId27" display="https://www.digikey.com/product-detail/en/3m/3302-16-300SF/MC16M-100-ND/145737"/>
+    <hyperlink ref="H41" r:id="rId28" display="https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2004A.12.02/C2004W-100-ND/57495"/>
+    <hyperlink ref="H46" r:id="rId29" display="https://www.adafruit.com/product/2240"/>
+    <hyperlink ref="H48" r:id="rId30" display="https://www.tapplastics.com/product/plastics/cut_to_size_plastic/satinice_white/655"/>
+    <hyperlink ref="H54" r:id="rId31" display="https://www.atlas-scientific.com/product_pages/circuits/ezo_ph.html"/>
+    <hyperlink ref="H55" r:id="rId32" display="https://www.atlas-scientific.com/product_pages/probes/ph_probe.html"/>
+    <hyperlink ref="H56" r:id="rId33" display="https://www.atlas-scientific.com/product_pages/components/single_carrier_iso.html"/>
+    <hyperlink ref="H57" r:id="rId34" display="https://www.hach.com/ph-buffer-solution-kit-color-coded-ph-4-01-ph-7-00-and-ph-10-01-500-ml-each/product?id=7640205069"/>
+    <hyperlink ref="H58" r:id="rId35" display="https://www.hach.com/electrolyte-solution-kcl-3m-50ml/product-parameter-reagent?id=7640207762"/>
+    <hyperlink ref="H63" r:id="rId36" display="https://www.mcmaster.com/8972T11"/>
+    <hyperlink ref="H64" r:id="rId37" display="https://www.mcmaster.com/4339T5"/>
+    <hyperlink ref="H70" r:id="rId38" display="https://github.com/lperovich/seeboat/tree/master/hardware/conductivity"/>
+    <hyperlink ref="H71" r:id="rId39" display="https://www.digikey.com/product-detail/en/yageo/AT0603FRE0710KL/YAG2122CT-ND/5139570"/>
+    <hyperlink ref="H72" r:id="rId40" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP0603FTD2K74/RNCP0603FTD2K74CT-ND/2240457"/>
+    <hyperlink ref="H73" r:id="rId41" display="https://www.digikey.com/product-detail/en/yageo/RT0603BRD071ML/YAG4498CT-ND/6616654"/>
+    <hyperlink ref="H74" r:id="rId42" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP0603FTD1K00/RNCP0603FTD1K00CT-ND/2240445"/>
+    <hyperlink ref="H75" r:id="rId43" display="https://www.digikey.com/product-detail/en/yageo/RT0603BRD0742K2L/YAG4556CT-ND/6616712"/>
+    <hyperlink ref="H76" r:id="rId44" display="https://www.digikey.com/product-detail/en/yageo/RT0603DRE071K2L/311-2461-1-ND/6128880"/>
+    <hyperlink ref="H77" r:id="rId45" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X8R1H104K080AB/445-8818-1-ND/3248223"/>
+    <hyperlink ref="H78" r:id="rId46" display="https://www.digikey.com/products/en?keywords=641-1331-1-ND"/>
+    <hyperlink ref="H79" r:id="rId47" display="https://www.digikey.com/product-detail/en/texas-instruments/TLE2426CD/296-6547-5-ND/371934"/>
+    <hyperlink ref="H80" r:id="rId48" display="https://www.digikey.com/product-detail/en/analog-devices-inc/AD8655ARZ-REEL7/AD8655ARZ-REEL7CT-ND/3678589"/>
+    <hyperlink ref="H81" r:id="rId49" display="https://www.digikey.com/product-detail/en/texas-instruments/TLV2374IDR/296-11967-1-ND/390435"/>
+    <hyperlink ref="H82" r:id="rId50" display="https://www.digikey.com/product-detail/en/AYZ0202AGRLC/401-2013-1-ND/1640122"/>
+    <hyperlink ref="H84" r:id="rId51" display="https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2117A.12.06/C2117G-100-ND/16217"/>
+    <hyperlink ref="H85" r:id="rId52" display="https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2004A.12.02/C2004W-100-ND/57495"/>
+    <hyperlink ref="H86" r:id="rId53" display="https://www.digikey.com/products/en?keywords=%09WM4800-ND"/>
+    <hyperlink ref="H87" r:id="rId54" display="https://www.digikey.com/products/en?keywords=WM24819-ND"/>
+    <hyperlink ref="H93" r:id="rId55" display="https://www.amazon.com/gp/product/B01IBOK7FE/"/>
+    <hyperlink ref="H98" r:id="rId56" display="https://www.amazon.com/gp/product/B01F2R2EPE/"/>
+    <hyperlink ref="H99" r:id="rId57" display="https://www.amazon.com/gp/product/B01F7L9QD8/"/>
+    <hyperlink ref="H104" r:id="rId58" display="https://www.digikey.com/product-detail/en/vishay-semiconductor-opto-division/VSMY2850G/VSMY2850GCT-ND/2615293"/>
+    <hyperlink ref="H105" r:id="rId59" display="https://www.digikey.com/product-detail/en/ams/TSL237T/TSL237-TCT-ND/3095287"/>
+    <hyperlink ref="H106" r:id="rId60" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X8R1H104K080AB/445-8818-1-ND/3248223"/>
+    <hyperlink ref="H107" r:id="rId61" display="https://www.digikey.com/product-detail/en/yageo/RT0603DRD07200RL/311-200DCT-ND/1035740"/>
+    <hyperlink ref="H108" r:id="rId62" display="https://github.com/lperovich/seeboat/tree/master/hardware/turbiditySensor"/>
+    <hyperlink ref="H109" r:id="rId63" display="https://github.com/lperovich/seeboat/tree/master/hardware/turbidityLED"/>
+    <hyperlink ref="H110" r:id="rId64" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-BK005/422010-BK005-ND/3705786"/>
+    <hyperlink ref="H111" r:id="rId65" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-RD005/422010-RD005-ND/4935160"/>
+    <hyperlink ref="H112" r:id="rId66" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-SL005/422010-SL005-ND/4935161"/>
+    <hyperlink ref="H113" r:id="rId67" display="https://www.amazon.com/Source-One-LLC-Acrylic-Plexiglass/dp/B06XNXHKQN/"/>
+    <hyperlink ref="H114" r:id="rId68" location="product-description-iframe" display="https://www.amazon.com/MG-Chemicals-Thermally-Conductive-Encapsulating/dp/B008UH4CRM#product-description-iframe"/>
+    <hyperlink ref="H115" r:id="rId69" display="https://www.amazon.com/CRC-SL2512-Soluble-Oil-32/dp/B000M8O010/"/>
+    <hyperlink ref="H116" r:id="rId70" display="https://www.discountvials.com/6-dram-glass-vial-w-cap/"/>
+    <hyperlink ref="H117" r:id="rId71" display="http://www.hach.com/formazin-turbidity-standard-4000-ntu-500-ml/product?id=7640455437"/>
+    <hyperlink ref="H122" r:id="rId72" display="https://github.com/lperovich/seeboat/tree/master/hardware/temperatureSensor"/>
+    <hyperlink ref="H123" r:id="rId73" display="https://www.digikey.com/product-detail/en/microchip-technology/AT30TS750A-SS8M-T/1611-AT30TS750A-SS8M-TCT-ND/6831450"/>
+    <hyperlink ref="H124" r:id="rId74" display="http://www.digikey.com/product-detail/en/RC1206FR-0710KL/311-10.0KFRCT-ND/731430"/>
+    <hyperlink ref="H125" r:id="rId75" display="https://www.digikey.com/product-detail/en/avx-corporation/1206VC104KAT2A/478-5724-1-ND/2136332"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5143,122 +5153,122 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="26" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="G3" s="51" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="26" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="26" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="26" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="D9" s="52" t="s">
+        <v>296</v>
+      </c>
+      <c r="E9" s="26" t="s">
         <v>294</v>
       </c>
-      <c r="D9" s="52" t="s">
-        <v>295</v>
-      </c>
-      <c r="E9" s="26" t="s">
-        <v>293</v>
-      </c>
       <c r="F9" s="26" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G9" s="53" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="26" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D10" s="52" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="26" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D11" s="52" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="52" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="52" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D15" s="52" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5267,52 +5277,52 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="52" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="54" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E19" s="26" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="26" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D20" s="52" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E20" s="54" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="F20" s="26" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="13" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -5324,7 +5334,7 @@
         <v>16</v>
       </c>
       <c r="H28" s="56" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="I28" s="25"/>
       <c r="J28" s="25"/>
@@ -5349,10 +5359,10 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="13" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
@@ -5364,7 +5374,7 @@
         <v>16</v>
       </c>
       <c r="H29" s="56" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="I29" s="25"/>
       <c r="J29" s="25"/>
@@ -5389,15 +5399,15 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="13" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
       <c r="D30" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F30" s="55" t="n">
         <v>4</v>
@@ -5406,7 +5416,7 @@
         <v>0.5</v>
       </c>
       <c r="H30" s="56" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="I30" s="25"/>
       <c r="J30" s="13"/>
@@ -5431,12 +5441,12 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="13" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="55" t="n">
@@ -5446,7 +5456,7 @@
         <v>1.5</v>
       </c>
       <c r="H31" s="56" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="I31" s="25"/>
       <c r="J31" s="13"/>
@@ -5471,15 +5481,15 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="13" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
       <c r="D35" s="13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="F35" s="55" t="n">
         <v>1</v>
@@ -5488,7 +5498,7 @@
         <v>31</v>
       </c>
       <c r="H35" s="56" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="J35" s="25"/>
       <c r="K35" s="25"/>
@@ -5512,13 +5522,13 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="26" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E36" s="26" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F36" s="26" t="n">
         <v>1</v>
@@ -5527,18 +5537,18 @@
         <v>8</v>
       </c>
       <c r="H36" s="52" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="26" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F37" s="26" t="n">
         <v>1</v>
@@ -5547,18 +5557,18 @@
         <v>27</v>
       </c>
       <c r="H37" s="52" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="26" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="F38" s="26" t="n">
         <v>1</v>
@@ -5567,18 +5577,18 @@
         <v>25</v>
       </c>
       <c r="H38" s="52" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="26" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F39" s="26" t="n">
         <v>1</v>
@@ -5589,13 +5599,13 @@
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="26" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D40" s="26" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="F40" s="26" t="n">
         <v>1</v>
@@ -5604,7 +5614,7 @@
         <v>10</v>
       </c>
       <c r="H40" s="52" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add tubing conductivity holder, update boat parts
</commit_message>
<xml_diff>
--- a/hardware/SeeBoat_fullPartsList.xlsx
+++ b/hardware/SeeBoat_fullPartsList.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="349">
   <si>
     <t xml:space="preserve">Parts list for SeeBoat &amp; full sensor suite</t>
   </si>
@@ -68,7 +68,7 @@
     <t xml:space="preserve">Horizon Hobby</t>
   </si>
   <si>
-    <t xml:space="preserve">the full boat, including radio controller</t>
+    <t xml:space="preserve">ArtBoat full boat, including radio controller</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.horizonhobby.com/blackjack-24-inch-catamaran-brushless%3A-rtr-prb08007</t>
@@ -128,6 +128,9 @@
     <t xml:space="preserve">https://www.amazon.com/INDUSTRIES-4471-Sandpaper-9-Inch-11-Inch/dp/B001AVYXVU</t>
   </si>
   <si>
+    <t xml:space="preserve">Amazon</t>
+  </si>
+  <si>
     <t xml:space="preserve">HobbyKing 350w 25A Power Supply (100v~120v)</t>
   </si>
   <si>
@@ -149,12 +152,18 @@
     <t xml:space="preserve">Stealthwake 23" Brushed Deep-V RTR</t>
   </si>
   <si>
-    <t xml:space="preserve">alternative cheaper boat that may also work--test this</t>
+    <t xml:space="preserve">SeeBoat boat, including radio controller, and more space for the sensors than the ArtBoat boat</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.horizonhobby.com/boats/electric-boats/stealthwake-rtr-23-inch-brushed-deep-v-prb08015</t>
   </si>
   <si>
+    <t xml:space="preserve">Reaction 7.4V 5000mAh 2S 30C LiPo Hardcase: EC3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">large battery for the boat, a Ni battery is included with the boat, but this one is better for longer use</t>
+  </si>
+  <si>
     <t xml:space="preserve">CONTROL BOARD</t>
   </si>
   <si>
@@ -218,9 +227,6 @@
     <t xml:space="preserve">micro USB cable</t>
   </si>
   <si>
-    <t xml:space="preserve">Amazon</t>
-  </si>
-  <si>
     <t xml:space="preserve">cable for programming feather</t>
   </si>
   <si>
@@ -650,25 +656,19 @@
     <t xml:space="preserve">sensor probe</t>
   </si>
   <si>
-    <t xml:space="preserve">3D printed probe housing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">connects to the boat directly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plastic screws</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to connect the probe housing to the boat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plastic nuts</t>
+    <t xml:space="preserve">foam tubing: Multipurpose Blended Neoprene Foam Tube, 1"  OD, 3/4" ID, 10 Feet Long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">connects to the boat directly to hold the conductivity probe in place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mcmaster.com/2029n13</t>
   </si>
   <si>
     <t xml:space="preserve">plastic to plastic epoxy</t>
   </si>
   <si>
-    <t xml:space="preserve">to glue the probe to the boat</t>
+    <t xml:space="preserve">to glue the foam tubing to the boat, also used for the turbidity holder and the LED panels</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.amazon.com/gp/product/B01IBOK7FE/</t>
@@ -1483,6 +1483,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1497,10 +1501,6 @@
     </xf>
     <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1696,10 +1696,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB130"/>
+  <dimension ref="A1:AB1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1972,230 +1972,180 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="17"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="16"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="21" t="s">
+      <c r="D14" s="16" t="s">
         <v>35</v>
       </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="20"/>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="17"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
-      <c r="D15" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G15" s="19" t="n">
-        <v>46</v>
-      </c>
-      <c r="H15" s="20" t="s">
-        <v>38</v>
-      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="21" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="D16" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F16" s="16" t="n">
         <v>1</v>
       </c>
       <c r="G16" s="19" t="n">
-        <v>126</v>
+        <v>46</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="19" t="n">
+        <v>126</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G17" s="19" t="n">
+      <c r="E18" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="19" t="n">
         <v>160</v>
       </c>
-      <c r="H17" s="20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="26"/>
-      <c r="H18" s="26"/>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="27"/>
-      <c r="O19" s="27"/>
-      <c r="P19" s="27"/>
-      <c r="Q19" s="27"/>
-      <c r="R19" s="27"/>
-      <c r="S19" s="27"/>
-      <c r="T19" s="27"/>
-      <c r="U19" s="27"/>
-      <c r="V19" s="27"/>
-      <c r="W19" s="27"/>
-      <c r="X19" s="27"/>
-      <c r="Y19" s="27"/>
-      <c r="Z19" s="27"/>
-      <c r="AA19" s="27"/>
-      <c r="AB19" s="27"/>
+      <c r="H18" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" s="19" t="n">
+        <v>50</v>
+      </c>
+      <c r="H19" s="26" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="11"/>
+      <c r="A20" s="27"/>
+      <c r="H20" s="27"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="28"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="28"/>
+      <c r="R21" s="28"/>
+      <c r="S21" s="28"/>
+      <c r="T21" s="28"/>
+      <c r="U21" s="28"/>
+      <c r="V21" s="28"/>
+      <c r="W21" s="28"/>
+      <c r="X21" s="28"/>
+      <c r="Y21" s="28"/>
+      <c r="Z21" s="28"/>
+      <c r="AA21" s="28"/>
+      <c r="AB21" s="28"/>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="11"/>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="12" t="s">
+      <c r="B23" s="13"/>
+      <c r="C23" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D23" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E23" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F23" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G23" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="12" t="s">
+      <c r="H23" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
-      <c r="U21" s="13"/>
-      <c r="V21" s="13"/>
-      <c r="W21" s="13"/>
-      <c r="X21" s="13"/>
-      <c r="Y21" s="13"/>
-      <c r="Z21" s="13"/>
-      <c r="AA21" s="13"/>
-      <c r="AB21" s="13"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G22" s="23" t="n">
-        <v>35</v>
-      </c>
-      <c r="H22" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="I22" s="28"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13"/>
-      <c r="U22" s="13"/>
-      <c r="V22" s="13"/>
-      <c r="W22" s="13"/>
-      <c r="X22" s="13"/>
-      <c r="Y22" s="13"/>
-      <c r="Z22" s="13"/>
-      <c r="AA22" s="13"/>
-      <c r="AB22" s="13"/>
-    </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G23" s="23" t="n">
-        <v>40</v>
-      </c>
-      <c r="H23" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="I23" s="28"/>
+      <c r="I23" s="13"/>
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
@@ -2216,28 +2166,28 @@
       <c r="AA23" s="13"/>
       <c r="AB23" s="13"/>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F24" s="22" t="n">
         <v>1</v>
       </c>
       <c r="G24" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="H24" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="I24" s="28"/>
+        <v>35</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="I24" s="29"/>
       <c r="J24" s="13"/>
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
@@ -2260,26 +2210,26 @@
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F25" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="G25" s="29" t="n">
-        <v>3</v>
+      <c r="G25" s="23" t="n">
+        <v>40</v>
       </c>
       <c r="H25" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="I25" s="28"/>
+        <v>54</v>
+      </c>
+      <c r="I25" s="29"/>
       <c r="J25" s="13"/>
       <c r="K25" s="13"/>
       <c r="L25" s="13"/>
@@ -2302,26 +2252,26 @@
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F26" s="22" t="n">
-        <v>4</v>
-      </c>
-      <c r="G26" s="29" t="n">
-        <v>1.25</v>
+        <v>1</v>
+      </c>
+      <c r="G26" s="23" t="n">
+        <v>1</v>
       </c>
       <c r="H26" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="I26" s="28"/>
+        <v>57</v>
+      </c>
+      <c r="I26" s="29"/>
       <c r="J26" s="13"/>
       <c r="K26" s="13"/>
       <c r="L26" s="13"/>
@@ -2344,26 +2294,26 @@
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F27" s="22" t="n">
-        <v>4</v>
-      </c>
-      <c r="G27" s="29" t="n">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="G27" s="30" t="n">
+        <v>3</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I27" s="28"/>
+        <v>60</v>
+      </c>
+      <c r="I27" s="29"/>
       <c r="J27" s="13"/>
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
@@ -2386,26 +2336,26 @@
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="16" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
       <c r="D28" s="16" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F28" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G28" s="29" t="n">
-        <v>5.59</v>
+        <v>4</v>
+      </c>
+      <c r="G28" s="30" t="n">
+        <v>1.25</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="I28" s="28"/>
+        <v>63</v>
+      </c>
+      <c r="I28" s="29"/>
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
       <c r="L28" s="13"/>
@@ -2428,26 +2378,26 @@
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
       <c r="D29" s="16" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F29" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G29" s="23" t="n">
-        <v>15</v>
+        <v>4</v>
+      </c>
+      <c r="G29" s="30" t="n">
+        <v>1</v>
       </c>
       <c r="H29" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="I29" s="16"/>
+        <v>66</v>
+      </c>
+      <c r="I29" s="29"/>
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
       <c r="L29" s="13"/>
@@ -2465,454 +2415,457 @@
       <c r="X29" s="13"/>
       <c r="Y29" s="13"/>
       <c r="Z29" s="13"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="16"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="17"/>
+      <c r="AA29" s="13"/>
+      <c r="AB29" s="13"/>
+    </row>
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="F30" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" s="30" t="n">
+        <v>5.59</v>
+      </c>
+      <c r="H30" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I30" s="29"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="13"/>
+      <c r="V30" s="13"/>
+      <c r="W30" s="13"/>
+      <c r="X30" s="13"/>
+      <c r="Y30" s="13"/>
+      <c r="Z30" s="13"/>
+      <c r="AA30" s="13"/>
+      <c r="AB30" s="13"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="16" t="s">
+      <c r="F31" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" s="23" t="n">
+        <v>15</v>
+      </c>
+      <c r="H31" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="E31" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="F31" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G31" s="19" t="n">
-        <v>5</v>
-      </c>
-      <c r="H31" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="I31" s="17"/>
-    </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="16" t="s">
-        <v>75</v>
-      </c>
+      <c r="I31" s="16"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="13"/>
+      <c r="V31" s="13"/>
+      <c r="W31" s="13"/>
+      <c r="X31" s="13"/>
+      <c r="Y31" s="13"/>
+      <c r="Z31" s="13"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="16"/>
       <c r="B32" s="17"/>
-      <c r="C32" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="F32" s="16" t="n">
-        <v>2</v>
-      </c>
-      <c r="G32" s="31" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="H32" s="20" t="s">
-        <v>79</v>
-      </c>
+      <c r="C32" s="17"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="16"/>
       <c r="I32" s="17"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="16" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B33" s="17"/>
-      <c r="C33" s="21" t="s">
-        <v>81</v>
-      </c>
+      <c r="C33" s="17"/>
       <c r="D33" s="16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F33" s="16" t="n">
-        <v>3</v>
-      </c>
-      <c r="G33" s="31" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="H33" s="20" t="s">
-        <v>83</v>
+        <v>1</v>
+      </c>
+      <c r="G33" s="19" t="n">
+        <v>5</v>
+      </c>
+      <c r="H33" s="26" t="s">
+        <v>76</v>
       </c>
       <c r="I33" s="17"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="16" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="21" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F34" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G34" s="29" t="n">
-        <v>1.07</v>
+        <v>2</v>
+      </c>
+      <c r="G34" s="31" t="n">
+        <v>0.1</v>
       </c>
       <c r="H34" s="20" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="I34" s="17"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="16" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B35" s="17"/>
-      <c r="C35" s="21" t="n">
-        <v>2343</v>
+      <c r="C35" s="21" t="s">
+        <v>83</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F35" s="16" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G35" s="31" t="n">
-        <v>4.5</v>
+        <v>0.1</v>
       </c>
       <c r="H35" s="20" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I35" s="17"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="16" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B36" s="17"/>
       <c r="C36" s="21" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F36" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="G36" s="31" t="n">
-        <v>0.94</v>
+        <v>1</v>
+      </c>
+      <c r="G36" s="30" t="n">
+        <v>1.07</v>
       </c>
       <c r="H36" s="20" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I36" s="17"/>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="16" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B37" s="17"/>
-      <c r="C37" s="21" t="s">
-        <v>96</v>
+      <c r="C37" s="21" t="n">
+        <v>2343</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F37" s="16" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G37" s="31" t="n">
-        <v>1.46</v>
+        <v>4.5</v>
       </c>
       <c r="H37" s="20" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="I37" s="17"/>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="16" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B38" s="17"/>
       <c r="C38" s="21" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F38" s="16" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G38" s="31" t="n">
-        <v>0.87</v>
+        <v>0.94</v>
       </c>
       <c r="H38" s="20" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="I38" s="17"/>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="16" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B39" s="17"/>
       <c r="C39" s="21" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F39" s="16" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G39" s="31" t="n">
-        <v>0.99</v>
+        <v>1.46</v>
       </c>
       <c r="H39" s="20" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="I39" s="17"/>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="16" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B40" s="17"/>
       <c r="C40" s="21" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F40" s="16" t="n">
         <v>1</v>
       </c>
       <c r="G40" s="31" t="n">
-        <v>95.15</v>
+        <v>0.87</v>
       </c>
       <c r="H40" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="I40" s="16" t="s">
-        <v>111</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="I40" s="17"/>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B41" s="17"/>
+      <c r="C41" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="F41" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G41" s="31" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="H41" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="I41" s="17"/>
+    </row>
+    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B42" s="17"/>
+      <c r="C42" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F42" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" s="31" t="n">
+        <v>95.15</v>
+      </c>
+      <c r="H42" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="I42" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="C41" s="21" t="s">
+    </row>
+    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="D41" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="E41" s="16" t="s">
+      <c r="B43" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="F41" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G41" s="23" t="n">
+      <c r="C43" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="F43" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G43" s="23" t="n">
         <v>16</v>
       </c>
-      <c r="H41" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="I41" s="28"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="25"/>
-      <c r="L41" s="25"/>
-      <c r="M41" s="25"/>
-      <c r="N41" s="13"/>
-      <c r="O41" s="13"/>
-      <c r="P41" s="13"/>
-      <c r="Q41" s="13"/>
-      <c r="R41" s="13"/>
-      <c r="S41" s="13"/>
-      <c r="T41" s="13"/>
-      <c r="U41" s="13"/>
-      <c r="V41" s="13"/>
-      <c r="W41" s="13"/>
-      <c r="X41" s="13"/>
-      <c r="Y41" s="13"/>
-      <c r="Z41" s="13"/>
-      <c r="AA41" s="13"/>
-      <c r="AB41" s="13"/>
-    </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="27"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="27"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
-      <c r="K43" s="27"/>
-      <c r="L43" s="27"/>
-      <c r="M43" s="27"/>
-      <c r="N43" s="27"/>
-      <c r="O43" s="27"/>
-      <c r="P43" s="27"/>
-      <c r="Q43" s="27"/>
-      <c r="R43" s="27"/>
-      <c r="S43" s="27"/>
-      <c r="T43" s="27"/>
-      <c r="U43" s="27"/>
-      <c r="V43" s="27"/>
-      <c r="W43" s="27"/>
-      <c r="X43" s="27"/>
-      <c r="Y43" s="27"/>
-      <c r="Z43" s="27"/>
-      <c r="AA43" s="27"/>
-      <c r="AB43" s="27"/>
-    </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="D44" s="11"/>
+      <c r="H43" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="I43" s="29"/>
+      <c r="J43" s="25"/>
+      <c r="K43" s="25"/>
+      <c r="L43" s="25"/>
+      <c r="M43" s="25"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
+      <c r="P43" s="13"/>
+      <c r="Q43" s="13"/>
+      <c r="R43" s="13"/>
+      <c r="S43" s="13"/>
+      <c r="T43" s="13"/>
+      <c r="U43" s="13"/>
+      <c r="V43" s="13"/>
+      <c r="W43" s="13"/>
+      <c r="X43" s="13"/>
+      <c r="Y43" s="13"/>
+      <c r="Z43" s="13"/>
+      <c r="AA43" s="13"/>
+      <c r="AB43" s="13"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="12" t="s">
+      <c r="A45" s="28"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="28"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="28"/>
+      <c r="K45" s="28"/>
+      <c r="L45" s="28"/>
+      <c r="M45" s="28"/>
+      <c r="N45" s="28"/>
+      <c r="O45" s="28"/>
+      <c r="P45" s="28"/>
+      <c r="Q45" s="28"/>
+      <c r="R45" s="28"/>
+      <c r="S45" s="28"/>
+      <c r="T45" s="28"/>
+      <c r="U45" s="28"/>
+      <c r="V45" s="28"/>
+      <c r="W45" s="28"/>
+      <c r="X45" s="28"/>
+      <c r="Y45" s="28"/>
+      <c r="Z45" s="28"/>
+      <c r="AA45" s="28"/>
+      <c r="AB45" s="28"/>
+    </row>
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="D46" s="11"/>
+    </row>
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B45" s="13"/>
-      <c r="C45" s="12" t="s">
+      <c r="B47" s="13"/>
+      <c r="C47" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D47" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E45" s="12" t="s">
+      <c r="E47" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F45" s="14" t="s">
+      <c r="F47" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G45" s="15" t="s">
+      <c r="G47" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H45" s="12" t="s">
+      <c r="H47" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I45" s="13"/>
-      <c r="J45" s="13"/>
-      <c r="K45" s="13"/>
-      <c r="L45" s="13"/>
-      <c r="M45" s="13"/>
-      <c r="N45" s="13"/>
-      <c r="O45" s="13"/>
-      <c r="P45" s="13"/>
-      <c r="Q45" s="13"/>
-      <c r="R45" s="13"/>
-      <c r="S45" s="13"/>
-      <c r="T45" s="13"/>
-      <c r="U45" s="13"/>
-      <c r="V45" s="13"/>
-      <c r="W45" s="13"/>
-      <c r="X45" s="13"/>
-      <c r="Y45" s="13"/>
-      <c r="Z45" s="13"/>
-      <c r="AA45" s="13"/>
-      <c r="AB45" s="13"/>
-    </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="B46" s="28"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E46" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="F46" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G46" s="23" t="n">
-        <v>30</v>
-      </c>
-      <c r="H46" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="J46" s="13"/>
-      <c r="K46" s="13"/>
-      <c r="L46" s="13"/>
-      <c r="M46" s="13"/>
-      <c r="N46" s="13"/>
-      <c r="O46" s="13"/>
-      <c r="P46" s="13"/>
-      <c r="Q46" s="13"/>
-      <c r="R46" s="13"/>
-      <c r="S46" s="13"/>
-      <c r="T46" s="13"/>
-      <c r="U46" s="13"/>
-      <c r="V46" s="13"/>
-      <c r="W46" s="13"/>
-      <c r="X46" s="13"/>
-      <c r="Y46" s="13"/>
-      <c r="Z46" s="13"/>
-      <c r="AA46" s="13"/>
-      <c r="AB46" s="13"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="B47" s="28"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="E47" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="F47" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G47" s="29" t="n">
-        <v>8</v>
-      </c>
-      <c r="H47" s="16"/>
       <c r="I47" s="13"/>
       <c r="J47" s="13"/>
       <c r="K47" s="13"/>
@@ -2935,175 +2888,174 @@
       <c r="AB47" s="13"/>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="16" t="s">
+      <c r="A48" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="B48" s="29"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="F48" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G48" s="23" t="n">
+        <v>30</v>
+      </c>
+      <c r="H48" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="13"/>
+      <c r="N48" s="13"/>
+      <c r="O48" s="13"/>
+      <c r="P48" s="13"/>
+      <c r="Q48" s="13"/>
+      <c r="R48" s="13"/>
+      <c r="S48" s="13"/>
+      <c r="T48" s="13"/>
+      <c r="U48" s="13"/>
+      <c r="V48" s="13"/>
+      <c r="W48" s="13"/>
+      <c r="X48" s="13"/>
+      <c r="Y48" s="13"/>
+      <c r="Z48" s="13"/>
+      <c r="AA48" s="13"/>
+      <c r="AB48" s="13"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="B49" s="29"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="16" t="s">
+      <c r="E49" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="E48" s="16" t="s">
+      <c r="F49" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G49" s="30" t="n">
+        <v>8</v>
+      </c>
+      <c r="H49" s="16"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="13"/>
+      <c r="N49" s="13"/>
+      <c r="O49" s="13"/>
+      <c r="P49" s="13"/>
+      <c r="Q49" s="13"/>
+      <c r="R49" s="13"/>
+      <c r="S49" s="13"/>
+      <c r="T49" s="13"/>
+      <c r="U49" s="13"/>
+      <c r="V49" s="13"/>
+      <c r="W49" s="13"/>
+      <c r="X49" s="13"/>
+      <c r="Y49" s="13"/>
+      <c r="Z49" s="13"/>
+      <c r="AA49" s="13"/>
+      <c r="AB49" s="13"/>
+    </row>
+    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="F48" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G48" s="19" t="n">
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="F50" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G50" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="H48" s="20" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="10"/>
-    </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="10"/>
+      <c r="H50" s="20" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="27"/>
-      <c r="B51" s="27"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="27"/>
-      <c r="G51" s="27"/>
-      <c r="H51" s="27"/>
-      <c r="I51" s="27"/>
-      <c r="J51" s="27"/>
-      <c r="K51" s="27"/>
-      <c r="L51" s="27"/>
-      <c r="M51" s="27"/>
-      <c r="N51" s="27"/>
-      <c r="O51" s="27"/>
-      <c r="P51" s="27"/>
-      <c r="Q51" s="27"/>
-      <c r="R51" s="27"/>
-      <c r="S51" s="27"/>
-      <c r="T51" s="27"/>
-      <c r="U51" s="27"/>
-      <c r="V51" s="27"/>
-      <c r="W51" s="27"/>
-      <c r="X51" s="27"/>
-      <c r="Y51" s="27"/>
-      <c r="Z51" s="27"/>
-      <c r="AA51" s="27"/>
-      <c r="AB51" s="27"/>
+      <c r="A51" s="10"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="D52" s="11"/>
+      <c r="A52" s="10"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="12" t="s">
+      <c r="A53" s="28"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="28"/>
+      <c r="G53" s="28"/>
+      <c r="H53" s="28"/>
+      <c r="I53" s="28"/>
+      <c r="J53" s="28"/>
+      <c r="K53" s="28"/>
+      <c r="L53" s="28"/>
+      <c r="M53" s="28"/>
+      <c r="N53" s="28"/>
+      <c r="O53" s="28"/>
+      <c r="P53" s="28"/>
+      <c r="Q53" s="28"/>
+      <c r="R53" s="28"/>
+      <c r="S53" s="28"/>
+      <c r="T53" s="28"/>
+      <c r="U53" s="28"/>
+      <c r="V53" s="28"/>
+      <c r="W53" s="28"/>
+      <c r="X53" s="28"/>
+      <c r="Y53" s="28"/>
+      <c r="Z53" s="28"/>
+      <c r="AA53" s="28"/>
+      <c r="AB53" s="28"/>
+    </row>
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D54" s="11"/>
+    </row>
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="13"/>
-      <c r="C53" s="12" t="s">
+      <c r="B55" s="13"/>
+      <c r="C55" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D55" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E53" s="12" t="s">
+      <c r="E55" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F53" s="14" t="s">
+      <c r="F55" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G53" s="15" t="s">
+      <c r="G55" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H53" s="12" t="s">
+      <c r="H55" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I53" s="13"/>
-      <c r="J53" s="13"/>
-      <c r="K53" s="13"/>
-      <c r="L53" s="13"/>
-      <c r="M53" s="13"/>
-      <c r="N53" s="13"/>
-      <c r="O53" s="13"/>
-      <c r="P53" s="13"/>
-      <c r="Q53" s="13"/>
-      <c r="R53" s="13"/>
-      <c r="S53" s="13"/>
-      <c r="T53" s="13"/>
-      <c r="U53" s="13"/>
-      <c r="V53" s="13"/>
-      <c r="W53" s="13"/>
-      <c r="X53" s="13"/>
-      <c r="Y53" s="13"/>
-      <c r="Z53" s="13"/>
-      <c r="AA53" s="13"/>
-      <c r="AB53" s="13"/>
-    </row>
-    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="B54" s="16"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="E54" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="F54" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G54" s="23" t="n">
-        <v>38</v>
-      </c>
-      <c r="H54" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="I54" s="25"/>
-      <c r="J54" s="13"/>
-      <c r="K54" s="13"/>
-      <c r="L54" s="13"/>
-      <c r="M54" s="13"/>
-      <c r="N54" s="13"/>
-      <c r="O54" s="13"/>
-      <c r="P54" s="13"/>
-      <c r="Q54" s="13"/>
-      <c r="R54" s="13"/>
-      <c r="S54" s="13"/>
-      <c r="T54" s="13"/>
-      <c r="U54" s="13"/>
-      <c r="V54" s="13"/>
-      <c r="W54" s="13"/>
-      <c r="X54" s="13"/>
-      <c r="Y54" s="13"/>
-      <c r="Z54" s="13"/>
-    </row>
-    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="B55" s="16"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="E55" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="F55" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G55" s="23" t="n">
-        <v>72</v>
-      </c>
-      <c r="H55" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="I55" s="25"/>
+      <c r="I55" s="13"/>
       <c r="J55" s="13"/>
       <c r="K55" s="13"/>
       <c r="L55" s="13"/>
@@ -3121,30 +3073,32 @@
       <c r="X55" s="13"/>
       <c r="Y55" s="13"/>
       <c r="Z55" s="13"/>
+      <c r="AA55" s="13"/>
+      <c r="AB55" s="13"/>
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="16" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B56" s="16"/>
       <c r="C56" s="16"/>
       <c r="D56" s="16" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F56" s="22" t="n">
         <v>1</v>
       </c>
       <c r="G56" s="23" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H56" s="24" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I56" s="25"/>
-      <c r="J56" s="25"/>
+      <c r="J56" s="13"/>
       <c r="K56" s="13"/>
       <c r="L56" s="13"/>
       <c r="M56" s="13"/>
@@ -3164,406 +3118,402 @@
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
+        <v>135</v>
+      </c>
+      <c r="B57" s="16"/>
+      <c r="C57" s="16"/>
       <c r="D57" s="16" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E57" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="F57" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G57" s="19" t="n">
-        <v>30</v>
-      </c>
-      <c r="H57" s="20" t="s">
-        <v>141</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="F57" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G57" s="23" t="n">
+        <v>72</v>
+      </c>
+      <c r="H57" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="I57" s="25"/>
+      <c r="J57" s="13"/>
+      <c r="K57" s="13"/>
+      <c r="L57" s="13"/>
+      <c r="M57" s="13"/>
+      <c r="N57" s="13"/>
+      <c r="O57" s="13"/>
+      <c r="P57" s="13"/>
+      <c r="Q57" s="13"/>
+      <c r="R57" s="13"/>
+      <c r="S57" s="13"/>
+      <c r="T57" s="13"/>
+      <c r="U57" s="13"/>
+      <c r="V57" s="13"/>
+      <c r="W57" s="13"/>
+      <c r="X57" s="13"/>
+      <c r="Y57" s="13"/>
+      <c r="Z57" s="13"/>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="B58" s="17"/>
-      <c r="C58" s="17"/>
+        <v>137</v>
+      </c>
+      <c r="B58" s="16"/>
+      <c r="C58" s="16"/>
       <c r="D58" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E58" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="F58" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G58" s="23" t="n">
+        <v>40</v>
+      </c>
+      <c r="H58" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="E58" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="F58" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G58" s="19" t="n">
-        <v>12</v>
-      </c>
-      <c r="H58" s="20" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="16"/>
+      <c r="I58" s="25"/>
+      <c r="J58" s="25"/>
+      <c r="K58" s="13"/>
+      <c r="L58" s="13"/>
+      <c r="M58" s="13"/>
+      <c r="N58" s="13"/>
+      <c r="O58" s="13"/>
+      <c r="P58" s="13"/>
+      <c r="Q58" s="13"/>
+      <c r="R58" s="13"/>
+      <c r="S58" s="13"/>
+      <c r="T58" s="13"/>
+      <c r="U58" s="13"/>
+      <c r="V58" s="13"/>
+      <c r="W58" s="13"/>
+      <c r="X58" s="13"/>
+      <c r="Y58" s="13"/>
+      <c r="Z58" s="13"/>
+    </row>
+    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="16" t="s">
+        <v>140</v>
+      </c>
       <c r="B59" s="17"/>
       <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D59" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="E59" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="F59" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G59" s="19" t="n">
+        <v>30</v>
+      </c>
+      <c r="H59" s="20" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B60" s="17"/>
       <c r="C60" s="17"/>
-      <c r="D60" s="17" t="s">
+      <c r="D60" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="E60" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="F60" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" s="19" t="n">
+        <v>12</v>
+      </c>
+      <c r="H60" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="E60" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="F60" s="17" t="n">
-        <v>2</v>
-      </c>
-      <c r="G60" s="19" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="H60" s="17"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="16" t="s">
-        <v>148</v>
-      </c>
+      <c r="A61" s="16"/>
       <c r="B61" s="17"/>
       <c r="C61" s="17"/>
-      <c r="D61" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="E61" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="F61" s="17" t="n">
-        <v>2</v>
-      </c>
-      <c r="G61" s="19" t="n">
-        <v>0.08</v>
-      </c>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="17"/>
       <c r="H61" s="17"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B62" s="17"/>
       <c r="C62" s="17"/>
       <c r="D62" s="17" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E62" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="F62" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="G62" s="19" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="H62" s="17"/>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="16" t="s">
         <v>150</v>
-      </c>
-      <c r="F62" s="17" t="n">
-        <v>4</v>
-      </c>
-      <c r="G62" s="19" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="H62" s="17"/>
-    </row>
-    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="16" t="s">
-        <v>151</v>
       </c>
       <c r="B63" s="17"/>
       <c r="C63" s="17"/>
       <c r="D63" s="17" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E63" s="17" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F63" s="17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G63" s="19" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="H63" s="32" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.08</v>
+      </c>
+      <c r="H63" s="17"/>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="16" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B64" s="17"/>
       <c r="C64" s="17"/>
       <c r="D64" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E64" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="E64" s="17" t="s">
-        <v>156</v>
-      </c>
       <c r="F64" s="17" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G64" s="19" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H64" s="32" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.14</v>
+      </c>
+      <c r="H64" s="17"/>
+    </row>
+    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="16" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B65" s="17"/>
       <c r="C65" s="17"/>
-      <c r="D65" s="17"/>
+      <c r="D65" s="17" t="s">
+        <v>154</v>
+      </c>
       <c r="E65" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F65" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="G65" s="19" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="H65" s="32" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B66" s="17"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="E66" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="F66" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="G66" s="19" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="H66" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="F65" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G65" s="19" t="n">
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B67" s="17"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="F67" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="G67" s="19" t="n">
         <v>0.14</v>
       </c>
-      <c r="H65" s="16"/>
-    </row>
-    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="26"/>
-    </row>
-    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="27"/>
-      <c r="B67" s="27"/>
-      <c r="C67" s="27"/>
-      <c r="D67" s="27"/>
-      <c r="E67" s="27"/>
-      <c r="F67" s="27"/>
-      <c r="G67" s="27"/>
-      <c r="H67" s="27"/>
-      <c r="I67" s="27"/>
-      <c r="J67" s="27"/>
-      <c r="K67" s="27"/>
-      <c r="L67" s="27"/>
-      <c r="M67" s="27"/>
-      <c r="N67" s="27"/>
-      <c r="O67" s="27"/>
-      <c r="P67" s="27"/>
-      <c r="Q67" s="27"/>
-      <c r="R67" s="27"/>
-      <c r="S67" s="27"/>
-      <c r="T67" s="27"/>
-      <c r="U67" s="27"/>
-      <c r="V67" s="27"/>
-      <c r="W67" s="27"/>
-      <c r="X67" s="27"/>
-      <c r="Y67" s="27"/>
-      <c r="Z67" s="27"/>
-      <c r="AA67" s="27"/>
-      <c r="AB67" s="27"/>
+      <c r="H67" s="16"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="10" t="s">
-        <v>160</v>
-      </c>
+      <c r="A68" s="27"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="12" t="s">
+      <c r="A69" s="28"/>
+      <c r="B69" s="28"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="28"/>
+      <c r="E69" s="28"/>
+      <c r="F69" s="28"/>
+      <c r="G69" s="28"/>
+      <c r="H69" s="28"/>
+      <c r="I69" s="28"/>
+      <c r="J69" s="28"/>
+      <c r="K69" s="28"/>
+      <c r="L69" s="28"/>
+      <c r="M69" s="28"/>
+      <c r="N69" s="28"/>
+      <c r="O69" s="28"/>
+      <c r="P69" s="28"/>
+      <c r="Q69" s="28"/>
+      <c r="R69" s="28"/>
+      <c r="S69" s="28"/>
+      <c r="T69" s="28"/>
+      <c r="U69" s="28"/>
+      <c r="V69" s="28"/>
+      <c r="W69" s="28"/>
+      <c r="X69" s="28"/>
+      <c r="Y69" s="28"/>
+      <c r="Z69" s="28"/>
+      <c r="AA69" s="28"/>
+      <c r="AB69" s="28"/>
+    </row>
+    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B69" s="13"/>
-      <c r="C69" s="12" t="s">
+      <c r="B71" s="13"/>
+      <c r="C71" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D69" s="12" t="s">
+      <c r="D71" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E69" s="12" t="s">
+      <c r="E71" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F69" s="14" t="s">
+      <c r="F71" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G69" s="15" t="s">
+      <c r="G71" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H69" s="12" t="s">
+      <c r="H71" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I69" s="13"/>
-      <c r="J69" s="13"/>
-      <c r="K69" s="13"/>
-      <c r="L69" s="13"/>
-      <c r="M69" s="13"/>
-      <c r="N69" s="13"/>
-      <c r="O69" s="13"/>
-      <c r="P69" s="13"/>
-      <c r="Q69" s="13"/>
-      <c r="R69" s="13"/>
-      <c r="S69" s="13"/>
-      <c r="T69" s="13"/>
-      <c r="U69" s="13"/>
-      <c r="V69" s="13"/>
-      <c r="W69" s="13"/>
-      <c r="X69" s="13"/>
-      <c r="Y69" s="13"/>
-      <c r="Z69" s="13"/>
-      <c r="AA69" s="13"/>
-      <c r="AB69" s="13"/>
-    </row>
-    <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="C70" s="17"/>
-      <c r="D70" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E70" s="33"/>
-      <c r="F70" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G70" s="19" t="n">
-        <v>7</v>
-      </c>
-      <c r="H70" s="30" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="C71" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="D71" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="E71" s="17"/>
-      <c r="F71" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="G71" s="31" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="H71" s="20" t="s">
-        <v>165</v>
-      </c>
+      <c r="I71" s="13"/>
+      <c r="J71" s="13"/>
+      <c r="K71" s="13"/>
+      <c r="L71" s="13"/>
+      <c r="M71" s="13"/>
+      <c r="N71" s="13"/>
+      <c r="O71" s="13"/>
+      <c r="P71" s="13"/>
+      <c r="Q71" s="13"/>
+      <c r="R71" s="13"/>
+      <c r="S71" s="13"/>
+      <c r="T71" s="13"/>
+      <c r="U71" s="13"/>
+      <c r="V71" s="13"/>
+      <c r="W71" s="13"/>
+      <c r="X71" s="13"/>
+      <c r="Y71" s="13"/>
+      <c r="Z71" s="13"/>
+      <c r="AA71" s="13"/>
+      <c r="AB71" s="13"/>
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="B72" s="13"/>
-      <c r="C72" s="21" t="s">
-        <v>76</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="C72" s="17"/>
       <c r="D72" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="E72" s="16"/>
-      <c r="F72" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G72" s="31" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="H72" s="34" t="s">
-        <v>167</v>
-      </c>
-      <c r="I72" s="13"/>
-      <c r="J72" s="13"/>
-      <c r="K72" s="13"/>
-      <c r="L72" s="13"/>
-      <c r="M72" s="13"/>
-      <c r="N72" s="13"/>
-      <c r="O72" s="13"/>
-      <c r="P72" s="13"/>
-      <c r="Q72" s="13"/>
-      <c r="R72" s="13"/>
-      <c r="S72" s="13"/>
-      <c r="T72" s="13"/>
-      <c r="U72" s="13"/>
-      <c r="V72" s="13"/>
-      <c r="W72" s="13"/>
-      <c r="X72" s="13"/>
-      <c r="Y72" s="13"/>
-      <c r="Z72" s="13"/>
-      <c r="AA72" s="13"/>
-      <c r="AB72" s="13"/>
+        <v>74</v>
+      </c>
+      <c r="E72" s="33"/>
+      <c r="F72" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G72" s="19" t="n">
+        <v>7</v>
+      </c>
+      <c r="H72" s="26" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="B73" s="13"/>
+        <v>165</v>
+      </c>
       <c r="C73" s="21" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D73" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="E73" s="16"/>
-      <c r="F73" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G73" s="29" t="n">
-        <v>0.34</v>
-      </c>
-      <c r="H73" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="I73" s="13"/>
-      <c r="J73" s="13"/>
-      <c r="K73" s="13"/>
-      <c r="L73" s="13"/>
-      <c r="M73" s="13"/>
-      <c r="N73" s="13"/>
-      <c r="O73" s="13"/>
-      <c r="P73" s="13"/>
-      <c r="Q73" s="13"/>
-      <c r="R73" s="13"/>
-      <c r="S73" s="13"/>
-      <c r="T73" s="13"/>
-      <c r="U73" s="13"/>
-      <c r="V73" s="13"/>
-      <c r="W73" s="13"/>
-      <c r="X73" s="13"/>
-      <c r="Y73" s="13"/>
-      <c r="Z73" s="13"/>
-      <c r="AA73" s="13"/>
-      <c r="AB73" s="13"/>
+        <v>79</v>
+      </c>
+      <c r="E73" s="17"/>
+      <c r="F73" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="G73" s="31" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="H73" s="20" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="16" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B74" s="13"/>
       <c r="C74" s="21" t="s">
-        <v>172</v>
+        <v>78</v>
       </c>
       <c r="D74" s="16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E74" s="16"/>
       <c r="F74" s="22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G74" s="31" t="n">
         <v>0.1</v>
       </c>
-      <c r="H74" s="35" t="s">
-        <v>173</v>
+      <c r="H74" s="34" t="s">
+        <v>169</v>
       </c>
       <c r="I74" s="13"/>
       <c r="J74" s="13"/>
@@ -3588,24 +3538,24 @@
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="16" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B75" s="13"/>
       <c r="C75" s="21" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E75" s="16"/>
       <c r="F75" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="G75" s="31" t="n">
+      <c r="G75" s="30" t="n">
         <v>0.34</v>
       </c>
       <c r="H75" s="34" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="I75" s="13"/>
       <c r="J75" s="13"/>
@@ -3630,24 +3580,24 @@
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="16" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B76" s="13"/>
       <c r="C76" s="21" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D76" s="16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E76" s="16"/>
       <c r="F76" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G76" s="29" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="H76" s="34" t="s">
-        <v>179</v>
+        <v>2</v>
+      </c>
+      <c r="G76" s="31" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H76" s="35" t="s">
+        <v>175</v>
       </c>
       <c r="I76" s="13"/>
       <c r="J76" s="13"/>
@@ -3671,25 +3621,25 @@
       <c r="AB76" s="13"/>
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="36" t="s">
-        <v>180</v>
+      <c r="A77" s="16" t="s">
+        <v>176</v>
       </c>
       <c r="B77" s="13"/>
-      <c r="C77" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="D77" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="E77" s="17"/>
-      <c r="F77" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G77" s="29" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="H77" s="20" t="s">
-        <v>182</v>
+      <c r="C77" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="D77" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E77" s="16"/>
+      <c r="F77" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G77" s="31" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="H77" s="34" t="s">
+        <v>178</v>
       </c>
       <c r="I77" s="13"/>
       <c r="J77" s="13"/>
@@ -3713,50 +3663,71 @@
       <c r="AB77" s="13"/>
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="36" t="s">
+      <c r="A78" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B78" s="13"/>
+      <c r="C78" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="D78" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E78" s="16"/>
+      <c r="F78" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G78" s="30" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="H78" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="I78" s="13"/>
+      <c r="J78" s="13"/>
+      <c r="K78" s="13"/>
+      <c r="L78" s="13"/>
+      <c r="M78" s="13"/>
+      <c r="N78" s="13"/>
+      <c r="O78" s="13"/>
+      <c r="P78" s="13"/>
+      <c r="Q78" s="13"/>
+      <c r="R78" s="13"/>
+      <c r="S78" s="13"/>
+      <c r="T78" s="13"/>
+      <c r="U78" s="13"/>
+      <c r="V78" s="13"/>
+      <c r="W78" s="13"/>
+      <c r="X78" s="13"/>
+      <c r="Y78" s="13"/>
+      <c r="Z78" s="13"/>
+      <c r="AA78" s="13"/>
+      <c r="AB78" s="13"/>
+    </row>
+    <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="B79" s="13"/>
+      <c r="C79" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="C78" s="36" t="s">
+      <c r="D79" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E79" s="17"/>
+      <c r="F79" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G79" s="30" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="H79" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="D78" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="E78" s="33"/>
-      <c r="F78" s="22" t="n">
-        <v>2</v>
-      </c>
-      <c r="G78" s="31" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="H78" s="30" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="B79" s="13"/>
-      <c r="C79" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="D79" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="E79" s="17"/>
-      <c r="F79" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G79" s="23" t="n">
-        <v>1.86</v>
-      </c>
-      <c r="H79" s="37" t="s">
-        <v>188</v>
-      </c>
-      <c r="I79" s="25"/>
-      <c r="J79" s="25"/>
-      <c r="K79" s="25"/>
+      <c r="I79" s="13"/>
+      <c r="J79" s="13"/>
+      <c r="K79" s="13"/>
       <c r="L79" s="13"/>
       <c r="M79" s="13"/>
       <c r="N79" s="13"/>
@@ -3772,65 +3743,50 @@
       <c r="X79" s="13"/>
       <c r="Y79" s="13"/>
       <c r="Z79" s="13"/>
+      <c r="AA79" s="13"/>
+      <c r="AB79" s="13"/>
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="B80" s="13"/>
-      <c r="C80" s="18" t="s">
-        <v>190</v>
+      <c r="A80" s="36" t="s">
+        <v>185</v>
+      </c>
+      <c r="C80" s="36" t="s">
+        <v>186</v>
       </c>
       <c r="D80" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="E80" s="17"/>
+        <v>79</v>
+      </c>
+      <c r="E80" s="33"/>
       <c r="F80" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G80" s="29" t="n">
-        <v>2.64</v>
-      </c>
-      <c r="H80" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="I80" s="25"/>
-      <c r="J80" s="25"/>
-      <c r="K80" s="25"/>
-      <c r="L80" s="25"/>
-      <c r="M80" s="13"/>
-      <c r="N80" s="13"/>
-      <c r="O80" s="13"/>
-      <c r="P80" s="13"/>
-      <c r="Q80" s="13"/>
-      <c r="R80" s="13"/>
-      <c r="S80" s="13"/>
-      <c r="T80" s="13"/>
-      <c r="U80" s="13"/>
-      <c r="V80" s="13"/>
-      <c r="W80" s="13"/>
-      <c r="X80" s="13"/>
-      <c r="Y80" s="13"/>
-      <c r="Z80" s="13"/>
+        <v>2</v>
+      </c>
+      <c r="G80" s="31" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="H80" s="26" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B81" s="13"/>
       <c r="C81" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="D81" s="17"/>
-      <c r="E81" s="16"/>
+        <v>189</v>
+      </c>
+      <c r="D81" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E81" s="17"/>
       <c r="F81" s="22" t="n">
         <v>1</v>
       </c>
       <c r="G81" s="23" t="n">
-        <v>1.81</v>
+        <v>1.86</v>
       </c>
       <c r="H81" s="37" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I81" s="25"/>
       <c r="J81" s="25"/>
@@ -3853,39 +3809,66 @@
     </row>
     <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="C82" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="D82" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="E82" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="B82" s="13"/>
+      <c r="C82" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="D82" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E82" s="17"/>
+      <c r="F82" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G82" s="30" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="H82" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="I82" s="25"/>
+      <c r="J82" s="25"/>
+      <c r="K82" s="25"/>
+      <c r="L82" s="25"/>
+      <c r="M82" s="13"/>
+      <c r="N82" s="13"/>
+      <c r="O82" s="13"/>
+      <c r="P82" s="13"/>
+      <c r="Q82" s="13"/>
+      <c r="R82" s="13"/>
+      <c r="S82" s="13"/>
+      <c r="T82" s="13"/>
+      <c r="U82" s="13"/>
+      <c r="V82" s="13"/>
+      <c r="W82" s="13"/>
+      <c r="X82" s="13"/>
+      <c r="Y82" s="13"/>
+      <c r="Z82" s="13"/>
+    </row>
+    <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="B83" s="13"/>
+      <c r="C83" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="F82" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G82" s="29" t="n">
-        <v>1.07</v>
-      </c>
-      <c r="H82" s="20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="16"/>
-      <c r="B83" s="13"/>
-      <c r="C83" s="21"/>
-      <c r="D83" s="16"/>
+      <c r="D83" s="17"/>
       <c r="E83" s="16"/>
-      <c r="F83" s="22"/>
-      <c r="G83" s="23"/>
-      <c r="H83" s="34"/>
-      <c r="I83" s="13"/>
-      <c r="J83" s="13"/>
-      <c r="K83" s="13"/>
+      <c r="F83" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G83" s="23" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="H83" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="I83" s="25"/>
+      <c r="J83" s="25"/>
+      <c r="K83" s="25"/>
       <c r="L83" s="13"/>
       <c r="M83" s="13"/>
       <c r="N83" s="13"/>
@@ -3901,85 +3884,44 @@
       <c r="X83" s="13"/>
       <c r="Y83" s="13"/>
       <c r="Z83" s="13"/>
-      <c r="AA83" s="13"/>
-      <c r="AB83" s="13"/>
     </row>
     <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="B84" s="13" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="C84" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D84" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E84" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="D84" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="E84" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="F84" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G84" s="23" t="n">
-        <v>16</v>
-      </c>
-      <c r="H84" s="24" t="s">
-        <v>198</v>
-      </c>
-      <c r="I84" s="25"/>
-      <c r="J84" s="25"/>
-      <c r="K84" s="25"/>
-      <c r="L84" s="25"/>
-      <c r="M84" s="25"/>
-      <c r="N84" s="13"/>
-      <c r="O84" s="13"/>
-      <c r="P84" s="13"/>
-      <c r="Q84" s="13"/>
-      <c r="R84" s="13"/>
-      <c r="S84" s="13"/>
-      <c r="T84" s="13"/>
-      <c r="U84" s="13"/>
-      <c r="V84" s="13"/>
-      <c r="W84" s="13"/>
-      <c r="X84" s="13"/>
-      <c r="Y84" s="13"/>
-      <c r="Z84" s="13"/>
-      <c r="AA84" s="13"/>
-      <c r="AB84" s="13"/>
-    </row>
-    <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="B85" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C85" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="D85" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="E85" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="F85" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G85" s="23" t="n">
-        <v>16</v>
-      </c>
-      <c r="H85" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="I85" s="25"/>
-      <c r="J85" s="25"/>
-      <c r="K85" s="25"/>
-      <c r="L85" s="25"/>
-      <c r="M85" s="25"/>
+      <c r="F84" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G84" s="30" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="H84" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="16"/>
+      <c r="B85" s="13"/>
+      <c r="C85" s="21"/>
+      <c r="D85" s="16"/>
+      <c r="E85" s="16"/>
+      <c r="F85" s="22"/>
+      <c r="G85" s="23"/>
+      <c r="H85" s="34"/>
+      <c r="I85" s="13"/>
+      <c r="J85" s="13"/>
+      <c r="K85" s="13"/>
+      <c r="L85" s="13"/>
+      <c r="M85" s="13"/>
       <c r="N85" s="13"/>
       <c r="O85" s="13"/>
       <c r="P85" s="13"/>
@@ -3998,26 +3940,28 @@
     </row>
     <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="B86" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C86" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="D86" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E86" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="B86" s="13"/>
-      <c r="C86" s="38" t="s">
+      <c r="F86" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G86" s="23" t="n">
+        <v>16</v>
+      </c>
+      <c r="H86" s="24" t="s">
         <v>200</v>
-      </c>
-      <c r="D86" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="E86" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="F86" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G86" s="23" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="H86" s="39" t="s">
-        <v>202</v>
       </c>
       <c r="I86" s="25"/>
       <c r="J86" s="25"/>
@@ -4042,26 +3986,28 @@
     </row>
     <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="B87" s="13"/>
-      <c r="C87" s="38" t="s">
-        <v>204</v>
+        <v>114</v>
+      </c>
+      <c r="B87" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C87" s="21" t="s">
+        <v>116</v>
       </c>
       <c r="D87" s="16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E87" s="16" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F87" s="22" t="n">
         <v>1</v>
       </c>
       <c r="G87" s="23" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="H87" s="39" t="s">
-        <v>205</v>
+        <v>16</v>
+      </c>
+      <c r="H87" s="24" t="s">
+        <v>118</v>
       </c>
       <c r="I87" s="25"/>
       <c r="J87" s="25"/>
@@ -4084,78 +4030,140 @@
       <c r="AA87" s="13"/>
       <c r="AB87" s="13"/>
     </row>
-    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="17"/>
-      <c r="C88" s="17"/>
-      <c r="D88" s="17"/>
-      <c r="E88" s="17"/>
-      <c r="F88" s="17"/>
-      <c r="G88" s="17"/>
-      <c r="H88" s="17"/>
-    </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="B88" s="13"/>
+      <c r="C88" s="38" t="s">
+        <v>202</v>
+      </c>
+      <c r="D88" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E88" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="F88" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G88" s="23" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="H88" s="39" t="s">
+        <v>204</v>
+      </c>
+      <c r="I88" s="25"/>
+      <c r="J88" s="25"/>
+      <c r="K88" s="25"/>
+      <c r="L88" s="25"/>
+      <c r="M88" s="25"/>
+      <c r="N88" s="13"/>
+      <c r="O88" s="13"/>
+      <c r="P88" s="13"/>
+      <c r="Q88" s="13"/>
+      <c r="R88" s="13"/>
+      <c r="S88" s="13"/>
+      <c r="T88" s="13"/>
+      <c r="U88" s="13"/>
+      <c r="V88" s="13"/>
+      <c r="W88" s="13"/>
+      <c r="X88" s="13"/>
+      <c r="Y88" s="13"/>
+      <c r="Z88" s="13"/>
+      <c r="AA88" s="13"/>
+      <c r="AB88" s="13"/>
+    </row>
+    <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="B89" s="13"/>
+      <c r="C89" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="C89" s="17"/>
-      <c r="D89" s="17" t="s">
+      <c r="D89" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E89" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="F89" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G89" s="23" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="H89" s="39" t="s">
         <v>207</v>
       </c>
-      <c r="E89" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="F89" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G89" s="17"/>
-      <c r="H89" s="17"/>
-    </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="16" t="s">
-        <v>209</v>
-      </c>
+      <c r="I89" s="25"/>
+      <c r="J89" s="25"/>
+      <c r="K89" s="25"/>
+      <c r="L89" s="25"/>
+      <c r="M89" s="25"/>
+      <c r="N89" s="13"/>
+      <c r="O89" s="13"/>
+      <c r="P89" s="13"/>
+      <c r="Q89" s="13"/>
+      <c r="R89" s="13"/>
+      <c r="S89" s="13"/>
+      <c r="T89" s="13"/>
+      <c r="U89" s="13"/>
+      <c r="V89" s="13"/>
+      <c r="W89" s="13"/>
+      <c r="X89" s="13"/>
+      <c r="Y89" s="13"/>
+      <c r="Z89" s="13"/>
+      <c r="AA89" s="13"/>
+      <c r="AB89" s="13"/>
+    </row>
+    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A90" s="17"/>
       <c r="C90" s="17"/>
-      <c r="D90" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="E90" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="F90" s="16" t="n">
-        <v>1</v>
-      </c>
+      <c r="D90" s="17"/>
+      <c r="E90" s="17"/>
+      <c r="F90" s="17"/>
       <c r="G90" s="17"/>
       <c r="H90" s="17"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="16" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C91" s="17"/>
-      <c r="D91" s="17"/>
+      <c r="D91" s="17" t="s">
+        <v>209</v>
+      </c>
       <c r="E91" s="17" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F91" s="16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G91" s="17"/>
       <c r="H91" s="17"/>
     </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C92" s="17"/>
-      <c r="D92" s="17"/>
+      <c r="D92" s="17" t="s">
+        <v>154</v>
+      </c>
       <c r="E92" s="17" t="s">
         <v>212</v>
       </c>
       <c r="F92" s="16" t="n">
-        <v>2</v>
-      </c>
-      <c r="G92" s="17"/>
-      <c r="H92" s="17"/>
+        <v>1</v>
+      </c>
+      <c r="G92" s="40" t="n">
+        <v>9.21</v>
+      </c>
+      <c r="H92" s="17" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="16" t="s">
@@ -4163,7 +4171,7 @@
       </c>
       <c r="C93" s="17"/>
       <c r="D93" s="17" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="E93" s="17" t="s">
         <v>215</v>
@@ -4266,10 +4274,10 @@
       </c>
       <c r="C98" s="17"/>
       <c r="D98" s="16" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="E98" s="16" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F98" s="16" t="n">
         <v>1</v>
@@ -4287,10 +4295,10 @@
       </c>
       <c r="C99" s="17"/>
       <c r="D99" s="16" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="E99" s="16" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F99" s="16" t="n">
         <v>1</v>
@@ -4303,34 +4311,34 @@
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="27"/>
-      <c r="B101" s="27"/>
-      <c r="C101" s="27"/>
-      <c r="D101" s="27"/>
-      <c r="E101" s="27"/>
-      <c r="F101" s="27"/>
-      <c r="G101" s="27"/>
-      <c r="H101" s="27"/>
-      <c r="I101" s="27"/>
-      <c r="J101" s="27"/>
-      <c r="K101" s="27"/>
-      <c r="L101" s="27"/>
-      <c r="M101" s="27"/>
-      <c r="N101" s="27"/>
-      <c r="O101" s="27"/>
-      <c r="P101" s="27"/>
-      <c r="Q101" s="27"/>
-      <c r="R101" s="27"/>
-      <c r="S101" s="27"/>
-      <c r="T101" s="27"/>
-      <c r="U101" s="27"/>
-      <c r="V101" s="27"/>
-      <c r="W101" s="27"/>
-      <c r="X101" s="27"/>
-      <c r="Y101" s="27"/>
-      <c r="Z101" s="27"/>
-      <c r="AA101" s="27"/>
-      <c r="AB101" s="27"/>
+      <c r="A101" s="28"/>
+      <c r="B101" s="28"/>
+      <c r="C101" s="28"/>
+      <c r="D101" s="28"/>
+      <c r="E101" s="28"/>
+      <c r="F101" s="28"/>
+      <c r="G101" s="28"/>
+      <c r="H101" s="28"/>
+      <c r="I101" s="28"/>
+      <c r="J101" s="28"/>
+      <c r="K101" s="28"/>
+      <c r="L101" s="28"/>
+      <c r="M101" s="28"/>
+      <c r="N101" s="28"/>
+      <c r="O101" s="28"/>
+      <c r="P101" s="28"/>
+      <c r="Q101" s="28"/>
+      <c r="R101" s="28"/>
+      <c r="S101" s="28"/>
+      <c r="T101" s="28"/>
+      <c r="U101" s="28"/>
+      <c r="V101" s="28"/>
+      <c r="W101" s="28"/>
+      <c r="X101" s="28"/>
+      <c r="Y101" s="28"/>
+      <c r="Z101" s="28"/>
+      <c r="AA101" s="28"/>
+      <c r="AB101" s="28"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="10" t="s">
@@ -4390,13 +4398,13 @@
         <v>229</v>
       </c>
       <c r="D104" s="21" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E104" s="16"/>
       <c r="F104" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="G104" s="29" t="n">
+      <c r="G104" s="30" t="n">
         <v>1.06</v>
       </c>
       <c r="H104" s="20" t="s">
@@ -4412,13 +4420,13 @@
         <v>232</v>
       </c>
       <c r="D105" s="21" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E105" s="16"/>
       <c r="F105" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="G105" s="29" t="n">
+      <c r="G105" s="30" t="n">
         <v>5.31</v>
       </c>
       <c r="H105" s="20" t="s">
@@ -4431,20 +4439,20 @@
       </c>
       <c r="B106" s="17"/>
       <c r="C106" s="16" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D106" s="21" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E106" s="17"/>
       <c r="F106" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="G106" s="29" t="n">
+      <c r="G106" s="30" t="n">
         <v>0.32</v>
       </c>
       <c r="H106" s="20" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4456,13 +4464,13 @@
         <v>236</v>
       </c>
       <c r="D107" s="21" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E107" s="17"/>
       <c r="F107" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="G107" s="29" t="n">
+      <c r="G107" s="30" t="n">
         <v>0.12</v>
       </c>
       <c r="H107" s="20" t="s">
@@ -4476,7 +4484,7 @@
       <c r="B108" s="17"/>
       <c r="C108" s="17"/>
       <c r="D108" s="16" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E108" s="17"/>
       <c r="F108" s="16" t="n">
@@ -4496,7 +4504,7 @@
       <c r="B109" s="17"/>
       <c r="C109" s="17"/>
       <c r="D109" s="16" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E109" s="17"/>
       <c r="F109" s="16" t="n">
@@ -4518,7 +4526,7 @@
       </c>
       <c r="C110" s="16"/>
       <c r="D110" s="16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E110" s="16" t="s">
         <v>244</v>
@@ -4542,7 +4550,7 @@
       </c>
       <c r="C111" s="16"/>
       <c r="D111" s="16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E111" s="16" t="s">
         <v>244</v>
@@ -4586,7 +4594,7 @@
       </c>
       <c r="C112" s="16"/>
       <c r="D112" s="16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E112" s="16" t="s">
         <v>244</v>
@@ -4628,7 +4636,7 @@
       <c r="B113" s="17"/>
       <c r="C113" s="17"/>
       <c r="D113" s="16" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="E113" s="16" t="s">
         <v>251</v>
@@ -4650,7 +4658,7 @@
       <c r="B114" s="17"/>
       <c r="C114" s="17"/>
       <c r="D114" s="16" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="E114" s="16" t="s">
         <v>254</v>
@@ -4672,7 +4680,7 @@
       <c r="B115" s="17"/>
       <c r="C115" s="17"/>
       <c r="D115" s="16" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="E115" s="16" t="s">
         <v>257</v>
@@ -4716,7 +4724,7 @@
       <c r="B117" s="44"/>
       <c r="C117" s="41"/>
       <c r="D117" s="41" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E117" s="41" t="s">
         <v>263</v>
@@ -4752,37 +4760,37 @@
       <c r="AB117" s="42"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="26"/>
+      <c r="A118" s="27"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="27"/>
-      <c r="B119" s="27"/>
-      <c r="C119" s="27"/>
-      <c r="D119" s="27"/>
-      <c r="E119" s="27"/>
-      <c r="F119" s="27"/>
-      <c r="G119" s="27"/>
-      <c r="H119" s="27"/>
-      <c r="I119" s="27"/>
-      <c r="J119" s="27"/>
-      <c r="K119" s="27"/>
-      <c r="L119" s="27"/>
-      <c r="M119" s="27"/>
-      <c r="N119" s="27"/>
-      <c r="O119" s="27"/>
-      <c r="P119" s="27"/>
-      <c r="Q119" s="27"/>
-      <c r="R119" s="27"/>
-      <c r="S119" s="27"/>
-      <c r="T119" s="27"/>
-      <c r="U119" s="27"/>
-      <c r="V119" s="27"/>
-      <c r="W119" s="27"/>
-      <c r="X119" s="27"/>
-      <c r="Y119" s="27"/>
-      <c r="Z119" s="27"/>
-      <c r="AA119" s="27"/>
-      <c r="AB119" s="27"/>
+      <c r="A119" s="28"/>
+      <c r="B119" s="28"/>
+      <c r="C119" s="28"/>
+      <c r="D119" s="28"/>
+      <c r="E119" s="28"/>
+      <c r="F119" s="28"/>
+      <c r="G119" s="28"/>
+      <c r="H119" s="28"/>
+      <c r="I119" s="28"/>
+      <c r="J119" s="28"/>
+      <c r="K119" s="28"/>
+      <c r="L119" s="28"/>
+      <c r="M119" s="28"/>
+      <c r="N119" s="28"/>
+      <c r="O119" s="28"/>
+      <c r="P119" s="28"/>
+      <c r="Q119" s="28"/>
+      <c r="R119" s="28"/>
+      <c r="S119" s="28"/>
+      <c r="T119" s="28"/>
+      <c r="U119" s="28"/>
+      <c r="V119" s="28"/>
+      <c r="W119" s="28"/>
+      <c r="X119" s="28"/>
+      <c r="Y119" s="28"/>
+      <c r="Z119" s="28"/>
+      <c r="AA119" s="28"/>
+      <c r="AB119" s="28"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="10" t="s">
@@ -4841,7 +4849,7 @@
       <c r="B122" s="17"/>
       <c r="C122" s="17"/>
       <c r="D122" s="16" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E122" s="16" t="s">
         <v>267</v>
@@ -4865,7 +4873,7 @@
         <v>270</v>
       </c>
       <c r="D123" s="16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E123" s="16" t="s">
         <v>271</v>
@@ -4889,7 +4897,7 @@
         <v>274</v>
       </c>
       <c r="D124" s="16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E124" s="16" t="s">
         <v>275</v>
@@ -4913,7 +4921,7 @@
         <v>278</v>
       </c>
       <c r="D125" s="16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E125" s="17"/>
       <c r="F125" s="16" t="n">
@@ -4928,7 +4936,7 @@
     </row>
     <row r="126" s="50" customFormat="true" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="49" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C126" s="49" t="s">
         <v>280</v>
@@ -5013,35 +5021,37 @@
       <c r="AB127" s="42"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="27"/>
-      <c r="B130" s="27"/>
-      <c r="C130" s="27"/>
-      <c r="D130" s="27"/>
-      <c r="E130" s="27"/>
-      <c r="F130" s="27"/>
-      <c r="G130" s="27"/>
-      <c r="H130" s="27"/>
-      <c r="I130" s="27"/>
-      <c r="J130" s="27"/>
-      <c r="K130" s="27"/>
-      <c r="L130" s="27"/>
-      <c r="M130" s="27"/>
-      <c r="N130" s="27"/>
-      <c r="O130" s="27"/>
-      <c r="P130" s="27"/>
-      <c r="Q130" s="27"/>
-      <c r="R130" s="27"/>
-      <c r="S130" s="27"/>
-      <c r="T130" s="27"/>
-      <c r="U130" s="27"/>
-      <c r="V130" s="27"/>
-      <c r="W130" s="27"/>
-      <c r="X130" s="27"/>
-      <c r="Y130" s="27"/>
-      <c r="Z130" s="27"/>
-      <c r="AA130" s="27"/>
-      <c r="AB130" s="27"/>
-    </row>
+      <c r="A130" s="28"/>
+      <c r="B130" s="28"/>
+      <c r="C130" s="28"/>
+      <c r="D130" s="28"/>
+      <c r="E130" s="28"/>
+      <c r="F130" s="28"/>
+      <c r="G130" s="28"/>
+      <c r="H130" s="28"/>
+      <c r="I130" s="28"/>
+      <c r="J130" s="28"/>
+      <c r="K130" s="28"/>
+      <c r="L130" s="28"/>
+      <c r="M130" s="28"/>
+      <c r="N130" s="28"/>
+      <c r="O130" s="28"/>
+      <c r="P130" s="28"/>
+      <c r="Q130" s="28"/>
+      <c r="R130" s="28"/>
+      <c r="S130" s="28"/>
+      <c r="T130" s="28"/>
+      <c r="U130" s="28"/>
+      <c r="V130" s="28"/>
+      <c r="W130" s="28"/>
+      <c r="X130" s="28"/>
+      <c r="Y130" s="28"/>
+      <c r="Z130" s="28"/>
+      <c r="AA130" s="28"/>
+      <c r="AB130" s="28"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H7" r:id="rId1" display="https://www.horizonhobby.com/blackjack-24-inch-catamaran-brushless%3A-rtr-prb08007"/>
@@ -5051,74 +5061,76 @@
     <hyperlink ref="H11" r:id="rId5" display="https://www.amazon.com/Duracell-MN1500-Duralock-Alkaline-Batteries/dp/B003VSCLMI/"/>
     <hyperlink ref="H12" r:id="rId6" display="https://www.amazon.com/STIKK-Painters-Release-Finishing-Masking/dp/B01MYP8R5B"/>
     <hyperlink ref="H13" r:id="rId7" display="https://www.amazon.com/INDUSTRIES-4471-Sandpaper-9-Inch-11-Inch/dp/B001AVYXVU"/>
-    <hyperlink ref="H15" r:id="rId8" display="https://hobbyking.com/en_us/hobbyking-350w-25a-power-supply-100v-120v.html"/>
-    <hyperlink ref="H16" r:id="rId9" display="https://hobbyking.com/en_us/icharger-206b-300w-8s-balance-charger.html"/>
-    <hyperlink ref="H17" r:id="rId10" display="https://www.horizonhobby.com/boats/electric-boats/stealthwake-rtr-23-inch-brushed-deep-v-prb08015"/>
-    <hyperlink ref="H23" r:id="rId11" display="https://www.adafruit.com/product/3133"/>
-    <hyperlink ref="H24" r:id="rId12" display="https://www.adafruit.com/product/380"/>
-    <hyperlink ref="H25" r:id="rId13" display="https://www.adafruit.com/product/392"/>
-    <hyperlink ref="H26" r:id="rId14" display="https://www.adafruit.com/product/2830"/>
-    <hyperlink ref="H27" r:id="rId15" display="https://www.adafruit.com/product/2886"/>
-    <hyperlink ref="H28" r:id="rId16" display="https://www.amazon.com/gp/product/B00NH13O7K"/>
-    <hyperlink ref="H29" r:id="rId17" display="https://www.adafruit.com/product/328"/>
-    <hyperlink ref="H31" r:id="rId18" display="https://github.com/lperovich/seeboat/tree/master/hardware/controlBoard"/>
-    <hyperlink ref="H32" r:id="rId19" display="https://www.digikey.com/products/en?keywords=RNCP0603FTD2K74CT-ND"/>
-    <hyperlink ref="H33" r:id="rId20" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP0603FTD100R/RNCP0603FTD100RCT-ND/2240425"/>
-    <hyperlink ref="H34" r:id="rId21" display="https://www.digikey.com/product-detail/en/AYZ0202AGRLC/401-2013-1-ND/1640122"/>
-    <hyperlink ref="H35" r:id="rId22" display="https://www.adafruit.com/product/2343"/>
-    <hyperlink ref="H36" r:id="rId23" display="https://www.digikey.com/products/en?keywords=WM4802-ND"/>
-    <hyperlink ref="H37" r:id="rId24" display="https://www.digikey.com/products/en?keywords=WM9131-ND"/>
-    <hyperlink ref="H38" r:id="rId25" display="https://www.digikey.com/products/en?keywords=WM4801-ND"/>
-    <hyperlink ref="H39" r:id="rId26" display="https://www.digikey.com/products/en?keywords=WM10647-ND"/>
-    <hyperlink ref="H40" r:id="rId27" display="https://www.digikey.com/product-detail/en/3m/3302-16-300SF/MC16M-100-ND/145737"/>
-    <hyperlink ref="H41" r:id="rId28" display="https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2004A.12.02/C2004W-100-ND/57495"/>
-    <hyperlink ref="H46" r:id="rId29" display="https://www.adafruit.com/product/2240"/>
-    <hyperlink ref="H48" r:id="rId30" display="https://www.tapplastics.com/product/plastics/cut_to_size_plastic/satinice_white/655"/>
-    <hyperlink ref="H54" r:id="rId31" display="https://www.atlas-scientific.com/product_pages/circuits/ezo_ph.html"/>
-    <hyperlink ref="H55" r:id="rId32" display="https://www.atlas-scientific.com/product_pages/probes/ph_probe.html"/>
-    <hyperlink ref="H56" r:id="rId33" display="https://www.atlas-scientific.com/product_pages/components/single_carrier_iso.html"/>
-    <hyperlink ref="H57" r:id="rId34" display="https://www.hach.com/ph-buffer-solution-kit-color-coded-ph-4-01-ph-7-00-and-ph-10-01-500-ml-each/product?id=7640205069"/>
-    <hyperlink ref="H58" r:id="rId35" display="https://www.hach.com/electrolyte-solution-kcl-3m-50ml/product-parameter-reagent?id=7640207762"/>
-    <hyperlink ref="H63" r:id="rId36" display="https://www.mcmaster.com/8972T11"/>
-    <hyperlink ref="H64" r:id="rId37" display="https://www.mcmaster.com/4339T5"/>
-    <hyperlink ref="H70" r:id="rId38" display="https://github.com/lperovich/seeboat/tree/master/hardware/conductivity"/>
-    <hyperlink ref="H71" r:id="rId39" display="https://www.digikey.com/product-detail/en/yageo/AT0603FRE0710KL/YAG2122CT-ND/5139570"/>
-    <hyperlink ref="H72" r:id="rId40" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP0603FTD2K74/RNCP0603FTD2K74CT-ND/2240457"/>
-    <hyperlink ref="H73" r:id="rId41" display="https://www.digikey.com/product-detail/en/yageo/RT0603BRD071ML/YAG4498CT-ND/6616654"/>
-    <hyperlink ref="H74" r:id="rId42" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP0603FTD1K00/RNCP0603FTD1K00CT-ND/2240445"/>
-    <hyperlink ref="H75" r:id="rId43" display="https://www.digikey.com/product-detail/en/yageo/RT0603BRD0742K2L/YAG4556CT-ND/6616712"/>
-    <hyperlink ref="H76" r:id="rId44" display="https://www.digikey.com/product-detail/en/yageo/RT0603DRE071K2L/311-2461-1-ND/6128880"/>
-    <hyperlink ref="H77" r:id="rId45" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X8R1H104K080AB/445-8818-1-ND/3248223"/>
-    <hyperlink ref="H78" r:id="rId46" display="https://www.digikey.com/products/en?keywords=641-1331-1-ND"/>
-    <hyperlink ref="H79" r:id="rId47" display="https://www.digikey.com/product-detail/en/texas-instruments/TLE2426CD/296-6547-5-ND/371934"/>
-    <hyperlink ref="H80" r:id="rId48" display="https://www.digikey.com/product-detail/en/analog-devices-inc/AD8655ARZ-REEL7/AD8655ARZ-REEL7CT-ND/3678589"/>
-    <hyperlink ref="H81" r:id="rId49" display="https://www.digikey.com/product-detail/en/texas-instruments/TLV2374IDR/296-11967-1-ND/390435"/>
-    <hyperlink ref="H82" r:id="rId50" display="https://www.digikey.com/product-detail/en/AYZ0202AGRLC/401-2013-1-ND/1640122"/>
-    <hyperlink ref="H84" r:id="rId51" display="https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2117A.12.06/C2117G-100-ND/16217"/>
-    <hyperlink ref="H85" r:id="rId52" display="https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2004A.12.02/C2004W-100-ND/57495"/>
-    <hyperlink ref="H86" r:id="rId53" display="https://www.digikey.com/products/en?keywords=%09WM4800-ND"/>
-    <hyperlink ref="H87" r:id="rId54" display="https://www.digikey.com/products/en?keywords=WM24819-ND"/>
-    <hyperlink ref="H93" r:id="rId55" display="https://www.amazon.com/gp/product/B01IBOK7FE/"/>
-    <hyperlink ref="H98" r:id="rId56" display="https://www.amazon.com/gp/product/B01F2R2EPE/"/>
-    <hyperlink ref="H99" r:id="rId57" display="https://www.amazon.com/gp/product/B01F7L9QD8/"/>
-    <hyperlink ref="H104" r:id="rId58" display="https://www.digikey.com/product-detail/en/vishay-semiconductor-opto-division/VSMY2850G/VSMY2850GCT-ND/2615293"/>
-    <hyperlink ref="H105" r:id="rId59" display="https://www.digikey.com/product-detail/en/ams/TSL237T/TSL237-TCT-ND/3095287"/>
-    <hyperlink ref="H106" r:id="rId60" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X8R1H104K080AB/445-8818-1-ND/3248223"/>
-    <hyperlink ref="H107" r:id="rId61" display="https://www.digikey.com/product-detail/en/yageo/RT0603DRD07200RL/311-200DCT-ND/1035740"/>
-    <hyperlink ref="H108" r:id="rId62" display="https://github.com/lperovich/seeboat/tree/master/hardware/turbiditySensor"/>
-    <hyperlink ref="H109" r:id="rId63" display="https://github.com/lperovich/seeboat/tree/master/hardware/turbidityLED"/>
-    <hyperlink ref="H110" r:id="rId64" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-BK005/422010-BK005-ND/3705786"/>
-    <hyperlink ref="H111" r:id="rId65" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-RD005/422010-RD005-ND/4935160"/>
-    <hyperlink ref="H112" r:id="rId66" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-SL005/422010-SL005-ND/4935161"/>
-    <hyperlink ref="H113" r:id="rId67" display="https://www.amazon.com/Source-One-LLC-Acrylic-Plexiglass/dp/B06XNXHKQN/"/>
-    <hyperlink ref="H114" r:id="rId68" location="product-description-iframe" display="https://www.amazon.com/MG-Chemicals-Thermally-Conductive-Encapsulating/dp/B008UH4CRM#product-description-iframe"/>
-    <hyperlink ref="H115" r:id="rId69" display="https://www.amazon.com/CRC-SL2512-Soluble-Oil-32/dp/B000M8O010/"/>
-    <hyperlink ref="H116" r:id="rId70" display="https://www.discountvials.com/6-dram-glass-vial-w-cap/"/>
-    <hyperlink ref="H117" r:id="rId71" display="http://www.hach.com/formazin-turbidity-standard-4000-ntu-500-ml/product?id=7640455437"/>
-    <hyperlink ref="H122" r:id="rId72" display="https://github.com/lperovich/seeboat/tree/master/hardware/temperatureSensor"/>
-    <hyperlink ref="H123" r:id="rId73" display="https://www.digikey.com/product-detail/en/microchip-technology/AT30TS750A-SS8M-T/1611-AT30TS750A-SS8M-TCT-ND/6831450"/>
-    <hyperlink ref="H124" r:id="rId74" display="http://www.digikey.com/product-detail/en/RC1206FR-0710KL/311-10.0KFRCT-ND/731430"/>
-    <hyperlink ref="H125" r:id="rId75" display="https://www.digikey.com/product-detail/en/avx-corporation/1206VC104KAT2A/478-5724-1-ND/2136332"/>
+    <hyperlink ref="H16" r:id="rId8" display="https://hobbyking.com/en_us/hobbyking-350w-25a-power-supply-100v-120v.html"/>
+    <hyperlink ref="H17" r:id="rId9" display="https://hobbyking.com/en_us/icharger-206b-300w-8s-balance-charger.html"/>
+    <hyperlink ref="H18" r:id="rId10" display="https://www.horizonhobby.com/boats/electric-boats/stealthwake-rtr-23-inch-brushed-deep-v-prb08015"/>
+    <hyperlink ref="H19" r:id="rId11" display="https://www.horizonhobby.com/74v-5000mah-2s-30c-lipo-hardcase%3A-ec3-dyn9005ec"/>
+    <hyperlink ref="H25" r:id="rId12" display="https://www.adafruit.com/product/3133"/>
+    <hyperlink ref="H26" r:id="rId13" display="https://www.adafruit.com/product/380"/>
+    <hyperlink ref="H27" r:id="rId14" display="https://www.adafruit.com/product/392"/>
+    <hyperlink ref="H28" r:id="rId15" display="https://www.adafruit.com/product/2830"/>
+    <hyperlink ref="H29" r:id="rId16" display="https://www.adafruit.com/product/2886"/>
+    <hyperlink ref="H30" r:id="rId17" display="https://www.amazon.com/gp/product/B00NH13O7K"/>
+    <hyperlink ref="H31" r:id="rId18" display="https://www.adafruit.com/product/328"/>
+    <hyperlink ref="H33" r:id="rId19" display="https://github.com/lperovich/seeboat/tree/master/hardware/controlBoard"/>
+    <hyperlink ref="H34" r:id="rId20" display="https://www.digikey.com/products/en?keywords=RNCP0603FTD2K74CT-ND"/>
+    <hyperlink ref="H35" r:id="rId21" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP0603FTD100R/RNCP0603FTD100RCT-ND/2240425"/>
+    <hyperlink ref="H36" r:id="rId22" display="https://www.digikey.com/product-detail/en/AYZ0202AGRLC/401-2013-1-ND/1640122"/>
+    <hyperlink ref="H37" r:id="rId23" display="https://www.adafruit.com/product/2343"/>
+    <hyperlink ref="H38" r:id="rId24" display="https://www.digikey.com/products/en?keywords=WM4802-ND"/>
+    <hyperlink ref="H39" r:id="rId25" display="https://www.digikey.com/products/en?keywords=WM9131-ND"/>
+    <hyperlink ref="H40" r:id="rId26" display="https://www.digikey.com/products/en?keywords=WM4801-ND"/>
+    <hyperlink ref="H41" r:id="rId27" display="https://www.digikey.com/products/en?keywords=WM10647-ND"/>
+    <hyperlink ref="H42" r:id="rId28" display="https://www.digikey.com/product-detail/en/3m/3302-16-300SF/MC16M-100-ND/145737"/>
+    <hyperlink ref="H43" r:id="rId29" display="https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2004A.12.02/C2004W-100-ND/57495"/>
+    <hyperlink ref="H48" r:id="rId30" display="https://www.adafruit.com/product/2240"/>
+    <hyperlink ref="H50" r:id="rId31" display="https://www.tapplastics.com/product/plastics/cut_to_size_plastic/satinice_white/655"/>
+    <hyperlink ref="H56" r:id="rId32" display="https://www.atlas-scientific.com/product_pages/circuits/ezo_ph.html"/>
+    <hyperlink ref="H57" r:id="rId33" display="https://www.atlas-scientific.com/product_pages/probes/ph_probe.html"/>
+    <hyperlink ref="H58" r:id="rId34" display="https://www.atlas-scientific.com/product_pages/components/single_carrier_iso.html"/>
+    <hyperlink ref="H59" r:id="rId35" display="https://www.hach.com/ph-buffer-solution-kit-color-coded-ph-4-01-ph-7-00-and-ph-10-01-500-ml-each/product?id=7640205069"/>
+    <hyperlink ref="H60" r:id="rId36" display="https://www.hach.com/electrolyte-solution-kcl-3m-50ml/product-parameter-reagent?id=7640207762"/>
+    <hyperlink ref="H65" r:id="rId37" display="https://www.mcmaster.com/8972T11"/>
+    <hyperlink ref="H66" r:id="rId38" display="https://www.mcmaster.com/4339T5"/>
+    <hyperlink ref="H72" r:id="rId39" display="https://github.com/lperovich/seeboat/tree/master/hardware/conductivity"/>
+    <hyperlink ref="H73" r:id="rId40" display="https://www.digikey.com/product-detail/en/yageo/AT0603FRE0710KL/YAG2122CT-ND/5139570"/>
+    <hyperlink ref="H74" r:id="rId41" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP0603FTD2K74/RNCP0603FTD2K74CT-ND/2240457"/>
+    <hyperlink ref="H75" r:id="rId42" display="https://www.digikey.com/product-detail/en/yageo/RT0603BRD071ML/YAG4498CT-ND/6616654"/>
+    <hyperlink ref="H76" r:id="rId43" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP0603FTD1K00/RNCP0603FTD1K00CT-ND/2240445"/>
+    <hyperlink ref="H77" r:id="rId44" display="https://www.digikey.com/product-detail/en/yageo/RT0603BRD0742K2L/YAG4556CT-ND/6616712"/>
+    <hyperlink ref="H78" r:id="rId45" display="https://www.digikey.com/product-detail/en/yageo/RT0603DRE071K2L/311-2461-1-ND/6128880"/>
+    <hyperlink ref="H79" r:id="rId46" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X8R1H104K080AB/445-8818-1-ND/3248223"/>
+    <hyperlink ref="H80" r:id="rId47" display="https://www.digikey.com/products/en?keywords=641-1331-1-ND"/>
+    <hyperlink ref="H81" r:id="rId48" display="https://www.digikey.com/product-detail/en/texas-instruments/TLE2426CD/296-6547-5-ND/371934"/>
+    <hyperlink ref="H82" r:id="rId49" display="https://www.digikey.com/product-detail/en/analog-devices-inc/AD8655ARZ-REEL7/AD8655ARZ-REEL7CT-ND/3678589"/>
+    <hyperlink ref="H83" r:id="rId50" display="https://www.digikey.com/product-detail/en/texas-instruments/TLV2374IDR/296-11967-1-ND/390435"/>
+    <hyperlink ref="H84" r:id="rId51" display="https://www.digikey.com/product-detail/en/AYZ0202AGRLC/401-2013-1-ND/1640122"/>
+    <hyperlink ref="H86" r:id="rId52" display="https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2117A.12.06/C2117G-100-ND/16217"/>
+    <hyperlink ref="H87" r:id="rId53" display="https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2004A.12.02/C2004W-100-ND/57495"/>
+    <hyperlink ref="H88" r:id="rId54" display="https://www.digikey.com/products/en?keywords=%09WM4800-ND"/>
+    <hyperlink ref="H89" r:id="rId55" display="https://www.digikey.com/products/en?keywords=WM24819-ND"/>
+    <hyperlink ref="H92" r:id="rId56" display="https://www.mcmaster.com/2029n13"/>
+    <hyperlink ref="H93" r:id="rId57" display="https://www.amazon.com/gp/product/B01IBOK7FE/"/>
+    <hyperlink ref="H98" r:id="rId58" display="https://www.amazon.com/gp/product/B01F2R2EPE/"/>
+    <hyperlink ref="H99" r:id="rId59" display="https://www.amazon.com/gp/product/B01F7L9QD8/"/>
+    <hyperlink ref="H104" r:id="rId60" display="https://www.digikey.com/product-detail/en/vishay-semiconductor-opto-division/VSMY2850G/VSMY2850GCT-ND/2615293"/>
+    <hyperlink ref="H105" r:id="rId61" display="https://www.digikey.com/product-detail/en/ams/TSL237T/TSL237-TCT-ND/3095287"/>
+    <hyperlink ref="H106" r:id="rId62" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X8R1H104K080AB/445-8818-1-ND/3248223"/>
+    <hyperlink ref="H107" r:id="rId63" display="https://www.digikey.com/product-detail/en/yageo/RT0603DRD07200RL/311-200DCT-ND/1035740"/>
+    <hyperlink ref="H108" r:id="rId64" display="https://github.com/lperovich/seeboat/tree/master/hardware/turbiditySensor"/>
+    <hyperlink ref="H109" r:id="rId65" display="https://github.com/lperovich/seeboat/tree/master/hardware/turbidityLED"/>
+    <hyperlink ref="H110" r:id="rId66" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-BK005/422010-BK005-ND/3705786"/>
+    <hyperlink ref="H111" r:id="rId67" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-RD005/422010-RD005-ND/4935160"/>
+    <hyperlink ref="H112" r:id="rId68" display="https://www.digikey.com/product-detail/en/alpha-wire/422010-SL005/422010-SL005-ND/4935161"/>
+    <hyperlink ref="H113" r:id="rId69" display="https://www.amazon.com/Source-One-LLC-Acrylic-Plexiglass/dp/B06XNXHKQN/"/>
+    <hyperlink ref="H114" r:id="rId70" location="product-description-iframe" display="https://www.amazon.com/MG-Chemicals-Thermally-Conductive-Encapsulating/dp/B008UH4CRM#product-description-iframe"/>
+    <hyperlink ref="H115" r:id="rId71" display="https://www.amazon.com/CRC-SL2512-Soluble-Oil-32/dp/B000M8O010/"/>
+    <hyperlink ref="H116" r:id="rId72" display="https://www.discountvials.com/6-dram-glass-vial-w-cap/"/>
+    <hyperlink ref="H117" r:id="rId73" display="http://www.hach.com/formazin-turbidity-standard-4000-ntu-500-ml/product?id=7640455437"/>
+    <hyperlink ref="H122" r:id="rId74" display="https://github.com/lperovich/seeboat/tree/master/hardware/temperatureSensor"/>
+    <hyperlink ref="H123" r:id="rId75" display="https://www.digikey.com/product-detail/en/microchip-technology/AT30TS750A-SS8M-T/1611-AT30TS750A-SS8M-TCT-ND/6831450"/>
+    <hyperlink ref="H124" r:id="rId76" display="http://www.digikey.com/product-detail/en/RC1206FR-0710KL/311-10.0KFRCT-ND/731430"/>
+    <hyperlink ref="H125" r:id="rId77" display="https://www.digikey.com/product-detail/en/avx-corporation/1206VC104KAT2A/478-5724-1-ND/2136332"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5152,7 +5164,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>283</v>
       </c>
     </row>
@@ -5165,85 +5177,85 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="27" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="27" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="27" t="s">
         <v>288</v>
       </c>
       <c r="D7" s="52" t="s">
         <v>289</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="27" t="s">
         <v>290</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="27" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="27" t="s">
         <v>292</v>
       </c>
       <c r="D8" s="52" t="s">
         <v>293</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="27" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="27" t="s">
         <v>295</v>
       </c>
       <c r="D9" s="52" t="s">
         <v>296</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="27" t="s">
         <v>294</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="27" t="s">
         <v>297</v>
       </c>
       <c r="G9" s="53" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="27" t="s">
         <v>298</v>
       </c>
       <c r="D10" s="52" t="s">
         <v>299</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="27" t="s">
         <v>300</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="27" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="27" t="s">
         <v>302</v>
       </c>
       <c r="D11" s="52" t="s">
         <v>303</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="27" t="s">
         <v>290</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="27" t="s">
         <v>304</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="G11" s="27" t="s">
         <v>305</v>
       </c>
     </row>
@@ -5251,7 +5263,7 @@
       <c r="D13" s="52" t="s">
         <v>306</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="27" t="s">
         <v>307</v>
       </c>
     </row>
@@ -5259,7 +5271,7 @@
       <c r="D14" s="52" t="s">
         <v>308</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="27" t="s">
         <v>309</v>
       </c>
     </row>
@@ -5267,19 +5279,19 @@
       <c r="D15" s="52" t="s">
         <v>310</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="27" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="52" t="s">
         <v>312</v>
       </c>
-      <c r="E17" s="26" t="s">
+      <c r="E17" s="27" t="s">
         <v>313</v>
       </c>
     </row>
@@ -5289,12 +5301,12 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E19" s="26" t="s">
+      <c r="E19" s="27" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="27" t="s">
         <v>316</v>
       </c>
       <c r="D20" s="52" t="s">
@@ -5303,7 +5315,7 @@
       <c r="E20" s="54" t="s">
         <v>318</v>
       </c>
-      <c r="F20" s="26" t="s">
+      <c r="F20" s="27" t="s">
         <v>319</v>
       </c>
     </row>
@@ -5322,7 +5334,7 @@
         <v>322</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -5362,7 +5374,7 @@
         <v>324</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
@@ -5404,10 +5416,10 @@
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
       <c r="D30" s="13" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F30" s="55" t="n">
         <v>4</v>
@@ -5446,7 +5458,7 @@
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="55" t="n">
@@ -5486,7 +5498,7 @@
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
       <c r="D35" s="13" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="E35" s="13" t="s">
         <v>331</v>
@@ -5521,16 +5533,16 @@
       <c r="AB35" s="13"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="27" t="s">
         <v>333</v>
       </c>
-      <c r="D36" s="26" t="s">
+      <c r="D36" s="27" t="s">
         <v>334</v>
       </c>
-      <c r="E36" s="26" t="s">
+      <c r="E36" s="27" t="s">
         <v>335</v>
       </c>
-      <c r="F36" s="26" t="n">
+      <c r="F36" s="27" t="n">
         <v>1</v>
       </c>
       <c r="G36" s="59" t="n">
@@ -5541,16 +5553,16 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="26" t="s">
+      <c r="A37" s="27" t="s">
         <v>337</v>
       </c>
-      <c r="D37" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="E37" s="26" t="s">
+      <c r="D37" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" s="27" t="s">
         <v>338</v>
       </c>
-      <c r="F37" s="26" t="n">
+      <c r="F37" s="27" t="n">
         <v>1</v>
       </c>
       <c r="G37" s="59" t="n">
@@ -5561,16 +5573,16 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="26" t="s">
+      <c r="A38" s="27" t="s">
         <v>340</v>
       </c>
-      <c r="D38" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="E38" s="26" t="s">
+      <c r="D38" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" s="27" t="s">
         <v>341</v>
       </c>
-      <c r="F38" s="26" t="n">
+      <c r="F38" s="27" t="n">
         <v>1</v>
       </c>
       <c r="G38" s="59" t="n">
@@ -5581,16 +5593,16 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="26" t="s">
+      <c r="A39" s="27" t="s">
         <v>343</v>
       </c>
-      <c r="D39" s="26" t="s">
+      <c r="D39" s="27" t="s">
         <v>344</v>
       </c>
-      <c r="E39" s="26" t="s">
+      <c r="E39" s="27" t="s">
         <v>345</v>
       </c>
-      <c r="F39" s="26" t="n">
+      <c r="F39" s="27" t="n">
         <v>1</v>
       </c>
       <c r="G39" s="59" t="n">
@@ -5598,16 +5610,16 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="26" t="s">
+      <c r="A40" s="27" t="s">
         <v>346</v>
       </c>
-      <c r="D40" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="E40" s="26" t="s">
+      <c r="D40" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E40" s="27" t="s">
         <v>347</v>
       </c>
-      <c r="F40" s="26" t="n">
+      <c r="F40" s="27" t="n">
         <v>1</v>
       </c>
       <c r="G40" s="59" t="n">

</xml_diff>